<commit_message>
Small improvements to projects
</commit_message>
<xml_diff>
--- a/core/import_data/resources/projects_v2/project_clusters_06_05_2025.xlsx
+++ b/core/import_data/resources/projects_v2/project_clusters_06_05_2025.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="77">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -31,6 +31,9 @@
     <t xml:space="preserve">Category</t>
   </si>
   <si>
+    <t xml:space="preserve">Dashboard group</t>
+  </si>
+  <si>
     <t xml:space="preserve">Action</t>
   </si>
   <si>
@@ -46,6 +49,9 @@
     <t xml:space="preserve">MYA</t>
   </si>
   <si>
+    <t xml:space="preserve">Consumption</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kigali Implementation Plan Stage 2</t>
   </si>
   <si>
@@ -64,6 +70,9 @@
     <t xml:space="preserve">KPP1</t>
   </si>
   <si>
+    <t xml:space="preserve">Production</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kigali Implementation Plan Production Stage 2</t>
   </si>
   <si>
@@ -109,6 +118,9 @@
     <t xml:space="preserve">Both</t>
   </si>
   <si>
+    <t xml:space="preserve">HFC-23</t>
+  </si>
+  <si>
     <t xml:space="preserve">HCFC production phase-out management plan stage 1</t>
   </si>
   <si>
@@ -136,12 +148,36 @@
     <t xml:space="preserve">IND</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Consumption</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/Production</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">HCFC Individual</t>
   </si>
   <si>
     <t xml:space="preserve">HCFCIND</t>
   </si>
   <si>
+    <t xml:space="preserve">Consumption </t>
+  </si>
+  <si>
     <t xml:space="preserve">Energy Efficiency</t>
   </si>
   <si>
@@ -203,6 +239,9 @@
   </si>
   <si>
     <t xml:space="preserve">GOV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IS</t>
   </si>
   <si>
     <t xml:space="preserve">Agency Programme</t>
@@ -240,7 +279,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -274,7 +313,22 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -285,10 +339,23 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -353,7 +420,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -366,19 +433,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -386,7 +453,31 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -394,11 +485,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -652,10 +751,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:WS1048576"/>
+  <dimension ref="A1:WT1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D:D"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -663,215 +762,257 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="49.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.8"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="25.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.8"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="C2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="A8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="A9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="A10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="A11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="A12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="A13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="G14" s="1"/>
+      <c r="A14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1431,20 +1572,23 @@
       <c r="UR14" s="1"/>
       <c r="US14" s="1"/>
       <c r="UT14" s="1"/>
+      <c r="UU14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="G15" s="1"/>
+      <c r="A15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -2004,20 +2148,23 @@
       <c r="UR15" s="1"/>
       <c r="US15" s="1"/>
       <c r="UT15" s="1"/>
+      <c r="UU15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="G16" s="1"/>
+      <c r="A16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -2577,65 +2724,75 @@
       <c r="UR16" s="1"/>
       <c r="US16" s="1"/>
       <c r="UT16" s="1"/>
+      <c r="UU16" s="1"/>
     </row>
     <row r="17" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="A17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="2" t="s">
+      <c r="A18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>43</v>
+      <c r="D18" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" s="6" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="1"/>
+      <c r="A19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" s="10" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="3"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -2654,22 +2811,23 @@
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
-    </row>
-    <row r="21" s="6" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="1"/>
+      <c r="Y20" s="1"/>
+    </row>
+    <row r="21" s="10" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="3"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -2688,145 +2846,158 @@
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
     </row>
     <row r="22" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="2"/>
+      <c r="A22" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="3"/>
     </row>
     <row r="23" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="2" t="s">
+      <c r="A23" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="2"/>
+      <c r="F23" s="3"/>
     </row>
     <row r="24" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="2"/>
+      <c r="A24" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F24" s="3"/>
     </row>
     <row r="25" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E25" s="2"/>
+      <c r="A25" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" s="3"/>
     </row>
     <row r="26" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="A26" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
     </row>
     <row r="27" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="A27" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="12"/>
     </row>
     <row r="28" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>48</v>
+      <c r="A28" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="12"/>
+      <c r="E28" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="29" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>48</v>
+      <c r="A29" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="14"/>
+      <c r="E29" s="15" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>37</v>
-      </c>
+      <c r="A30" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="14"/>
     </row>
     <row r="31" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>37</v>
-      </c>
+      <c r="A31" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="14"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C32" s="8"/>
-      <c r="D32" s="1"/>
-      <c r="G32" s="1"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -3437,11 +3608,12 @@
       <c r="WQ32" s="1"/>
       <c r="WR32" s="1"/>
       <c r="WS32" s="1"/>
+      <c r="WT32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C33" s="8"/>
-      <c r="D33" s="1"/>
-      <c r="G33" s="1"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -4052,11 +4224,12 @@
       <c r="WQ33" s="1"/>
       <c r="WR33" s="1"/>
       <c r="WS33" s="1"/>
+      <c r="WT33" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C34" s="8"/>
-      <c r="D34" s="1"/>
-      <c r="G34" s="1"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -4667,11 +4840,12 @@
       <c r="WQ34" s="1"/>
       <c r="WR34" s="1"/>
       <c r="WS34" s="1"/>
+      <c r="WT34" s="1"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C35" s="8"/>
-      <c r="D35" s="1"/>
-      <c r="G35" s="1"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
@@ -5231,13 +5405,14 @@
       <c r="UR35" s="1"/>
       <c r="US35" s="1"/>
       <c r="UT35" s="1"/>
+      <c r="UU35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="10"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="G36" s="1"/>
+      <c r="A36" s="16"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="16"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
@@ -5797,495 +5972,656 @@
       <c r="UR36" s="1"/>
       <c r="US36" s="1"/>
       <c r="UT36" s="1"/>
+      <c r="UU36" s="1"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
+      <c r="A37" s="18"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="18"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C40" s="8"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="14"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C41" s="8"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="14"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C42" s="8"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="14"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C43" s="8"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="14"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C44" s="8"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="14"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C45" s="8"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="14"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C46" s="8"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="14"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C47" s="8"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="14"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C48" s="8"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="14"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C49" s="8"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="14"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C50" s="8"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="14"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C51" s="8"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="14"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C52" s="8"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="14"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C53" s="8"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="14"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C54" s="8"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="14"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C55" s="8"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="14"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C56" s="8"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="14"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C57" s="8"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="14"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C58" s="8"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="14"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C59" s="8"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="14"/>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C60" s="8"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="14"/>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C61" s="8"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="14"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C62" s="8"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="14"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C63" s="8"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="14"/>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C64" s="8"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="14"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C65" s="8"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="14"/>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C66" s="8"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="14"/>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C67" s="8"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="14"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C68" s="8"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="14"/>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C69" s="8"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="14"/>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C70" s="8"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="14"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C71" s="8"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="14"/>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C72" s="8"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="14"/>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C73" s="8"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="14"/>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C74" s="8"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="14"/>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C75" s="8"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="14"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C76" s="8"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="14"/>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C77" s="8"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="14"/>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C78" s="8"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="14"/>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C79" s="8"/>
+      <c r="C79" s="13"/>
+      <c r="D79" s="14"/>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C80" s="8"/>
+      <c r="C80" s="13"/>
+      <c r="D80" s="14"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C81" s="8"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="14"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C82" s="8"/>
+      <c r="C82" s="13"/>
+      <c r="D82" s="14"/>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C83" s="8"/>
+      <c r="C83" s="13"/>
+      <c r="D83" s="14"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C84" s="8"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="14"/>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C85" s="8"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="14"/>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C86" s="8"/>
+      <c r="C86" s="13"/>
+      <c r="D86" s="14"/>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C87" s="8"/>
+      <c r="C87" s="13"/>
+      <c r="D87" s="14"/>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C88" s="8"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="14"/>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C89" s="8"/>
+      <c r="C89" s="13"/>
+      <c r="D89" s="14"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C90" s="8"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="14"/>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C91" s="8"/>
+      <c r="C91" s="13"/>
+      <c r="D91" s="14"/>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C92" s="8"/>
+      <c r="C92" s="13"/>
+      <c r="D92" s="14"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C93" s="8"/>
+      <c r="C93" s="13"/>
+      <c r="D93" s="14"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C94" s="8"/>
+      <c r="C94" s="13"/>
+      <c r="D94" s="14"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C95" s="8"/>
+      <c r="C95" s="13"/>
+      <c r="D95" s="14"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C96" s="8"/>
+      <c r="C96" s="13"/>
+      <c r="D96" s="14"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C97" s="8"/>
+      <c r="C97" s="13"/>
+      <c r="D97" s="14"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C98" s="8"/>
+      <c r="C98" s="13"/>
+      <c r="D98" s="14"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C99" s="8"/>
+      <c r="C99" s="13"/>
+      <c r="D99" s="14"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C100" s="8"/>
+      <c r="C100" s="13"/>
+      <c r="D100" s="14"/>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C101" s="8"/>
+      <c r="C101" s="13"/>
+      <c r="D101" s="14"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C102" s="8"/>
+      <c r="C102" s="13"/>
+      <c r="D102" s="14"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C103" s="8"/>
+      <c r="C103" s="13"/>
+      <c r="D103" s="14"/>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C104" s="8"/>
+      <c r="C104" s="13"/>
+      <c r="D104" s="14"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C105" s="8"/>
+      <c r="C105" s="13"/>
+      <c r="D105" s="14"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C106" s="8"/>
+      <c r="C106" s="13"/>
+      <c r="D106" s="14"/>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C107" s="8"/>
+      <c r="C107" s="13"/>
+      <c r="D107" s="14"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C108" s="8"/>
+      <c r="C108" s="13"/>
+      <c r="D108" s="14"/>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C109" s="8"/>
+      <c r="C109" s="13"/>
+      <c r="D109" s="14"/>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C110" s="8"/>
+      <c r="C110" s="13"/>
+      <c r="D110" s="14"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C111" s="8"/>
+      <c r="C111" s="13"/>
+      <c r="D111" s="14"/>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C112" s="8"/>
+      <c r="C112" s="13"/>
+      <c r="D112" s="14"/>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C113" s="8"/>
+      <c r="C113" s="13"/>
+      <c r="D113" s="14"/>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C114" s="8"/>
+      <c r="C114" s="13"/>
+      <c r="D114" s="14"/>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C115" s="8"/>
+      <c r="C115" s="13"/>
+      <c r="D115" s="14"/>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C116" s="8"/>
+      <c r="C116" s="13"/>
+      <c r="D116" s="14"/>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C117" s="8"/>
+      <c r="C117" s="13"/>
+      <c r="D117" s="14"/>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C118" s="8"/>
+      <c r="C118" s="13"/>
+      <c r="D118" s="14"/>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C119" s="8"/>
+      <c r="C119" s="13"/>
+      <c r="D119" s="14"/>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C120" s="8"/>
+      <c r="C120" s="13"/>
+      <c r="D120" s="14"/>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C121" s="8"/>
+      <c r="C121" s="13"/>
+      <c r="D121" s="14"/>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C122" s="8"/>
+      <c r="C122" s="13"/>
+      <c r="D122" s="14"/>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C123" s="8"/>
+      <c r="C123" s="13"/>
+      <c r="D123" s="14"/>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C124" s="8"/>
+      <c r="C124" s="13"/>
+      <c r="D124" s="14"/>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C125" s="8"/>
+      <c r="C125" s="13"/>
+      <c r="D125" s="14"/>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C126" s="8"/>
+      <c r="C126" s="13"/>
+      <c r="D126" s="14"/>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C127" s="8"/>
+      <c r="C127" s="13"/>
+      <c r="D127" s="14"/>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C128" s="8"/>
+      <c r="C128" s="13"/>
+      <c r="D128" s="14"/>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C129" s="8"/>
+      <c r="C129" s="13"/>
+      <c r="D129" s="14"/>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C130" s="8"/>
+      <c r="C130" s="13"/>
+      <c r="D130" s="14"/>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C131" s="8"/>
+      <c r="C131" s="13"/>
+      <c r="D131" s="14"/>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C132" s="8"/>
+      <c r="C132" s="13"/>
+      <c r="D132" s="14"/>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C133" s="8"/>
+      <c r="C133" s="13"/>
+      <c r="D133" s="14"/>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C134" s="8"/>
+      <c r="C134" s="13"/>
+      <c r="D134" s="14"/>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C135" s="8"/>
+      <c r="C135" s="13"/>
+      <c r="D135" s="14"/>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C136" s="8"/>
+      <c r="C136" s="13"/>
+      <c r="D136" s="14"/>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C137" s="8"/>
+      <c r="C137" s="13"/>
+      <c r="D137" s="14"/>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C138" s="8"/>
+      <c r="C138" s="13"/>
+      <c r="D138" s="14"/>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C139" s="8"/>
+      <c r="C139" s="13"/>
+      <c r="D139" s="14"/>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C140" s="8"/>
+      <c r="C140" s="13"/>
+      <c r="D140" s="14"/>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C141" s="8"/>
+      <c r="C141" s="13"/>
+      <c r="D141" s="14"/>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C142" s="8"/>
+      <c r="C142" s="13"/>
+      <c r="D142" s="14"/>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C143" s="8"/>
+      <c r="C143" s="13"/>
+      <c r="D143" s="14"/>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C144" s="8"/>
+      <c r="C144" s="13"/>
+      <c r="D144" s="14"/>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C145" s="8"/>
+      <c r="C145" s="13"/>
+      <c r="D145" s="14"/>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C146" s="8"/>
+      <c r="C146" s="13"/>
+      <c r="D146" s="14"/>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C147" s="8"/>
+      <c r="C147" s="13"/>
+      <c r="D147" s="14"/>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C148" s="8"/>
+      <c r="C148" s="13"/>
+      <c r="D148" s="14"/>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C149" s="8"/>
+      <c r="C149" s="13"/>
+      <c r="D149" s="14"/>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C150" s="8"/>
+      <c r="C150" s="13"/>
+      <c r="D150" s="14"/>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C151" s="8"/>
+      <c r="C151" s="13"/>
+      <c r="D151" s="14"/>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C152" s="8"/>
+      <c r="C152" s="13"/>
+      <c r="D152" s="14"/>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C153" s="8"/>
+      <c r="C153" s="13"/>
+      <c r="D153" s="14"/>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C154" s="8"/>
+      <c r="C154" s="13"/>
+      <c r="D154" s="14"/>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C155" s="8"/>
+      <c r="C155" s="13"/>
+      <c r="D155" s="14"/>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C156" s="8"/>
+      <c r="C156" s="13"/>
+      <c r="D156" s="14"/>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C157" s="8"/>
+      <c r="C157" s="13"/>
+      <c r="D157" s="14"/>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C158" s="8"/>
+      <c r="C158" s="13"/>
+      <c r="D158" s="14"/>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C159" s="8"/>
+      <c r="C159" s="13"/>
+      <c r="D159" s="14"/>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C160" s="8"/>
+      <c r="C160" s="13"/>
+      <c r="D160" s="14"/>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C161" s="8"/>
+      <c r="C161" s="13"/>
+      <c r="D161" s="14"/>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C162" s="8"/>
+      <c r="C162" s="13"/>
+      <c r="D162" s="14"/>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C163" s="8"/>
+      <c r="C163" s="13"/>
+      <c r="D163" s="14"/>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C164" s="8"/>
+      <c r="C164" s="13"/>
+      <c r="D164" s="14"/>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C165" s="8"/>
+      <c r="C165" s="13"/>
+      <c r="D165" s="14"/>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C166" s="8"/>
+      <c r="C166" s="13"/>
+      <c r="D166" s="14"/>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C167" s="8"/>
+      <c r="C167" s="13"/>
+      <c r="D167" s="14"/>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C168" s="8"/>
+      <c r="C168" s="13"/>
+      <c r="D168" s="14"/>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C169" s="8"/>
+      <c r="C169" s="13"/>
+      <c r="D169" s="14"/>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C170" s="8"/>
+      <c r="C170" s="13"/>
+      <c r="D170" s="14"/>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C171" s="8"/>
+      <c r="C171" s="13"/>
+      <c r="D171" s="14"/>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C172" s="8"/>
+      <c r="C172" s="13"/>
+      <c r="D172" s="14"/>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C173" s="8"/>
+      <c r="C173" s="13"/>
+      <c r="D173" s="14"/>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C174" s="8"/>
+      <c r="C174" s="13"/>
+      <c r="D174" s="14"/>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C175" s="8"/>
+      <c r="C175" s="13"/>
+      <c r="D175" s="14"/>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C176" s="8"/>
+      <c r="C176" s="13"/>
+      <c r="D176" s="14"/>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C177" s="8"/>
+      <c r="C177" s="13"/>
+      <c r="D177" s="14"/>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C178" s="8"/>
+      <c r="C178" s="13"/>
+      <c r="D178" s="14"/>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C179" s="8"/>
+      <c r="C179" s="13"/>
+      <c r="D179" s="14"/>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C180" s="8"/>
+      <c r="C180" s="13"/>
+      <c r="D180" s="14"/>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C181" s="8"/>
+      <c r="C181" s="13"/>
+      <c r="D181" s="14"/>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C182" s="8"/>
+      <c r="C182" s="13"/>
+      <c r="D182" s="14"/>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C183" s="8"/>
+      <c r="C183" s="13"/>
+      <c r="D183" s="14"/>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C184" s="8"/>
+      <c r="C184" s="13"/>
+      <c r="D184" s="14"/>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C185" s="8"/>
+      <c r="C185" s="13"/>
+      <c r="D185" s="14"/>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C186" s="8"/>
+      <c r="C186" s="13"/>
+      <c r="D186" s="14"/>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C187" s="8"/>
+      <c r="C187" s="13"/>
+      <c r="D187" s="14"/>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C188" s="8"/>
+      <c r="C188" s="13"/>
+      <c r="D188" s="14"/>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C189" s="8"/>
+      <c r="C189" s="13"/>
+      <c r="D189" s="14"/>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C190" s="8"/>
+      <c r="C190" s="13"/>
+      <c r="D190" s="14"/>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C191" s="8"/>
+      <c r="C191" s="13"/>
+      <c r="D191" s="14"/>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C192" s="8"/>
+      <c r="C192" s="13"/>
+      <c r="D192" s="14"/>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C193" s="8"/>
+      <c r="C193" s="13"/>
+      <c r="D193" s="14"/>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C194" s="8"/>
+      <c r="C194" s="13"/>
+      <c r="D194" s="14"/>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C195" s="8"/>
+      <c r="C195" s="13"/>
+      <c r="D195" s="14"/>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C196" s="8"/>
+      <c r="C196" s="13"/>
+      <c r="D196" s="14"/>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C197" s="8"/>
+      <c r="C197" s="13"/>
+      <c r="D197" s="14"/>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C198" s="8"/>
+      <c r="C198" s="13"/>
+      <c r="D198" s="14"/>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Small improvements to projects (#655)
</commit_message>
<xml_diff>
--- a/core/import_data/resources/projects_v2/project_clusters_06_05_2025.xlsx
+++ b/core/import_data/resources/projects_v2/project_clusters_06_05_2025.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="77">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -31,6 +31,9 @@
     <t xml:space="preserve">Category</t>
   </si>
   <si>
+    <t xml:space="preserve">Dashboard group</t>
+  </si>
+  <si>
     <t xml:space="preserve">Action</t>
   </si>
   <si>
@@ -46,6 +49,9 @@
     <t xml:space="preserve">MYA</t>
   </si>
   <si>
+    <t xml:space="preserve">Consumption</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kigali Implementation Plan Stage 2</t>
   </si>
   <si>
@@ -64,6 +70,9 @@
     <t xml:space="preserve">KPP1</t>
   </si>
   <si>
+    <t xml:space="preserve">Production</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kigali Implementation Plan Production Stage 2</t>
   </si>
   <si>
@@ -109,6 +118,9 @@
     <t xml:space="preserve">Both</t>
   </si>
   <si>
+    <t xml:space="preserve">HFC-23</t>
+  </si>
+  <si>
     <t xml:space="preserve">HCFC production phase-out management plan stage 1</t>
   </si>
   <si>
@@ -136,12 +148,36 @@
     <t xml:space="preserve">IND</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Consumption</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/Production</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">HCFC Individual</t>
   </si>
   <si>
     <t xml:space="preserve">HCFCIND</t>
   </si>
   <si>
+    <t xml:space="preserve">Consumption </t>
+  </si>
+  <si>
     <t xml:space="preserve">Energy Efficiency</t>
   </si>
   <si>
@@ -203,6 +239,9 @@
   </si>
   <si>
     <t xml:space="preserve">GOV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IS</t>
   </si>
   <si>
     <t xml:space="preserve">Agency Programme</t>
@@ -240,7 +279,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -274,7 +313,22 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -285,10 +339,23 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -353,7 +420,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -366,19 +433,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -386,7 +453,31 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -394,11 +485,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -652,10 +751,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:WS1048576"/>
+  <dimension ref="A1:WT1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D:D"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -663,215 +762,257 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="49.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.8"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="25.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.8"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="C2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="A8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="A9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="A10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="A11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="A12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="A13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="G14" s="1"/>
+      <c r="A14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1431,20 +1572,23 @@
       <c r="UR14" s="1"/>
       <c r="US14" s="1"/>
       <c r="UT14" s="1"/>
+      <c r="UU14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="G15" s="1"/>
+      <c r="A15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -2004,20 +2148,23 @@
       <c r="UR15" s="1"/>
       <c r="US15" s="1"/>
       <c r="UT15" s="1"/>
+      <c r="UU15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="G16" s="1"/>
+      <c r="A16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -2577,65 +2724,75 @@
       <c r="UR16" s="1"/>
       <c r="US16" s="1"/>
       <c r="UT16" s="1"/>
+      <c r="UU16" s="1"/>
     </row>
     <row r="17" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="A17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="2" t="s">
+      <c r="A18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>43</v>
+      <c r="D18" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" s="6" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="1"/>
+      <c r="A19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" s="10" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="3"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -2654,22 +2811,23 @@
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
-    </row>
-    <row r="21" s="6" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="1"/>
+      <c r="Y20" s="1"/>
+    </row>
+    <row r="21" s="10" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="3"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -2688,145 +2846,158 @@
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
     </row>
     <row r="22" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="2"/>
+      <c r="A22" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="3"/>
     </row>
     <row r="23" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="2" t="s">
+      <c r="A23" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="2"/>
+      <c r="F23" s="3"/>
     </row>
     <row r="24" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="2"/>
+      <c r="A24" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F24" s="3"/>
     </row>
     <row r="25" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E25" s="2"/>
+      <c r="A25" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" s="3"/>
     </row>
     <row r="26" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="A26" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
     </row>
     <row r="27" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="A27" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="12"/>
     </row>
     <row r="28" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>48</v>
+      <c r="A28" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="12"/>
+      <c r="E28" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="29" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>48</v>
+      <c r="A29" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="14"/>
+      <c r="E29" s="15" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>37</v>
-      </c>
+      <c r="A30" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="14"/>
     </row>
     <row r="31" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>37</v>
-      </c>
+      <c r="A31" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="14"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C32" s="8"/>
-      <c r="D32" s="1"/>
-      <c r="G32" s="1"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -3437,11 +3608,12 @@
       <c r="WQ32" s="1"/>
       <c r="WR32" s="1"/>
       <c r="WS32" s="1"/>
+      <c r="WT32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C33" s="8"/>
-      <c r="D33" s="1"/>
-      <c r="G33" s="1"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -4052,11 +4224,12 @@
       <c r="WQ33" s="1"/>
       <c r="WR33" s="1"/>
       <c r="WS33" s="1"/>
+      <c r="WT33" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C34" s="8"/>
-      <c r="D34" s="1"/>
-      <c r="G34" s="1"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -4667,11 +4840,12 @@
       <c r="WQ34" s="1"/>
       <c r="WR34" s="1"/>
       <c r="WS34" s="1"/>
+      <c r="WT34" s="1"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C35" s="8"/>
-      <c r="D35" s="1"/>
-      <c r="G35" s="1"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
@@ -5231,13 +5405,14 @@
       <c r="UR35" s="1"/>
       <c r="US35" s="1"/>
       <c r="UT35" s="1"/>
+      <c r="UU35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="10"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="G36" s="1"/>
+      <c r="A36" s="16"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="16"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
@@ -5797,495 +5972,656 @@
       <c r="UR36" s="1"/>
       <c r="US36" s="1"/>
       <c r="UT36" s="1"/>
+      <c r="UU36" s="1"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
+      <c r="A37" s="18"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="18"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C40" s="8"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="14"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C41" s="8"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="14"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C42" s="8"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="14"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C43" s="8"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="14"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C44" s="8"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="14"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C45" s="8"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="14"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C46" s="8"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="14"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C47" s="8"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="14"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C48" s="8"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="14"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C49" s="8"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="14"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C50" s="8"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="14"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C51" s="8"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="14"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C52" s="8"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="14"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C53" s="8"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="14"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C54" s="8"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="14"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C55" s="8"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="14"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C56" s="8"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="14"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C57" s="8"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="14"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C58" s="8"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="14"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C59" s="8"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="14"/>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C60" s="8"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="14"/>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C61" s="8"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="14"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C62" s="8"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="14"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C63" s="8"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="14"/>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C64" s="8"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="14"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C65" s="8"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="14"/>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C66" s="8"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="14"/>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C67" s="8"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="14"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C68" s="8"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="14"/>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C69" s="8"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="14"/>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C70" s="8"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="14"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C71" s="8"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="14"/>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C72" s="8"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="14"/>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C73" s="8"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="14"/>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C74" s="8"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="14"/>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C75" s="8"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="14"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C76" s="8"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="14"/>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C77" s="8"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="14"/>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C78" s="8"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="14"/>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C79" s="8"/>
+      <c r="C79" s="13"/>
+      <c r="D79" s="14"/>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C80" s="8"/>
+      <c r="C80" s="13"/>
+      <c r="D80" s="14"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C81" s="8"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="14"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C82" s="8"/>
+      <c r="C82" s="13"/>
+      <c r="D82" s="14"/>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C83" s="8"/>
+      <c r="C83" s="13"/>
+      <c r="D83" s="14"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C84" s="8"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="14"/>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C85" s="8"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="14"/>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C86" s="8"/>
+      <c r="C86" s="13"/>
+      <c r="D86" s="14"/>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C87" s="8"/>
+      <c r="C87" s="13"/>
+      <c r="D87" s="14"/>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C88" s="8"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="14"/>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C89" s="8"/>
+      <c r="C89" s="13"/>
+      <c r="D89" s="14"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C90" s="8"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="14"/>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C91" s="8"/>
+      <c r="C91" s="13"/>
+      <c r="D91" s="14"/>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C92" s="8"/>
+      <c r="C92" s="13"/>
+      <c r="D92" s="14"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C93" s="8"/>
+      <c r="C93" s="13"/>
+      <c r="D93" s="14"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C94" s="8"/>
+      <c r="C94" s="13"/>
+      <c r="D94" s="14"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C95" s="8"/>
+      <c r="C95" s="13"/>
+      <c r="D95" s="14"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C96" s="8"/>
+      <c r="C96" s="13"/>
+      <c r="D96" s="14"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C97" s="8"/>
+      <c r="C97" s="13"/>
+      <c r="D97" s="14"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C98" s="8"/>
+      <c r="C98" s="13"/>
+      <c r="D98" s="14"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C99" s="8"/>
+      <c r="C99" s="13"/>
+      <c r="D99" s="14"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C100" s="8"/>
+      <c r="C100" s="13"/>
+      <c r="D100" s="14"/>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C101" s="8"/>
+      <c r="C101" s="13"/>
+      <c r="D101" s="14"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C102" s="8"/>
+      <c r="C102" s="13"/>
+      <c r="D102" s="14"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C103" s="8"/>
+      <c r="C103" s="13"/>
+      <c r="D103" s="14"/>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C104" s="8"/>
+      <c r="C104" s="13"/>
+      <c r="D104" s="14"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C105" s="8"/>
+      <c r="C105" s="13"/>
+      <c r="D105" s="14"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C106" s="8"/>
+      <c r="C106" s="13"/>
+      <c r="D106" s="14"/>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C107" s="8"/>
+      <c r="C107" s="13"/>
+      <c r="D107" s="14"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C108" s="8"/>
+      <c r="C108" s="13"/>
+      <c r="D108" s="14"/>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C109" s="8"/>
+      <c r="C109" s="13"/>
+      <c r="D109" s="14"/>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C110" s="8"/>
+      <c r="C110" s="13"/>
+      <c r="D110" s="14"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C111" s="8"/>
+      <c r="C111" s="13"/>
+      <c r="D111" s="14"/>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C112" s="8"/>
+      <c r="C112" s="13"/>
+      <c r="D112" s="14"/>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C113" s="8"/>
+      <c r="C113" s="13"/>
+      <c r="D113" s="14"/>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C114" s="8"/>
+      <c r="C114" s="13"/>
+      <c r="D114" s="14"/>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C115" s="8"/>
+      <c r="C115" s="13"/>
+      <c r="D115" s="14"/>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C116" s="8"/>
+      <c r="C116" s="13"/>
+      <c r="D116" s="14"/>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C117" s="8"/>
+      <c r="C117" s="13"/>
+      <c r="D117" s="14"/>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C118" s="8"/>
+      <c r="C118" s="13"/>
+      <c r="D118" s="14"/>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C119" s="8"/>
+      <c r="C119" s="13"/>
+      <c r="D119" s="14"/>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C120" s="8"/>
+      <c r="C120" s="13"/>
+      <c r="D120" s="14"/>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C121" s="8"/>
+      <c r="C121" s="13"/>
+      <c r="D121" s="14"/>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C122" s="8"/>
+      <c r="C122" s="13"/>
+      <c r="D122" s="14"/>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C123" s="8"/>
+      <c r="C123" s="13"/>
+      <c r="D123" s="14"/>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C124" s="8"/>
+      <c r="C124" s="13"/>
+      <c r="D124" s="14"/>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C125" s="8"/>
+      <c r="C125" s="13"/>
+      <c r="D125" s="14"/>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C126" s="8"/>
+      <c r="C126" s="13"/>
+      <c r="D126" s="14"/>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C127" s="8"/>
+      <c r="C127" s="13"/>
+      <c r="D127" s="14"/>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C128" s="8"/>
+      <c r="C128" s="13"/>
+      <c r="D128" s="14"/>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C129" s="8"/>
+      <c r="C129" s="13"/>
+      <c r="D129" s="14"/>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C130" s="8"/>
+      <c r="C130" s="13"/>
+      <c r="D130" s="14"/>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C131" s="8"/>
+      <c r="C131" s="13"/>
+      <c r="D131" s="14"/>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C132" s="8"/>
+      <c r="C132" s="13"/>
+      <c r="D132" s="14"/>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C133" s="8"/>
+      <c r="C133" s="13"/>
+      <c r="D133" s="14"/>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C134" s="8"/>
+      <c r="C134" s="13"/>
+      <c r="D134" s="14"/>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C135" s="8"/>
+      <c r="C135" s="13"/>
+      <c r="D135" s="14"/>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C136" s="8"/>
+      <c r="C136" s="13"/>
+      <c r="D136" s="14"/>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C137" s="8"/>
+      <c r="C137" s="13"/>
+      <c r="D137" s="14"/>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C138" s="8"/>
+      <c r="C138" s="13"/>
+      <c r="D138" s="14"/>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C139" s="8"/>
+      <c r="C139" s="13"/>
+      <c r="D139" s="14"/>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C140" s="8"/>
+      <c r="C140" s="13"/>
+      <c r="D140" s="14"/>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C141" s="8"/>
+      <c r="C141" s="13"/>
+      <c r="D141" s="14"/>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C142" s="8"/>
+      <c r="C142" s="13"/>
+      <c r="D142" s="14"/>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C143" s="8"/>
+      <c r="C143" s="13"/>
+      <c r="D143" s="14"/>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C144" s="8"/>
+      <c r="C144" s="13"/>
+      <c r="D144" s="14"/>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C145" s="8"/>
+      <c r="C145" s="13"/>
+      <c r="D145" s="14"/>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C146" s="8"/>
+      <c r="C146" s="13"/>
+      <c r="D146" s="14"/>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C147" s="8"/>
+      <c r="C147" s="13"/>
+      <c r="D147" s="14"/>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C148" s="8"/>
+      <c r="C148" s="13"/>
+      <c r="D148" s="14"/>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C149" s="8"/>
+      <c r="C149" s="13"/>
+      <c r="D149" s="14"/>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C150" s="8"/>
+      <c r="C150" s="13"/>
+      <c r="D150" s="14"/>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C151" s="8"/>
+      <c r="C151" s="13"/>
+      <c r="D151" s="14"/>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C152" s="8"/>
+      <c r="C152" s="13"/>
+      <c r="D152" s="14"/>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C153" s="8"/>
+      <c r="C153" s="13"/>
+      <c r="D153" s="14"/>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C154" s="8"/>
+      <c r="C154" s="13"/>
+      <c r="D154" s="14"/>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C155" s="8"/>
+      <c r="C155" s="13"/>
+      <c r="D155" s="14"/>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C156" s="8"/>
+      <c r="C156" s="13"/>
+      <c r="D156" s="14"/>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C157" s="8"/>
+      <c r="C157" s="13"/>
+      <c r="D157" s="14"/>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C158" s="8"/>
+      <c r="C158" s="13"/>
+      <c r="D158" s="14"/>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C159" s="8"/>
+      <c r="C159" s="13"/>
+      <c r="D159" s="14"/>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C160" s="8"/>
+      <c r="C160" s="13"/>
+      <c r="D160" s="14"/>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C161" s="8"/>
+      <c r="C161" s="13"/>
+      <c r="D161" s="14"/>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C162" s="8"/>
+      <c r="C162" s="13"/>
+      <c r="D162" s="14"/>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C163" s="8"/>
+      <c r="C163" s="13"/>
+      <c r="D163" s="14"/>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C164" s="8"/>
+      <c r="C164" s="13"/>
+      <c r="D164" s="14"/>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C165" s="8"/>
+      <c r="C165" s="13"/>
+      <c r="D165" s="14"/>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C166" s="8"/>
+      <c r="C166" s="13"/>
+      <c r="D166" s="14"/>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C167" s="8"/>
+      <c r="C167" s="13"/>
+      <c r="D167" s="14"/>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C168" s="8"/>
+      <c r="C168" s="13"/>
+      <c r="D168" s="14"/>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C169" s="8"/>
+      <c r="C169" s="13"/>
+      <c r="D169" s="14"/>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C170" s="8"/>
+      <c r="C170" s="13"/>
+      <c r="D170" s="14"/>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C171" s="8"/>
+      <c r="C171" s="13"/>
+      <c r="D171" s="14"/>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C172" s="8"/>
+      <c r="C172" s="13"/>
+      <c r="D172" s="14"/>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C173" s="8"/>
+      <c r="C173" s="13"/>
+      <c r="D173" s="14"/>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C174" s="8"/>
+      <c r="C174" s="13"/>
+      <c r="D174" s="14"/>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C175" s="8"/>
+      <c r="C175" s="13"/>
+      <c r="D175" s="14"/>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C176" s="8"/>
+      <c r="C176" s="13"/>
+      <c r="D176" s="14"/>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C177" s="8"/>
+      <c r="C177" s="13"/>
+      <c r="D177" s="14"/>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C178" s="8"/>
+      <c r="C178" s="13"/>
+      <c r="D178" s="14"/>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C179" s="8"/>
+      <c r="C179" s="13"/>
+      <c r="D179" s="14"/>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C180" s="8"/>
+      <c r="C180" s="13"/>
+      <c r="D180" s="14"/>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C181" s="8"/>
+      <c r="C181" s="13"/>
+      <c r="D181" s="14"/>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C182" s="8"/>
+      <c r="C182" s="13"/>
+      <c r="D182" s="14"/>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C183" s="8"/>
+      <c r="C183" s="13"/>
+      <c r="D183" s="14"/>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C184" s="8"/>
+      <c r="C184" s="13"/>
+      <c r="D184" s="14"/>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C185" s="8"/>
+      <c r="C185" s="13"/>
+      <c r="D185" s="14"/>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C186" s="8"/>
+      <c r="C186" s="13"/>
+      <c r="D186" s="14"/>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C187" s="8"/>
+      <c r="C187" s="13"/>
+      <c r="D187" s="14"/>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C188" s="8"/>
+      <c r="C188" s="13"/>
+      <c r="D188" s="14"/>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C189" s="8"/>
+      <c r="C189" s="13"/>
+      <c r="D189" s="14"/>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C190" s="8"/>
+      <c r="C190" s="13"/>
+      <c r="D190" s="14"/>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C191" s="8"/>
+      <c r="C191" s="13"/>
+      <c r="D191" s="14"/>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C192" s="8"/>
+      <c r="C192" s="13"/>
+      <c r="D192" s="14"/>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C193" s="8"/>
+      <c r="C193" s="13"/>
+      <c r="D193" s="14"/>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C194" s="8"/>
+      <c r="C194" s="13"/>
+      <c r="D194" s="14"/>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C195" s="8"/>
+      <c r="C195" s="13"/>
+      <c r="D195" s="14"/>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C196" s="8"/>
+      <c r="C196" s="13"/>
+      <c r="D196" s="14"/>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C197" s="8"/>
+      <c r="C197" s="13"/>
+      <c r="D197" s="14"/>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C198" s="8"/>
+      <c r="C198" s="13"/>
+      <c r="D198" s="14"/>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Add production to cluster and project
</commit_message>
<xml_diff>
--- a/core/import_data/resources/projects_v2/project_clusters_06_05_2025.xlsx
+++ b/core/import_data/resources/projects_v2/project_clusters_06_05_2025.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="77">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">Dashboard group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Production</t>
   </si>
   <si>
     <t xml:space="preserve">Action</t>
@@ -52,6 +55,9 @@
     <t xml:space="preserve">Consumption</t>
   </si>
   <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kigali Implementation Plan Stage 2</t>
   </si>
   <si>
@@ -70,7 +76,7 @@
     <t xml:space="preserve">KPP1</t>
   </si>
   <si>
-    <t xml:space="preserve">Production</t>
+    <t xml:space="preserve">Y</t>
   </si>
   <si>
     <t xml:space="preserve">Kigali Implementation Plan Production Stage 2</t>
@@ -148,34 +154,10 @@
     <t xml:space="preserve">IND</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Consumption</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/Production</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">HCFC Individual</t>
   </si>
   <si>
     <t xml:space="preserve">HCFCIND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consumption </t>
   </si>
   <si>
     <t xml:space="preserve">Energy Efficiency</t>
@@ -279,7 +261,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -337,12 +319,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -420,7 +396,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -457,11 +433,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -469,7 +441,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -477,7 +449,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -485,7 +457,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -493,7 +465,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -751,10 +723,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:WT1048576"/>
+  <dimension ref="A1:WU1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D:D"/>
+      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -763,8 +735,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="25.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.8"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.8"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -780,13 +753,15 @@
       <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6"/>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
@@ -805,215 +780,254 @@
       <c r="W1" s="6"/>
       <c r="X1" s="6"/>
       <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="E3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3"/>
       <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="3"/>
       <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="F14" s="3"/>
-      <c r="H14" s="1"/>
+      <c r="G14" s="3"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1573,23 +1587,26 @@
       <c r="US14" s="1"/>
       <c r="UT14" s="1"/>
       <c r="UU14" s="1"/>
+      <c r="UV14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="F15" s="3"/>
-      <c r="H15" s="1"/>
+      <c r="G15" s="3"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -2149,23 +2166,26 @@
       <c r="US15" s="1"/>
       <c r="UT15" s="1"/>
       <c r="UU15" s="1"/>
+      <c r="UV15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="F16" s="3"/>
-      <c r="H16" s="1"/>
+      <c r="G16" s="3"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -2725,22 +2745,26 @@
       <c r="US16" s="1"/>
       <c r="UT16" s="1"/>
       <c r="UU16" s="1"/>
+      <c r="UV16" s="1"/>
     </row>
     <row r="17" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>41</v>
-      </c>
       <c r="D17" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E17" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
     </row>
     <row r="18" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
@@ -2750,15 +2774,18 @@
         <v>47</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2770,15 +2797,18 @@
         <v>51</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="F19" s="3"/>
-    </row>
-    <row r="20" s="10" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" s="9" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
         <v>52</v>
       </c>
@@ -2786,14 +2816,16 @@
         <v>53</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D20" s="8"/>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="1"/>
+      <c r="G20" s="3"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -2812,8 +2844,9 @@
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
-    </row>
-    <row r="21" s="10" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="Z20" s="1"/>
+    </row>
+    <row r="21" s="9" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
         <v>55</v>
       </c>
@@ -2821,14 +2854,16 @@
         <v>56</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D21" s="8"/>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="1"/>
+      <c r="G21" s="3"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -2847,6 +2882,7 @@
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
     </row>
     <row r="22" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
@@ -2856,13 +2892,16 @@
         <v>58</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D22" s="8"/>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
     </row>
     <row r="23" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
@@ -2872,13 +2911,16 @@
         <v>60</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D23" s="8"/>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
     </row>
     <row r="24" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
@@ -2888,13 +2930,16 @@
         <v>62</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D24" s="8"/>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
     </row>
     <row r="25" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
@@ -2904,13 +2949,16 @@
         <v>64</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D25" s="8"/>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
     </row>
     <row r="26" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
@@ -2920,13 +2968,16 @@
         <v>66</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="E26" s="3"/>
+      <c r="E26" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
     </row>
     <row r="27" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
@@ -2935,10 +2986,13 @@
       <c r="B27" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="12"/>
+      <c r="C27" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="11"/>
+      <c r="E27" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="28" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
@@ -2947,11 +3001,14 @@
       <c r="B28" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C28" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="12"/>
-      <c r="E28" s="1" t="s">
+      <c r="C28" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="11"/>
+      <c r="E28" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2962,43 +3019,52 @@
       <c r="B29" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="14"/>
-      <c r="E29" s="15" t="s">
+      <c r="C29" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="13"/>
+      <c r="E29" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D30" s="14"/>
+      <c r="C30" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="13"/>
+      <c r="E30" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="31" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C31" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D31" s="14"/>
+      <c r="C31" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="13"/>
+      <c r="E31" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C32" s="13"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="1"/>
-      <c r="H32" s="1"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -3609,12 +3675,13 @@
       <c r="WR32" s="1"/>
       <c r="WS32" s="1"/>
       <c r="WT32" s="1"/>
+      <c r="WU32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C33" s="13"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="1"/>
-      <c r="H33" s="1"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -4225,12 +4292,13 @@
       <c r="WR33" s="1"/>
       <c r="WS33" s="1"/>
       <c r="WT33" s="1"/>
+      <c r="WU33" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C34" s="13"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="1"/>
-      <c r="H34" s="1"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
@@ -4841,12 +4909,13 @@
       <c r="WR34" s="1"/>
       <c r="WS34" s="1"/>
       <c r="WT34" s="1"/>
+      <c r="WU34" s="1"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C35" s="13"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="1"/>
-      <c r="H35" s="1"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -5406,14 +5475,15 @@
       <c r="US35" s="1"/>
       <c r="UT35" s="1"/>
       <c r="UU35" s="1"/>
+      <c r="UV35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="16"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="17"/>
+      <c r="A36" s="15"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="16"/>
       <c r="E36" s="16"/>
-      <c r="H36" s="1"/>
+      <c r="F36" s="15"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
@@ -5973,655 +6043,816 @@
       <c r="US36" s="1"/>
       <c r="UT36" s="1"/>
       <c r="UU36" s="1"/>
+      <c r="UV36" s="1"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="18"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="19"/>
+      <c r="A37" s="17"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="18"/>
       <c r="E37" s="18"/>
+      <c r="F37" s="17"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C40" s="13"/>
-      <c r="D40" s="14"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C41" s="13"/>
-      <c r="D41" s="14"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C42" s="13"/>
-      <c r="D42" s="14"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C43" s="13"/>
-      <c r="D43" s="14"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C44" s="13"/>
-      <c r="D44" s="14"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C45" s="13"/>
-      <c r="D45" s="14"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C46" s="13"/>
-      <c r="D46" s="14"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C47" s="13"/>
-      <c r="D47" s="14"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C48" s="13"/>
-      <c r="D48" s="14"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C49" s="13"/>
-      <c r="D49" s="14"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C50" s="13"/>
-      <c r="D50" s="14"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C51" s="13"/>
-      <c r="D51" s="14"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C52" s="13"/>
-      <c r="D52" s="14"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C53" s="13"/>
-      <c r="D53" s="14"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C54" s="13"/>
-      <c r="D54" s="14"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C55" s="13"/>
-      <c r="D55" s="14"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C56" s="13"/>
-      <c r="D56" s="14"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C57" s="13"/>
-      <c r="D57" s="14"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C58" s="13"/>
-      <c r="D58" s="14"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C59" s="13"/>
-      <c r="D59" s="14"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C60" s="13"/>
-      <c r="D60" s="14"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C61" s="13"/>
-      <c r="D61" s="14"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C62" s="13"/>
-      <c r="D62" s="14"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="13"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C63" s="13"/>
-      <c r="D63" s="14"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C64" s="13"/>
-      <c r="D64" s="14"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C65" s="13"/>
-      <c r="D65" s="14"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="13"/>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C66" s="13"/>
-      <c r="D66" s="14"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C67" s="13"/>
-      <c r="D67" s="14"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C68" s="13"/>
-      <c r="D68" s="14"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="13"/>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C69" s="13"/>
-      <c r="D69" s="14"/>
+      <c r="C69" s="12"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="13"/>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C70" s="13"/>
-      <c r="D70" s="14"/>
+      <c r="C70" s="12"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="13"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C71" s="13"/>
-      <c r="D71" s="14"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="13"/>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C72" s="13"/>
-      <c r="D72" s="14"/>
+      <c r="C72" s="12"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="13"/>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C73" s="13"/>
-      <c r="D73" s="14"/>
+      <c r="C73" s="12"/>
+      <c r="D73" s="13"/>
+      <c r="E73" s="13"/>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C74" s="13"/>
-      <c r="D74" s="14"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="13"/>
+      <c r="E74" s="13"/>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C75" s="13"/>
-      <c r="D75" s="14"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="13"/>
+      <c r="E75" s="13"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C76" s="13"/>
-      <c r="D76" s="14"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="13"/>
+      <c r="E76" s="13"/>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C77" s="13"/>
-      <c r="D77" s="14"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="13"/>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C78" s="13"/>
-      <c r="D78" s="14"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="13"/>
+      <c r="E78" s="13"/>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C79" s="13"/>
-      <c r="D79" s="14"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="13"/>
+      <c r="E79" s="13"/>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C80" s="13"/>
-      <c r="D80" s="14"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="13"/>
+      <c r="E80" s="13"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C81" s="13"/>
-      <c r="D81" s="14"/>
+      <c r="C81" s="12"/>
+      <c r="D81" s="13"/>
+      <c r="E81" s="13"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C82" s="13"/>
-      <c r="D82" s="14"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="13"/>
+      <c r="E82" s="13"/>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C83" s="13"/>
-      <c r="D83" s="14"/>
+      <c r="C83" s="12"/>
+      <c r="D83" s="13"/>
+      <c r="E83" s="13"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C84" s="13"/>
-      <c r="D84" s="14"/>
+      <c r="C84" s="12"/>
+      <c r="D84" s="13"/>
+      <c r="E84" s="13"/>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C85" s="13"/>
-      <c r="D85" s="14"/>
+      <c r="C85" s="12"/>
+      <c r="D85" s="13"/>
+      <c r="E85" s="13"/>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C86" s="13"/>
-      <c r="D86" s="14"/>
+      <c r="C86" s="12"/>
+      <c r="D86" s="13"/>
+      <c r="E86" s="13"/>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C87" s="13"/>
-      <c r="D87" s="14"/>
+      <c r="C87" s="12"/>
+      <c r="D87" s="13"/>
+      <c r="E87" s="13"/>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C88" s="13"/>
-      <c r="D88" s="14"/>
+      <c r="C88" s="12"/>
+      <c r="D88" s="13"/>
+      <c r="E88" s="13"/>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C89" s="13"/>
-      <c r="D89" s="14"/>
+      <c r="C89" s="12"/>
+      <c r="D89" s="13"/>
+      <c r="E89" s="13"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C90" s="13"/>
-      <c r="D90" s="14"/>
+      <c r="C90" s="12"/>
+      <c r="D90" s="13"/>
+      <c r="E90" s="13"/>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C91" s="13"/>
-      <c r="D91" s="14"/>
+      <c r="C91" s="12"/>
+      <c r="D91" s="13"/>
+      <c r="E91" s="13"/>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C92" s="13"/>
-      <c r="D92" s="14"/>
+      <c r="C92" s="12"/>
+      <c r="D92" s="13"/>
+      <c r="E92" s="13"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C93" s="13"/>
-      <c r="D93" s="14"/>
+      <c r="C93" s="12"/>
+      <c r="D93" s="13"/>
+      <c r="E93" s="13"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C94" s="13"/>
-      <c r="D94" s="14"/>
+      <c r="C94" s="12"/>
+      <c r="D94" s="13"/>
+      <c r="E94" s="13"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C95" s="13"/>
-      <c r="D95" s="14"/>
+      <c r="C95" s="12"/>
+      <c r="D95" s="13"/>
+      <c r="E95" s="13"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C96" s="13"/>
-      <c r="D96" s="14"/>
+      <c r="C96" s="12"/>
+      <c r="D96" s="13"/>
+      <c r="E96" s="13"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C97" s="13"/>
-      <c r="D97" s="14"/>
+      <c r="C97" s="12"/>
+      <c r="D97" s="13"/>
+      <c r="E97" s="13"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C98" s="13"/>
-      <c r="D98" s="14"/>
+      <c r="C98" s="12"/>
+      <c r="D98" s="13"/>
+      <c r="E98" s="13"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C99" s="13"/>
-      <c r="D99" s="14"/>
+      <c r="C99" s="12"/>
+      <c r="D99" s="13"/>
+      <c r="E99" s="13"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C100" s="13"/>
-      <c r="D100" s="14"/>
+      <c r="C100" s="12"/>
+      <c r="D100" s="13"/>
+      <c r="E100" s="13"/>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C101" s="13"/>
-      <c r="D101" s="14"/>
+      <c r="C101" s="12"/>
+      <c r="D101" s="13"/>
+      <c r="E101" s="13"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C102" s="13"/>
-      <c r="D102" s="14"/>
+      <c r="C102" s="12"/>
+      <c r="D102" s="13"/>
+      <c r="E102" s="13"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C103" s="13"/>
-      <c r="D103" s="14"/>
+      <c r="C103" s="12"/>
+      <c r="D103" s="13"/>
+      <c r="E103" s="13"/>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C104" s="13"/>
-      <c r="D104" s="14"/>
+      <c r="C104" s="12"/>
+      <c r="D104" s="13"/>
+      <c r="E104" s="13"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C105" s="13"/>
-      <c r="D105" s="14"/>
+      <c r="C105" s="12"/>
+      <c r="D105" s="13"/>
+      <c r="E105" s="13"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C106" s="13"/>
-      <c r="D106" s="14"/>
+      <c r="C106" s="12"/>
+      <c r="D106" s="13"/>
+      <c r="E106" s="13"/>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C107" s="13"/>
-      <c r="D107" s="14"/>
+      <c r="C107" s="12"/>
+      <c r="D107" s="13"/>
+      <c r="E107" s="13"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C108" s="13"/>
-      <c r="D108" s="14"/>
+      <c r="C108" s="12"/>
+      <c r="D108" s="13"/>
+      <c r="E108" s="13"/>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C109" s="13"/>
-      <c r="D109" s="14"/>
+      <c r="C109" s="12"/>
+      <c r="D109" s="13"/>
+      <c r="E109" s="13"/>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C110" s="13"/>
-      <c r="D110" s="14"/>
+      <c r="C110" s="12"/>
+      <c r="D110" s="13"/>
+      <c r="E110" s="13"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C111" s="13"/>
-      <c r="D111" s="14"/>
+      <c r="C111" s="12"/>
+      <c r="D111" s="13"/>
+      <c r="E111" s="13"/>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C112" s="13"/>
-      <c r="D112" s="14"/>
+      <c r="C112" s="12"/>
+      <c r="D112" s="13"/>
+      <c r="E112" s="13"/>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C113" s="13"/>
-      <c r="D113" s="14"/>
+      <c r="C113" s="12"/>
+      <c r="D113" s="13"/>
+      <c r="E113" s="13"/>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C114" s="13"/>
-      <c r="D114" s="14"/>
+      <c r="C114" s="12"/>
+      <c r="D114" s="13"/>
+      <c r="E114" s="13"/>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C115" s="13"/>
-      <c r="D115" s="14"/>
+      <c r="C115" s="12"/>
+      <c r="D115" s="13"/>
+      <c r="E115" s="13"/>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C116" s="13"/>
-      <c r="D116" s="14"/>
+      <c r="C116" s="12"/>
+      <c r="D116" s="13"/>
+      <c r="E116" s="13"/>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C117" s="13"/>
-      <c r="D117" s="14"/>
+      <c r="C117" s="12"/>
+      <c r="D117" s="13"/>
+      <c r="E117" s="13"/>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C118" s="13"/>
-      <c r="D118" s="14"/>
+      <c r="C118" s="12"/>
+      <c r="D118" s="13"/>
+      <c r="E118" s="13"/>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C119" s="13"/>
-      <c r="D119" s="14"/>
+      <c r="C119" s="12"/>
+      <c r="D119" s="13"/>
+      <c r="E119" s="13"/>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C120" s="13"/>
-      <c r="D120" s="14"/>
+      <c r="C120" s="12"/>
+      <c r="D120" s="13"/>
+      <c r="E120" s="13"/>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C121" s="13"/>
-      <c r="D121" s="14"/>
+      <c r="C121" s="12"/>
+      <c r="D121" s="13"/>
+      <c r="E121" s="13"/>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C122" s="13"/>
-      <c r="D122" s="14"/>
+      <c r="C122" s="12"/>
+      <c r="D122" s="13"/>
+      <c r="E122" s="13"/>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C123" s="13"/>
-      <c r="D123" s="14"/>
+      <c r="C123" s="12"/>
+      <c r="D123" s="13"/>
+      <c r="E123" s="13"/>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C124" s="13"/>
-      <c r="D124" s="14"/>
+      <c r="C124" s="12"/>
+      <c r="D124" s="13"/>
+      <c r="E124" s="13"/>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C125" s="13"/>
-      <c r="D125" s="14"/>
+      <c r="C125" s="12"/>
+      <c r="D125" s="13"/>
+      <c r="E125" s="13"/>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C126" s="13"/>
-      <c r="D126" s="14"/>
+      <c r="C126" s="12"/>
+      <c r="D126" s="13"/>
+      <c r="E126" s="13"/>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C127" s="13"/>
-      <c r="D127" s="14"/>
+      <c r="C127" s="12"/>
+      <c r="D127" s="13"/>
+      <c r="E127" s="13"/>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C128" s="13"/>
-      <c r="D128" s="14"/>
+      <c r="C128" s="12"/>
+      <c r="D128" s="13"/>
+      <c r="E128" s="13"/>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C129" s="13"/>
-      <c r="D129" s="14"/>
+      <c r="C129" s="12"/>
+      <c r="D129" s="13"/>
+      <c r="E129" s="13"/>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C130" s="13"/>
-      <c r="D130" s="14"/>
+      <c r="C130" s="12"/>
+      <c r="D130" s="13"/>
+      <c r="E130" s="13"/>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C131" s="13"/>
-      <c r="D131" s="14"/>
+      <c r="C131" s="12"/>
+      <c r="D131" s="13"/>
+      <c r="E131" s="13"/>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C132" s="13"/>
-      <c r="D132" s="14"/>
+      <c r="C132" s="12"/>
+      <c r="D132" s="13"/>
+      <c r="E132" s="13"/>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C133" s="13"/>
-      <c r="D133" s="14"/>
+      <c r="C133" s="12"/>
+      <c r="D133" s="13"/>
+      <c r="E133" s="13"/>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C134" s="13"/>
-      <c r="D134" s="14"/>
+      <c r="C134" s="12"/>
+      <c r="D134" s="13"/>
+      <c r="E134" s="13"/>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C135" s="13"/>
-      <c r="D135" s="14"/>
+      <c r="C135" s="12"/>
+      <c r="D135" s="13"/>
+      <c r="E135" s="13"/>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C136" s="13"/>
-      <c r="D136" s="14"/>
+      <c r="C136" s="12"/>
+      <c r="D136" s="13"/>
+      <c r="E136" s="13"/>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C137" s="13"/>
-      <c r="D137" s="14"/>
+      <c r="C137" s="12"/>
+      <c r="D137" s="13"/>
+      <c r="E137" s="13"/>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C138" s="13"/>
-      <c r="D138" s="14"/>
+      <c r="C138" s="12"/>
+      <c r="D138" s="13"/>
+      <c r="E138" s="13"/>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C139" s="13"/>
-      <c r="D139" s="14"/>
+      <c r="C139" s="12"/>
+      <c r="D139" s="13"/>
+      <c r="E139" s="13"/>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C140" s="13"/>
-      <c r="D140" s="14"/>
+      <c r="C140" s="12"/>
+      <c r="D140" s="13"/>
+      <c r="E140" s="13"/>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C141" s="13"/>
-      <c r="D141" s="14"/>
+      <c r="C141" s="12"/>
+      <c r="D141" s="13"/>
+      <c r="E141" s="13"/>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C142" s="13"/>
-      <c r="D142" s="14"/>
+      <c r="C142" s="12"/>
+      <c r="D142" s="13"/>
+      <c r="E142" s="13"/>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C143" s="13"/>
-      <c r="D143" s="14"/>
+      <c r="C143" s="12"/>
+      <c r="D143" s="13"/>
+      <c r="E143" s="13"/>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C144" s="13"/>
-      <c r="D144" s="14"/>
+      <c r="C144" s="12"/>
+      <c r="D144" s="13"/>
+      <c r="E144" s="13"/>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C145" s="13"/>
-      <c r="D145" s="14"/>
+      <c r="C145" s="12"/>
+      <c r="D145" s="13"/>
+      <c r="E145" s="13"/>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C146" s="13"/>
-      <c r="D146" s="14"/>
+      <c r="C146" s="12"/>
+      <c r="D146" s="13"/>
+      <c r="E146" s="13"/>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C147" s="13"/>
-      <c r="D147" s="14"/>
+      <c r="C147" s="12"/>
+      <c r="D147" s="13"/>
+      <c r="E147" s="13"/>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C148" s="13"/>
-      <c r="D148" s="14"/>
+      <c r="C148" s="12"/>
+      <c r="D148" s="13"/>
+      <c r="E148" s="13"/>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C149" s="13"/>
-      <c r="D149" s="14"/>
+      <c r="C149" s="12"/>
+      <c r="D149" s="13"/>
+      <c r="E149" s="13"/>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C150" s="13"/>
-      <c r="D150" s="14"/>
+      <c r="C150" s="12"/>
+      <c r="D150" s="13"/>
+      <c r="E150" s="13"/>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C151" s="13"/>
-      <c r="D151" s="14"/>
+      <c r="C151" s="12"/>
+      <c r="D151" s="13"/>
+      <c r="E151" s="13"/>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C152" s="13"/>
-      <c r="D152" s="14"/>
+      <c r="C152" s="12"/>
+      <c r="D152" s="13"/>
+      <c r="E152" s="13"/>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C153" s="13"/>
-      <c r="D153" s="14"/>
+      <c r="C153" s="12"/>
+      <c r="D153" s="13"/>
+      <c r="E153" s="13"/>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C154" s="13"/>
-      <c r="D154" s="14"/>
+      <c r="C154" s="12"/>
+      <c r="D154" s="13"/>
+      <c r="E154" s="13"/>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C155" s="13"/>
-      <c r="D155" s="14"/>
+      <c r="C155" s="12"/>
+      <c r="D155" s="13"/>
+      <c r="E155" s="13"/>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C156" s="13"/>
-      <c r="D156" s="14"/>
+      <c r="C156" s="12"/>
+      <c r="D156" s="13"/>
+      <c r="E156" s="13"/>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C157" s="13"/>
-      <c r="D157" s="14"/>
+      <c r="C157" s="12"/>
+      <c r="D157" s="13"/>
+      <c r="E157" s="13"/>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C158" s="13"/>
-      <c r="D158" s="14"/>
+      <c r="C158" s="12"/>
+      <c r="D158" s="13"/>
+      <c r="E158" s="13"/>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C159" s="13"/>
-      <c r="D159" s="14"/>
+      <c r="C159" s="12"/>
+      <c r="D159" s="13"/>
+      <c r="E159" s="13"/>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C160" s="13"/>
-      <c r="D160" s="14"/>
+      <c r="C160" s="12"/>
+      <c r="D160" s="13"/>
+      <c r="E160" s="13"/>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C161" s="13"/>
-      <c r="D161" s="14"/>
+      <c r="C161" s="12"/>
+      <c r="D161" s="13"/>
+      <c r="E161" s="13"/>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C162" s="13"/>
-      <c r="D162" s="14"/>
+      <c r="C162" s="12"/>
+      <c r="D162" s="13"/>
+      <c r="E162" s="13"/>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C163" s="13"/>
-      <c r="D163" s="14"/>
+      <c r="C163" s="12"/>
+      <c r="D163" s="13"/>
+      <c r="E163" s="13"/>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C164" s="13"/>
-      <c r="D164" s="14"/>
+      <c r="C164" s="12"/>
+      <c r="D164" s="13"/>
+      <c r="E164" s="13"/>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C165" s="13"/>
-      <c r="D165" s="14"/>
+      <c r="C165" s="12"/>
+      <c r="D165" s="13"/>
+      <c r="E165" s="13"/>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C166" s="13"/>
-      <c r="D166" s="14"/>
+      <c r="C166" s="12"/>
+      <c r="D166" s="13"/>
+      <c r="E166" s="13"/>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C167" s="13"/>
-      <c r="D167" s="14"/>
+      <c r="C167" s="12"/>
+      <c r="D167" s="13"/>
+      <c r="E167" s="13"/>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C168" s="13"/>
-      <c r="D168" s="14"/>
+      <c r="C168" s="12"/>
+      <c r="D168" s="13"/>
+      <c r="E168" s="13"/>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C169" s="13"/>
-      <c r="D169" s="14"/>
+      <c r="C169" s="12"/>
+      <c r="D169" s="13"/>
+      <c r="E169" s="13"/>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C170" s="13"/>
-      <c r="D170" s="14"/>
+      <c r="C170" s="12"/>
+      <c r="D170" s="13"/>
+      <c r="E170" s="13"/>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C171" s="13"/>
-      <c r="D171" s="14"/>
+      <c r="C171" s="12"/>
+      <c r="D171" s="13"/>
+      <c r="E171" s="13"/>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C172" s="13"/>
-      <c r="D172" s="14"/>
+      <c r="C172" s="12"/>
+      <c r="D172" s="13"/>
+      <c r="E172" s="13"/>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C173" s="13"/>
-      <c r="D173" s="14"/>
+      <c r="C173" s="12"/>
+      <c r="D173" s="13"/>
+      <c r="E173" s="13"/>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C174" s="13"/>
-      <c r="D174" s="14"/>
+      <c r="C174" s="12"/>
+      <c r="D174" s="13"/>
+      <c r="E174" s="13"/>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C175" s="13"/>
-      <c r="D175" s="14"/>
+      <c r="C175" s="12"/>
+      <c r="D175" s="13"/>
+      <c r="E175" s="13"/>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C176" s="13"/>
-      <c r="D176" s="14"/>
+      <c r="C176" s="12"/>
+      <c r="D176" s="13"/>
+      <c r="E176" s="13"/>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C177" s="13"/>
-      <c r="D177" s="14"/>
+      <c r="C177" s="12"/>
+      <c r="D177" s="13"/>
+      <c r="E177" s="13"/>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C178" s="13"/>
-      <c r="D178" s="14"/>
+      <c r="C178" s="12"/>
+      <c r="D178" s="13"/>
+      <c r="E178" s="13"/>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C179" s="13"/>
-      <c r="D179" s="14"/>
+      <c r="C179" s="12"/>
+      <c r="D179" s="13"/>
+      <c r="E179" s="13"/>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C180" s="13"/>
-      <c r="D180" s="14"/>
+      <c r="C180" s="12"/>
+      <c r="D180" s="13"/>
+      <c r="E180" s="13"/>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C181" s="13"/>
-      <c r="D181" s="14"/>
+      <c r="C181" s="12"/>
+      <c r="D181" s="13"/>
+      <c r="E181" s="13"/>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C182" s="13"/>
-      <c r="D182" s="14"/>
+      <c r="C182" s="12"/>
+      <c r="D182" s="13"/>
+      <c r="E182" s="13"/>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C183" s="13"/>
-      <c r="D183" s="14"/>
+      <c r="C183" s="12"/>
+      <c r="D183" s="13"/>
+      <c r="E183" s="13"/>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C184" s="13"/>
-      <c r="D184" s="14"/>
+      <c r="C184" s="12"/>
+      <c r="D184" s="13"/>
+      <c r="E184" s="13"/>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C185" s="13"/>
-      <c r="D185" s="14"/>
+      <c r="C185" s="12"/>
+      <c r="D185" s="13"/>
+      <c r="E185" s="13"/>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C186" s="13"/>
-      <c r="D186" s="14"/>
+      <c r="C186" s="12"/>
+      <c r="D186" s="13"/>
+      <c r="E186" s="13"/>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C187" s="13"/>
-      <c r="D187" s="14"/>
+      <c r="C187" s="12"/>
+      <c r="D187" s="13"/>
+      <c r="E187" s="13"/>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C188" s="13"/>
-      <c r="D188" s="14"/>
+      <c r="C188" s="12"/>
+      <c r="D188" s="13"/>
+      <c r="E188" s="13"/>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C189" s="13"/>
-      <c r="D189" s="14"/>
+      <c r="C189" s="12"/>
+      <c r="D189" s="13"/>
+      <c r="E189" s="13"/>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C190" s="13"/>
-      <c r="D190" s="14"/>
+      <c r="C190" s="12"/>
+      <c r="D190" s="13"/>
+      <c r="E190" s="13"/>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C191" s="13"/>
-      <c r="D191" s="14"/>
+      <c r="C191" s="12"/>
+      <c r="D191" s="13"/>
+      <c r="E191" s="13"/>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C192" s="13"/>
-      <c r="D192" s="14"/>
+      <c r="C192" s="12"/>
+      <c r="D192" s="13"/>
+      <c r="E192" s="13"/>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C193" s="13"/>
-      <c r="D193" s="14"/>
+      <c r="C193" s="12"/>
+      <c r="D193" s="13"/>
+      <c r="E193" s="13"/>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C194" s="13"/>
-      <c r="D194" s="14"/>
+      <c r="C194" s="12"/>
+      <c r="D194" s="13"/>
+      <c r="E194" s="13"/>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C195" s="13"/>
-      <c r="D195" s="14"/>
+      <c r="C195" s="12"/>
+      <c r="D195" s="13"/>
+      <c r="E195" s="13"/>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C196" s="13"/>
-      <c r="D196" s="14"/>
+      <c r="C196" s="12"/>
+      <c r="D196" s="13"/>
+      <c r="E196" s="13"/>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C197" s="13"/>
-      <c r="D197" s="14"/>
+      <c r="C197" s="12"/>
+      <c r="D197" s="13"/>
+      <c r="E197" s="13"/>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C198" s="13"/>
-      <c r="D198" s="14"/>
+      <c r="C198" s="12"/>
+      <c r="D198" s="13"/>
+      <c r="E198" s="13"/>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Add production to cluster and project (#708)
</commit_message>
<xml_diff>
--- a/core/import_data/resources/projects_v2/project_clusters_06_05_2025.xlsx
+++ b/core/import_data/resources/projects_v2/project_clusters_06_05_2025.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="77">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">Dashboard group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Production</t>
   </si>
   <si>
     <t xml:space="preserve">Action</t>
@@ -52,6 +55,9 @@
     <t xml:space="preserve">Consumption</t>
   </si>
   <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kigali Implementation Plan Stage 2</t>
   </si>
   <si>
@@ -70,7 +76,7 @@
     <t xml:space="preserve">KPP1</t>
   </si>
   <si>
-    <t xml:space="preserve">Production</t>
+    <t xml:space="preserve">Y</t>
   </si>
   <si>
     <t xml:space="preserve">Kigali Implementation Plan Production Stage 2</t>
@@ -148,34 +154,10 @@
     <t xml:space="preserve">IND</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Consumption</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">/Production</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">HCFC Individual</t>
   </si>
   <si>
     <t xml:space="preserve">HCFCIND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consumption </t>
   </si>
   <si>
     <t xml:space="preserve">Energy Efficiency</t>
@@ -279,7 +261,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -337,12 +319,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -420,7 +396,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -457,11 +433,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -469,7 +441,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -477,7 +449,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -485,7 +457,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -493,7 +465,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -751,10 +723,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:WT1048576"/>
+  <dimension ref="A1:WU1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D:D"/>
+      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -763,8 +735,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="25.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.8"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.8"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -780,13 +753,15 @@
       <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6"/>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
@@ -805,215 +780,254 @@
       <c r="W1" s="6"/>
       <c r="X1" s="6"/>
       <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="E3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3"/>
       <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="3"/>
       <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="F14" s="3"/>
-      <c r="H14" s="1"/>
+      <c r="G14" s="3"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1573,23 +1587,26 @@
       <c r="US14" s="1"/>
       <c r="UT14" s="1"/>
       <c r="UU14" s="1"/>
+      <c r="UV14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="F15" s="3"/>
-      <c r="H15" s="1"/>
+      <c r="G15" s="3"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -2149,23 +2166,26 @@
       <c r="US15" s="1"/>
       <c r="UT15" s="1"/>
       <c r="UU15" s="1"/>
+      <c r="UV15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="F16" s="3"/>
-      <c r="H16" s="1"/>
+      <c r="G16" s="3"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -2725,22 +2745,26 @@
       <c r="US16" s="1"/>
       <c r="UT16" s="1"/>
       <c r="UU16" s="1"/>
+      <c r="UV16" s="1"/>
     </row>
     <row r="17" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>41</v>
-      </c>
       <c r="D17" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E17" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
     </row>
     <row r="18" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
@@ -2750,15 +2774,18 @@
         <v>47</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2770,15 +2797,18 @@
         <v>51</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="F19" s="3"/>
-    </row>
-    <row r="20" s="10" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" s="9" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
         <v>52</v>
       </c>
@@ -2786,14 +2816,16 @@
         <v>53</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D20" s="8"/>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="1"/>
+      <c r="G20" s="3"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -2812,8 +2844,9 @@
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
-    </row>
-    <row r="21" s="10" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="Z20" s="1"/>
+    </row>
+    <row r="21" s="9" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
         <v>55</v>
       </c>
@@ -2821,14 +2854,16 @@
         <v>56</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D21" s="8"/>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="1"/>
+      <c r="G21" s="3"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -2847,6 +2882,7 @@
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
     </row>
     <row r="22" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
@@ -2856,13 +2892,16 @@
         <v>58</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D22" s="8"/>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
     </row>
     <row r="23" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
@@ -2872,13 +2911,16 @@
         <v>60</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D23" s="8"/>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
     </row>
     <row r="24" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
@@ -2888,13 +2930,16 @@
         <v>62</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D24" s="8"/>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
     </row>
     <row r="25" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
@@ -2904,13 +2949,16 @@
         <v>64</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D25" s="8"/>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
     </row>
     <row r="26" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
@@ -2920,13 +2968,16 @@
         <v>66</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="E26" s="3"/>
+      <c r="E26" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
     </row>
     <row r="27" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
@@ -2935,10 +2986,13 @@
       <c r="B27" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="12"/>
+      <c r="C27" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="11"/>
+      <c r="E27" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="28" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
@@ -2947,11 +3001,14 @@
       <c r="B28" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C28" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="12"/>
-      <c r="E28" s="1" t="s">
+      <c r="C28" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="11"/>
+      <c r="E28" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2962,43 +3019,52 @@
       <c r="B29" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="14"/>
-      <c r="E29" s="15" t="s">
+      <c r="C29" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="13"/>
+      <c r="E29" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D30" s="14"/>
+      <c r="C30" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="13"/>
+      <c r="E30" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="31" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C31" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D31" s="14"/>
+      <c r="C31" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="13"/>
+      <c r="E31" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C32" s="13"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="1"/>
-      <c r="H32" s="1"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -3609,12 +3675,13 @@
       <c r="WR32" s="1"/>
       <c r="WS32" s="1"/>
       <c r="WT32" s="1"/>
+      <c r="WU32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C33" s="13"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="1"/>
-      <c r="H33" s="1"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -4225,12 +4292,13 @@
       <c r="WR33" s="1"/>
       <c r="WS33" s="1"/>
       <c r="WT33" s="1"/>
+      <c r="WU33" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C34" s="13"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="1"/>
-      <c r="H34" s="1"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
@@ -4841,12 +4909,13 @@
       <c r="WR34" s="1"/>
       <c r="WS34" s="1"/>
       <c r="WT34" s="1"/>
+      <c r="WU34" s="1"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C35" s="13"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="1"/>
-      <c r="H35" s="1"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -5406,14 +5475,15 @@
       <c r="US35" s="1"/>
       <c r="UT35" s="1"/>
       <c r="UU35" s="1"/>
+      <c r="UV35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="16"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="17"/>
+      <c r="A36" s="15"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="16"/>
       <c r="E36" s="16"/>
-      <c r="H36" s="1"/>
+      <c r="F36" s="15"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
@@ -5973,655 +6043,816 @@
       <c r="US36" s="1"/>
       <c r="UT36" s="1"/>
       <c r="UU36" s="1"/>
+      <c r="UV36" s="1"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="18"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="19"/>
+      <c r="A37" s="17"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="18"/>
       <c r="E37" s="18"/>
+      <c r="F37" s="17"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C40" s="13"/>
-      <c r="D40" s="14"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C41" s="13"/>
-      <c r="D41" s="14"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C42" s="13"/>
-      <c r="D42" s="14"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C43" s="13"/>
-      <c r="D43" s="14"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C44" s="13"/>
-      <c r="D44" s="14"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C45" s="13"/>
-      <c r="D45" s="14"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C46" s="13"/>
-      <c r="D46" s="14"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C47" s="13"/>
-      <c r="D47" s="14"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C48" s="13"/>
-      <c r="D48" s="14"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C49" s="13"/>
-      <c r="D49" s="14"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C50" s="13"/>
-      <c r="D50" s="14"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C51" s="13"/>
-      <c r="D51" s="14"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C52" s="13"/>
-      <c r="D52" s="14"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C53" s="13"/>
-      <c r="D53" s="14"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C54" s="13"/>
-      <c r="D54" s="14"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C55" s="13"/>
-      <c r="D55" s="14"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C56" s="13"/>
-      <c r="D56" s="14"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C57" s="13"/>
-      <c r="D57" s="14"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C58" s="13"/>
-      <c r="D58" s="14"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C59" s="13"/>
-      <c r="D59" s="14"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C60" s="13"/>
-      <c r="D60" s="14"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C61" s="13"/>
-      <c r="D61" s="14"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C62" s="13"/>
-      <c r="D62" s="14"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="13"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C63" s="13"/>
-      <c r="D63" s="14"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C64" s="13"/>
-      <c r="D64" s="14"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C65" s="13"/>
-      <c r="D65" s="14"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="13"/>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C66" s="13"/>
-      <c r="D66" s="14"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C67" s="13"/>
-      <c r="D67" s="14"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C68" s="13"/>
-      <c r="D68" s="14"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="13"/>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C69" s="13"/>
-      <c r="D69" s="14"/>
+      <c r="C69" s="12"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="13"/>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C70" s="13"/>
-      <c r="D70" s="14"/>
+      <c r="C70" s="12"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="13"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C71" s="13"/>
-      <c r="D71" s="14"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="13"/>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C72" s="13"/>
-      <c r="D72" s="14"/>
+      <c r="C72" s="12"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="13"/>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C73" s="13"/>
-      <c r="D73" s="14"/>
+      <c r="C73" s="12"/>
+      <c r="D73" s="13"/>
+      <c r="E73" s="13"/>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C74" s="13"/>
-      <c r="D74" s="14"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="13"/>
+      <c r="E74" s="13"/>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C75" s="13"/>
-      <c r="D75" s="14"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="13"/>
+      <c r="E75" s="13"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C76" s="13"/>
-      <c r="D76" s="14"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="13"/>
+      <c r="E76" s="13"/>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C77" s="13"/>
-      <c r="D77" s="14"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="13"/>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C78" s="13"/>
-      <c r="D78" s="14"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="13"/>
+      <c r="E78" s="13"/>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C79" s="13"/>
-      <c r="D79" s="14"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="13"/>
+      <c r="E79" s="13"/>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C80" s="13"/>
-      <c r="D80" s="14"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="13"/>
+      <c r="E80" s="13"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C81" s="13"/>
-      <c r="D81" s="14"/>
+      <c r="C81" s="12"/>
+      <c r="D81" s="13"/>
+      <c r="E81" s="13"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C82" s="13"/>
-      <c r="D82" s="14"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="13"/>
+      <c r="E82" s="13"/>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C83" s="13"/>
-      <c r="D83" s="14"/>
+      <c r="C83" s="12"/>
+      <c r="D83" s="13"/>
+      <c r="E83" s="13"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C84" s="13"/>
-      <c r="D84" s="14"/>
+      <c r="C84" s="12"/>
+      <c r="D84" s="13"/>
+      <c r="E84" s="13"/>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C85" s="13"/>
-      <c r="D85" s="14"/>
+      <c r="C85" s="12"/>
+      <c r="D85" s="13"/>
+      <c r="E85" s="13"/>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C86" s="13"/>
-      <c r="D86" s="14"/>
+      <c r="C86" s="12"/>
+      <c r="D86" s="13"/>
+      <c r="E86" s="13"/>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C87" s="13"/>
-      <c r="D87" s="14"/>
+      <c r="C87" s="12"/>
+      <c r="D87" s="13"/>
+      <c r="E87" s="13"/>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C88" s="13"/>
-      <c r="D88" s="14"/>
+      <c r="C88" s="12"/>
+      <c r="D88" s="13"/>
+      <c r="E88" s="13"/>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C89" s="13"/>
-      <c r="D89" s="14"/>
+      <c r="C89" s="12"/>
+      <c r="D89" s="13"/>
+      <c r="E89" s="13"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C90" s="13"/>
-      <c r="D90" s="14"/>
+      <c r="C90" s="12"/>
+      <c r="D90" s="13"/>
+      <c r="E90" s="13"/>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C91" s="13"/>
-      <c r="D91" s="14"/>
+      <c r="C91" s="12"/>
+      <c r="D91" s="13"/>
+      <c r="E91" s="13"/>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C92" s="13"/>
-      <c r="D92" s="14"/>
+      <c r="C92" s="12"/>
+      <c r="D92" s="13"/>
+      <c r="E92" s="13"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C93" s="13"/>
-      <c r="D93" s="14"/>
+      <c r="C93" s="12"/>
+      <c r="D93" s="13"/>
+      <c r="E93" s="13"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C94" s="13"/>
-      <c r="D94" s="14"/>
+      <c r="C94" s="12"/>
+      <c r="D94" s="13"/>
+      <c r="E94" s="13"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C95" s="13"/>
-      <c r="D95" s="14"/>
+      <c r="C95" s="12"/>
+      <c r="D95" s="13"/>
+      <c r="E95" s="13"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C96" s="13"/>
-      <c r="D96" s="14"/>
+      <c r="C96" s="12"/>
+      <c r="D96" s="13"/>
+      <c r="E96" s="13"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C97" s="13"/>
-      <c r="D97" s="14"/>
+      <c r="C97" s="12"/>
+      <c r="D97" s="13"/>
+      <c r="E97" s="13"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C98" s="13"/>
-      <c r="D98" s="14"/>
+      <c r="C98" s="12"/>
+      <c r="D98" s="13"/>
+      <c r="E98" s="13"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C99" s="13"/>
-      <c r="D99" s="14"/>
+      <c r="C99" s="12"/>
+      <c r="D99" s="13"/>
+      <c r="E99" s="13"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C100" s="13"/>
-      <c r="D100" s="14"/>
+      <c r="C100" s="12"/>
+      <c r="D100" s="13"/>
+      <c r="E100" s="13"/>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C101" s="13"/>
-      <c r="D101" s="14"/>
+      <c r="C101" s="12"/>
+      <c r="D101" s="13"/>
+      <c r="E101" s="13"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C102" s="13"/>
-      <c r="D102" s="14"/>
+      <c r="C102" s="12"/>
+      <c r="D102" s="13"/>
+      <c r="E102" s="13"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C103" s="13"/>
-      <c r="D103" s="14"/>
+      <c r="C103" s="12"/>
+      <c r="D103" s="13"/>
+      <c r="E103" s="13"/>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C104" s="13"/>
-      <c r="D104" s="14"/>
+      <c r="C104" s="12"/>
+      <c r="D104" s="13"/>
+      <c r="E104" s="13"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C105" s="13"/>
-      <c r="D105" s="14"/>
+      <c r="C105" s="12"/>
+      <c r="D105" s="13"/>
+      <c r="E105" s="13"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C106" s="13"/>
-      <c r="D106" s="14"/>
+      <c r="C106" s="12"/>
+      <c r="D106" s="13"/>
+      <c r="E106" s="13"/>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C107" s="13"/>
-      <c r="D107" s="14"/>
+      <c r="C107" s="12"/>
+      <c r="D107" s="13"/>
+      <c r="E107" s="13"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C108" s="13"/>
-      <c r="D108" s="14"/>
+      <c r="C108" s="12"/>
+      <c r="D108" s="13"/>
+      <c r="E108" s="13"/>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C109" s="13"/>
-      <c r="D109" s="14"/>
+      <c r="C109" s="12"/>
+      <c r="D109" s="13"/>
+      <c r="E109" s="13"/>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C110" s="13"/>
-      <c r="D110" s="14"/>
+      <c r="C110" s="12"/>
+      <c r="D110" s="13"/>
+      <c r="E110" s="13"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C111" s="13"/>
-      <c r="D111" s="14"/>
+      <c r="C111" s="12"/>
+      <c r="D111" s="13"/>
+      <c r="E111" s="13"/>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C112" s="13"/>
-      <c r="D112" s="14"/>
+      <c r="C112" s="12"/>
+      <c r="D112" s="13"/>
+      <c r="E112" s="13"/>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C113" s="13"/>
-      <c r="D113" s="14"/>
+      <c r="C113" s="12"/>
+      <c r="D113" s="13"/>
+      <c r="E113" s="13"/>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C114" s="13"/>
-      <c r="D114" s="14"/>
+      <c r="C114" s="12"/>
+      <c r="D114" s="13"/>
+      <c r="E114" s="13"/>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C115" s="13"/>
-      <c r="D115" s="14"/>
+      <c r="C115" s="12"/>
+      <c r="D115" s="13"/>
+      <c r="E115" s="13"/>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C116" s="13"/>
-      <c r="D116" s="14"/>
+      <c r="C116" s="12"/>
+      <c r="D116" s="13"/>
+      <c r="E116" s="13"/>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C117" s="13"/>
-      <c r="D117" s="14"/>
+      <c r="C117" s="12"/>
+      <c r="D117" s="13"/>
+      <c r="E117" s="13"/>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C118" s="13"/>
-      <c r="D118" s="14"/>
+      <c r="C118" s="12"/>
+      <c r="D118" s="13"/>
+      <c r="E118" s="13"/>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C119" s="13"/>
-      <c r="D119" s="14"/>
+      <c r="C119" s="12"/>
+      <c r="D119" s="13"/>
+      <c r="E119" s="13"/>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C120" s="13"/>
-      <c r="D120" s="14"/>
+      <c r="C120" s="12"/>
+      <c r="D120" s="13"/>
+      <c r="E120" s="13"/>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C121" s="13"/>
-      <c r="D121" s="14"/>
+      <c r="C121" s="12"/>
+      <c r="D121" s="13"/>
+      <c r="E121" s="13"/>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C122" s="13"/>
-      <c r="D122" s="14"/>
+      <c r="C122" s="12"/>
+      <c r="D122" s="13"/>
+      <c r="E122" s="13"/>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C123" s="13"/>
-      <c r="D123" s="14"/>
+      <c r="C123" s="12"/>
+      <c r="D123" s="13"/>
+      <c r="E123" s="13"/>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C124" s="13"/>
-      <c r="D124" s="14"/>
+      <c r="C124" s="12"/>
+      <c r="D124" s="13"/>
+      <c r="E124" s="13"/>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C125" s="13"/>
-      <c r="D125" s="14"/>
+      <c r="C125" s="12"/>
+      <c r="D125" s="13"/>
+      <c r="E125" s="13"/>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C126" s="13"/>
-      <c r="D126" s="14"/>
+      <c r="C126" s="12"/>
+      <c r="D126" s="13"/>
+      <c r="E126" s="13"/>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C127" s="13"/>
-      <c r="D127" s="14"/>
+      <c r="C127" s="12"/>
+      <c r="D127" s="13"/>
+      <c r="E127" s="13"/>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C128" s="13"/>
-      <c r="D128" s="14"/>
+      <c r="C128" s="12"/>
+      <c r="D128" s="13"/>
+      <c r="E128" s="13"/>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C129" s="13"/>
-      <c r="D129" s="14"/>
+      <c r="C129" s="12"/>
+      <c r="D129" s="13"/>
+      <c r="E129" s="13"/>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C130" s="13"/>
-      <c r="D130" s="14"/>
+      <c r="C130" s="12"/>
+      <c r="D130" s="13"/>
+      <c r="E130" s="13"/>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C131" s="13"/>
-      <c r="D131" s="14"/>
+      <c r="C131" s="12"/>
+      <c r="D131" s="13"/>
+      <c r="E131" s="13"/>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C132" s="13"/>
-      <c r="D132" s="14"/>
+      <c r="C132" s="12"/>
+      <c r="D132" s="13"/>
+      <c r="E132" s="13"/>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C133" s="13"/>
-      <c r="D133" s="14"/>
+      <c r="C133" s="12"/>
+      <c r="D133" s="13"/>
+      <c r="E133" s="13"/>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C134" s="13"/>
-      <c r="D134" s="14"/>
+      <c r="C134" s="12"/>
+      <c r="D134" s="13"/>
+      <c r="E134" s="13"/>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C135" s="13"/>
-      <c r="D135" s="14"/>
+      <c r="C135" s="12"/>
+      <c r="D135" s="13"/>
+      <c r="E135" s="13"/>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C136" s="13"/>
-      <c r="D136" s="14"/>
+      <c r="C136" s="12"/>
+      <c r="D136" s="13"/>
+      <c r="E136" s="13"/>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C137" s="13"/>
-      <c r="D137" s="14"/>
+      <c r="C137" s="12"/>
+      <c r="D137" s="13"/>
+      <c r="E137" s="13"/>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C138" s="13"/>
-      <c r="D138" s="14"/>
+      <c r="C138" s="12"/>
+      <c r="D138" s="13"/>
+      <c r="E138" s="13"/>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C139" s="13"/>
-      <c r="D139" s="14"/>
+      <c r="C139" s="12"/>
+      <c r="D139" s="13"/>
+      <c r="E139" s="13"/>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C140" s="13"/>
-      <c r="D140" s="14"/>
+      <c r="C140" s="12"/>
+      <c r="D140" s="13"/>
+      <c r="E140" s="13"/>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C141" s="13"/>
-      <c r="D141" s="14"/>
+      <c r="C141" s="12"/>
+      <c r="D141" s="13"/>
+      <c r="E141" s="13"/>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C142" s="13"/>
-      <c r="D142" s="14"/>
+      <c r="C142" s="12"/>
+      <c r="D142" s="13"/>
+      <c r="E142" s="13"/>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C143" s="13"/>
-      <c r="D143" s="14"/>
+      <c r="C143" s="12"/>
+      <c r="D143" s="13"/>
+      <c r="E143" s="13"/>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C144" s="13"/>
-      <c r="D144" s="14"/>
+      <c r="C144" s="12"/>
+      <c r="D144" s="13"/>
+      <c r="E144" s="13"/>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C145" s="13"/>
-      <c r="D145" s="14"/>
+      <c r="C145" s="12"/>
+      <c r="D145" s="13"/>
+      <c r="E145" s="13"/>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C146" s="13"/>
-      <c r="D146" s="14"/>
+      <c r="C146" s="12"/>
+      <c r="D146" s="13"/>
+      <c r="E146" s="13"/>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C147" s="13"/>
-      <c r="D147" s="14"/>
+      <c r="C147" s="12"/>
+      <c r="D147" s="13"/>
+      <c r="E147" s="13"/>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C148" s="13"/>
-      <c r="D148" s="14"/>
+      <c r="C148" s="12"/>
+      <c r="D148" s="13"/>
+      <c r="E148" s="13"/>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C149" s="13"/>
-      <c r="D149" s="14"/>
+      <c r="C149" s="12"/>
+      <c r="D149" s="13"/>
+      <c r="E149" s="13"/>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C150" s="13"/>
-      <c r="D150" s="14"/>
+      <c r="C150" s="12"/>
+      <c r="D150" s="13"/>
+      <c r="E150" s="13"/>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C151" s="13"/>
-      <c r="D151" s="14"/>
+      <c r="C151" s="12"/>
+      <c r="D151" s="13"/>
+      <c r="E151" s="13"/>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C152" s="13"/>
-      <c r="D152" s="14"/>
+      <c r="C152" s="12"/>
+      <c r="D152" s="13"/>
+      <c r="E152" s="13"/>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C153" s="13"/>
-      <c r="D153" s="14"/>
+      <c r="C153" s="12"/>
+      <c r="D153" s="13"/>
+      <c r="E153" s="13"/>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C154" s="13"/>
-      <c r="D154" s="14"/>
+      <c r="C154" s="12"/>
+      <c r="D154" s="13"/>
+      <c r="E154" s="13"/>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C155" s="13"/>
-      <c r="D155" s="14"/>
+      <c r="C155" s="12"/>
+      <c r="D155" s="13"/>
+      <c r="E155" s="13"/>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C156" s="13"/>
-      <c r="D156" s="14"/>
+      <c r="C156" s="12"/>
+      <c r="D156" s="13"/>
+      <c r="E156" s="13"/>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C157" s="13"/>
-      <c r="D157" s="14"/>
+      <c r="C157" s="12"/>
+      <c r="D157" s="13"/>
+      <c r="E157" s="13"/>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C158" s="13"/>
-      <c r="D158" s="14"/>
+      <c r="C158" s="12"/>
+      <c r="D158" s="13"/>
+      <c r="E158" s="13"/>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C159" s="13"/>
-      <c r="D159" s="14"/>
+      <c r="C159" s="12"/>
+      <c r="D159" s="13"/>
+      <c r="E159" s="13"/>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C160" s="13"/>
-      <c r="D160" s="14"/>
+      <c r="C160" s="12"/>
+      <c r="D160" s="13"/>
+      <c r="E160" s="13"/>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C161" s="13"/>
-      <c r="D161" s="14"/>
+      <c r="C161" s="12"/>
+      <c r="D161" s="13"/>
+      <c r="E161" s="13"/>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C162" s="13"/>
-      <c r="D162" s="14"/>
+      <c r="C162" s="12"/>
+      <c r="D162" s="13"/>
+      <c r="E162" s="13"/>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C163" s="13"/>
-      <c r="D163" s="14"/>
+      <c r="C163" s="12"/>
+      <c r="D163" s="13"/>
+      <c r="E163" s="13"/>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C164" s="13"/>
-      <c r="D164" s="14"/>
+      <c r="C164" s="12"/>
+      <c r="D164" s="13"/>
+      <c r="E164" s="13"/>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C165" s="13"/>
-      <c r="D165" s="14"/>
+      <c r="C165" s="12"/>
+      <c r="D165" s="13"/>
+      <c r="E165" s="13"/>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C166" s="13"/>
-      <c r="D166" s="14"/>
+      <c r="C166" s="12"/>
+      <c r="D166" s="13"/>
+      <c r="E166" s="13"/>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C167" s="13"/>
-      <c r="D167" s="14"/>
+      <c r="C167" s="12"/>
+      <c r="D167" s="13"/>
+      <c r="E167" s="13"/>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C168" s="13"/>
-      <c r="D168" s="14"/>
+      <c r="C168" s="12"/>
+      <c r="D168" s="13"/>
+      <c r="E168" s="13"/>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C169" s="13"/>
-      <c r="D169" s="14"/>
+      <c r="C169" s="12"/>
+      <c r="D169" s="13"/>
+      <c r="E169" s="13"/>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C170" s="13"/>
-      <c r="D170" s="14"/>
+      <c r="C170" s="12"/>
+      <c r="D170" s="13"/>
+      <c r="E170" s="13"/>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C171" s="13"/>
-      <c r="D171" s="14"/>
+      <c r="C171" s="12"/>
+      <c r="D171" s="13"/>
+      <c r="E171" s="13"/>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C172" s="13"/>
-      <c r="D172" s="14"/>
+      <c r="C172" s="12"/>
+      <c r="D172" s="13"/>
+      <c r="E172" s="13"/>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C173" s="13"/>
-      <c r="D173" s="14"/>
+      <c r="C173" s="12"/>
+      <c r="D173" s="13"/>
+      <c r="E173" s="13"/>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C174" s="13"/>
-      <c r="D174" s="14"/>
+      <c r="C174" s="12"/>
+      <c r="D174" s="13"/>
+      <c r="E174" s="13"/>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C175" s="13"/>
-      <c r="D175" s="14"/>
+      <c r="C175" s="12"/>
+      <c r="D175" s="13"/>
+      <c r="E175" s="13"/>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C176" s="13"/>
-      <c r="D176" s="14"/>
+      <c r="C176" s="12"/>
+      <c r="D176" s="13"/>
+      <c r="E176" s="13"/>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C177" s="13"/>
-      <c r="D177" s="14"/>
+      <c r="C177" s="12"/>
+      <c r="D177" s="13"/>
+      <c r="E177" s="13"/>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C178" s="13"/>
-      <c r="D178" s="14"/>
+      <c r="C178" s="12"/>
+      <c r="D178" s="13"/>
+      <c r="E178" s="13"/>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C179" s="13"/>
-      <c r="D179" s="14"/>
+      <c r="C179" s="12"/>
+      <c r="D179" s="13"/>
+      <c r="E179" s="13"/>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C180" s="13"/>
-      <c r="D180" s="14"/>
+      <c r="C180" s="12"/>
+      <c r="D180" s="13"/>
+      <c r="E180" s="13"/>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C181" s="13"/>
-      <c r="D181" s="14"/>
+      <c r="C181" s="12"/>
+      <c r="D181" s="13"/>
+      <c r="E181" s="13"/>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C182" s="13"/>
-      <c r="D182" s="14"/>
+      <c r="C182" s="12"/>
+      <c r="D182" s="13"/>
+      <c r="E182" s="13"/>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C183" s="13"/>
-      <c r="D183" s="14"/>
+      <c r="C183" s="12"/>
+      <c r="D183" s="13"/>
+      <c r="E183" s="13"/>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C184" s="13"/>
-      <c r="D184" s="14"/>
+      <c r="C184" s="12"/>
+      <c r="D184" s="13"/>
+      <c r="E184" s="13"/>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C185" s="13"/>
-      <c r="D185" s="14"/>
+      <c r="C185" s="12"/>
+      <c r="D185" s="13"/>
+      <c r="E185" s="13"/>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C186" s="13"/>
-      <c r="D186" s="14"/>
+      <c r="C186" s="12"/>
+      <c r="D186" s="13"/>
+      <c r="E186" s="13"/>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C187" s="13"/>
-      <c r="D187" s="14"/>
+      <c r="C187" s="12"/>
+      <c r="D187" s="13"/>
+      <c r="E187" s="13"/>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C188" s="13"/>
-      <c r="D188" s="14"/>
+      <c r="C188" s="12"/>
+      <c r="D188" s="13"/>
+      <c r="E188" s="13"/>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C189" s="13"/>
-      <c r="D189" s="14"/>
+      <c r="C189" s="12"/>
+      <c r="D189" s="13"/>
+      <c r="E189" s="13"/>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C190" s="13"/>
-      <c r="D190" s="14"/>
+      <c r="C190" s="12"/>
+      <c r="D190" s="13"/>
+      <c r="E190" s="13"/>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C191" s="13"/>
-      <c r="D191" s="14"/>
+      <c r="C191" s="12"/>
+      <c r="D191" s="13"/>
+      <c r="E191" s="13"/>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C192" s="13"/>
-      <c r="D192" s="14"/>
+      <c r="C192" s="12"/>
+      <c r="D192" s="13"/>
+      <c r="E192" s="13"/>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C193" s="13"/>
-      <c r="D193" s="14"/>
+      <c r="C193" s="12"/>
+      <c r="D193" s="13"/>
+      <c r="E193" s="13"/>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C194" s="13"/>
-      <c r="D194" s="14"/>
+      <c r="C194" s="12"/>
+      <c r="D194" s="13"/>
+      <c r="E194" s="13"/>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C195" s="13"/>
-      <c r="D195" s="14"/>
+      <c r="C195" s="12"/>
+      <c r="D195" s="13"/>
+      <c r="E195" s="13"/>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C196" s="13"/>
-      <c r="D196" s="14"/>
+      <c r="C196" s="12"/>
+      <c r="D196" s="13"/>
+      <c r="E196" s="13"/>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C197" s="13"/>
-      <c r="D197" s="14"/>
+      <c r="C197" s="12"/>
+      <c r="D197" s="13"/>
+      <c r="E197" s="13"/>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C198" s="13"/>
-      <c r="D198" s="14"/>
+      <c r="C198" s="12"/>
+      <c r="D198" s="13"/>
+      <c r="E198" s="13"/>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Add annex groups in clusters and use in odsodp
</commit_message>
<xml_diff>
--- a/core/import_data/resources/projects_v2/project_clusters_06_05_2025.xlsx
+++ b/core/import_data/resources/projects_v2/project_clusters_06_05_2025.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="87">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -43,6 +43,9 @@
     <t xml:space="preserve">Old name</t>
   </si>
   <si>
+    <t xml:space="preserve">Annex groups</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kigali Implementation Plan Stage 1</t>
   </si>
   <si>
@@ -56,6 +59,9 @@
   </si>
   <si>
     <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
   </si>
   <si>
     <t xml:space="preserve">Kigali Implementation Plan Stage 2</t>
@@ -95,6 +101,9 @@
   </si>
   <si>
     <t xml:space="preserve">HPMP1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C/I</t>
   </si>
   <si>
     <t xml:space="preserve">HCFC phase-out management plan stage 2</t>
@@ -176,6 +185,9 @@
   </si>
   <si>
     <t xml:space="preserve">DISP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C/I,F</t>
   </si>
   <si>
     <t xml:space="preserve">CFC Individual</t>
@@ -279,7 +291,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -340,6 +352,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="0"/>
@@ -357,23 +375,11 @@
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -467,11 +473,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -483,27 +493,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -519,7 +525,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -775,8 +781,8 @@
   </sheetPr>
   <dimension ref="A1:WU1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -784,10 +790,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="49.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="25.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="21.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.8"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.04"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -812,7 +818,9 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6"/>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -834,250 +842,286 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>11</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
+      <c r="H3" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
+      <c r="H4" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
+      <c r="H5" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
+      <c r="H6" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
+      <c r="H7" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
+      <c r="H8" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
+      <c r="H9" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
+      <c r="H10" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
+      <c r="H11" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
+      <c r="H13" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
+      <c r="H14" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1641,22 +1685,25 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
+      <c r="H15" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -2220,22 +2267,25 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
+      <c r="H16" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -2799,22 +2849,25 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
+      <c r="H17" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -3429,25 +3482,25 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -4063,22 +4116,25 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
+      <c r="H19" s="9" t="s">
+        <v>55</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -4693,20 +4749,20 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G20" s="3"/>
       <c r="I20" s="1"/>
@@ -4727,616 +4783,616 @@
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
-      <c r="AA20" s="9"/>
-      <c r="AB20" s="9"/>
-      <c r="AC20" s="9"/>
-      <c r="AD20" s="9"/>
-      <c r="AE20" s="9"/>
-      <c r="AF20" s="9"/>
-      <c r="AG20" s="9"/>
-      <c r="AH20" s="9"/>
-      <c r="AI20" s="9"/>
-      <c r="AJ20" s="9"/>
-      <c r="AK20" s="9"/>
-      <c r="AL20" s="9"/>
-      <c r="AM20" s="9"/>
-      <c r="AN20" s="9"/>
-      <c r="AO20" s="9"/>
-      <c r="AP20" s="9"/>
-      <c r="AQ20" s="9"/>
-      <c r="AR20" s="9"/>
-      <c r="AS20" s="9"/>
-      <c r="AT20" s="9"/>
-      <c r="AU20" s="9"/>
-      <c r="AV20" s="9"/>
-      <c r="AW20" s="9"/>
-      <c r="AX20" s="9"/>
-      <c r="AY20" s="9"/>
-      <c r="AZ20" s="9"/>
-      <c r="BA20" s="9"/>
-      <c r="BB20" s="9"/>
-      <c r="BC20" s="9"/>
-      <c r="BD20" s="9"/>
-      <c r="BE20" s="9"/>
-      <c r="BF20" s="9"/>
-      <c r="BG20" s="9"/>
-      <c r="BH20" s="9"/>
-      <c r="BI20" s="9"/>
-      <c r="BJ20" s="9"/>
-      <c r="BK20" s="9"/>
-      <c r="BL20" s="9"/>
-      <c r="BM20" s="9"/>
-      <c r="BN20" s="9"/>
-      <c r="BO20" s="9"/>
-      <c r="BP20" s="9"/>
-      <c r="BQ20" s="9"/>
-      <c r="BR20" s="9"/>
-      <c r="BS20" s="9"/>
-      <c r="BT20" s="9"/>
-      <c r="BU20" s="9"/>
-      <c r="BV20" s="9"/>
-      <c r="BW20" s="9"/>
-      <c r="BX20" s="9"/>
-      <c r="BY20" s="9"/>
-      <c r="BZ20" s="9"/>
-      <c r="CA20" s="9"/>
-      <c r="CB20" s="9"/>
-      <c r="CC20" s="9"/>
-      <c r="CD20" s="9"/>
-      <c r="CE20" s="9"/>
-      <c r="CF20" s="9"/>
-      <c r="CG20" s="9"/>
-      <c r="CH20" s="9"/>
-      <c r="CI20" s="9"/>
-      <c r="CJ20" s="9"/>
-      <c r="CK20" s="9"/>
-      <c r="CL20" s="9"/>
-      <c r="CM20" s="9"/>
-      <c r="CN20" s="9"/>
-      <c r="CO20" s="9"/>
-      <c r="CP20" s="9"/>
-      <c r="CQ20" s="9"/>
-      <c r="CR20" s="9"/>
-      <c r="CS20" s="9"/>
-      <c r="CT20" s="9"/>
-      <c r="CU20" s="9"/>
-      <c r="CV20" s="9"/>
-      <c r="CW20" s="9"/>
-      <c r="CX20" s="9"/>
-      <c r="CY20" s="9"/>
-      <c r="CZ20" s="9"/>
-      <c r="DA20" s="9"/>
-      <c r="DB20" s="9"/>
-      <c r="DC20" s="9"/>
-      <c r="DD20" s="9"/>
-      <c r="DE20" s="9"/>
-      <c r="DF20" s="9"/>
-      <c r="DG20" s="9"/>
-      <c r="DH20" s="9"/>
-      <c r="DI20" s="9"/>
-      <c r="DJ20" s="9"/>
-      <c r="DK20" s="9"/>
-      <c r="DL20" s="9"/>
-      <c r="DM20" s="9"/>
-      <c r="DN20" s="9"/>
-      <c r="DO20" s="9"/>
-      <c r="DP20" s="9"/>
-      <c r="DQ20" s="9"/>
-      <c r="DR20" s="9"/>
-      <c r="DS20" s="9"/>
-      <c r="DT20" s="9"/>
-      <c r="DU20" s="9"/>
-      <c r="DV20" s="9"/>
-      <c r="DW20" s="9"/>
-      <c r="DX20" s="9"/>
-      <c r="DY20" s="9"/>
-      <c r="DZ20" s="9"/>
-      <c r="EA20" s="9"/>
-      <c r="EB20" s="9"/>
-      <c r="EC20" s="9"/>
-      <c r="ED20" s="9"/>
-      <c r="EE20" s="9"/>
-      <c r="EF20" s="9"/>
-      <c r="EG20" s="9"/>
-      <c r="EH20" s="9"/>
-      <c r="EI20" s="9"/>
-      <c r="EJ20" s="9"/>
-      <c r="EK20" s="9"/>
-      <c r="EL20" s="9"/>
-      <c r="EM20" s="9"/>
-      <c r="EN20" s="9"/>
-      <c r="EO20" s="9"/>
-      <c r="EP20" s="9"/>
-      <c r="EQ20" s="9"/>
-      <c r="ER20" s="9"/>
-      <c r="ES20" s="9"/>
-      <c r="ET20" s="9"/>
-      <c r="EU20" s="9"/>
-      <c r="EV20" s="9"/>
-      <c r="EW20" s="9"/>
-      <c r="EX20" s="9"/>
-      <c r="EY20" s="9"/>
-      <c r="EZ20" s="9"/>
-      <c r="FA20" s="9"/>
-      <c r="FB20" s="9"/>
-      <c r="FC20" s="9"/>
-      <c r="FD20" s="9"/>
-      <c r="FE20" s="9"/>
-      <c r="FF20" s="9"/>
-      <c r="FG20" s="9"/>
-      <c r="FH20" s="9"/>
-      <c r="FI20" s="9"/>
-      <c r="FJ20" s="9"/>
-      <c r="FK20" s="9"/>
-      <c r="FL20" s="9"/>
-      <c r="FM20" s="9"/>
-      <c r="FN20" s="9"/>
-      <c r="FO20" s="9"/>
-      <c r="FP20" s="9"/>
-      <c r="FQ20" s="9"/>
-      <c r="FR20" s="9"/>
-      <c r="FS20" s="9"/>
-      <c r="FT20" s="9"/>
-      <c r="FU20" s="9"/>
-      <c r="FV20" s="9"/>
-      <c r="FW20" s="9"/>
-      <c r="FX20" s="9"/>
-      <c r="FY20" s="9"/>
-      <c r="FZ20" s="9"/>
-      <c r="GA20" s="9"/>
-      <c r="GB20" s="9"/>
-      <c r="GC20" s="9"/>
-      <c r="GD20" s="9"/>
-      <c r="GE20" s="9"/>
-      <c r="GF20" s="9"/>
-      <c r="GG20" s="9"/>
-      <c r="GH20" s="9"/>
-      <c r="GI20" s="9"/>
-      <c r="GJ20" s="9"/>
-      <c r="GK20" s="9"/>
-      <c r="GL20" s="9"/>
-      <c r="GM20" s="9"/>
-      <c r="GN20" s="9"/>
-      <c r="GO20" s="9"/>
-      <c r="GP20" s="9"/>
-      <c r="GQ20" s="9"/>
-      <c r="GR20" s="9"/>
-      <c r="GS20" s="9"/>
-      <c r="GT20" s="9"/>
-      <c r="GU20" s="9"/>
-      <c r="GV20" s="9"/>
-      <c r="GW20" s="9"/>
-      <c r="GX20" s="9"/>
-      <c r="GY20" s="9"/>
-      <c r="GZ20" s="9"/>
-      <c r="HA20" s="9"/>
-      <c r="HB20" s="9"/>
-      <c r="HC20" s="9"/>
-      <c r="HD20" s="9"/>
-      <c r="HE20" s="9"/>
-      <c r="HF20" s="9"/>
-      <c r="HG20" s="9"/>
-      <c r="HH20" s="9"/>
-      <c r="HI20" s="9"/>
-      <c r="HJ20" s="9"/>
-      <c r="HK20" s="9"/>
-      <c r="HL20" s="9"/>
-      <c r="HM20" s="9"/>
-      <c r="HN20" s="9"/>
-      <c r="HO20" s="9"/>
-      <c r="HP20" s="9"/>
-      <c r="HQ20" s="9"/>
-      <c r="HR20" s="9"/>
-      <c r="HS20" s="9"/>
-      <c r="HT20" s="9"/>
-      <c r="HU20" s="9"/>
-      <c r="HV20" s="9"/>
-      <c r="HW20" s="9"/>
-      <c r="HX20" s="9"/>
-      <c r="HY20" s="9"/>
-      <c r="HZ20" s="9"/>
-      <c r="IA20" s="9"/>
-      <c r="IB20" s="9"/>
-      <c r="IC20" s="9"/>
-      <c r="ID20" s="9"/>
-      <c r="IE20" s="9"/>
-      <c r="IF20" s="9"/>
-      <c r="IG20" s="9"/>
-      <c r="IH20" s="9"/>
-      <c r="II20" s="9"/>
-      <c r="IJ20" s="9"/>
-      <c r="IK20" s="9"/>
-      <c r="IL20" s="9"/>
-      <c r="IM20" s="9"/>
-      <c r="IN20" s="9"/>
-      <c r="IO20" s="9"/>
-      <c r="IP20" s="9"/>
-      <c r="IQ20" s="9"/>
-      <c r="IR20" s="9"/>
-      <c r="IS20" s="9"/>
-      <c r="IT20" s="9"/>
-      <c r="IU20" s="9"/>
-      <c r="IV20" s="9"/>
-      <c r="IW20" s="9"/>
-      <c r="IX20" s="9"/>
-      <c r="IY20" s="9"/>
-      <c r="IZ20" s="9"/>
-      <c r="JA20" s="9"/>
-      <c r="JB20" s="9"/>
-      <c r="JC20" s="9"/>
-      <c r="JD20" s="9"/>
-      <c r="JE20" s="9"/>
-      <c r="JF20" s="9"/>
-      <c r="JG20" s="9"/>
-      <c r="JH20" s="9"/>
-      <c r="JI20" s="9"/>
-      <c r="JJ20" s="9"/>
-      <c r="JK20" s="9"/>
-      <c r="JL20" s="9"/>
-      <c r="JM20" s="9"/>
-      <c r="JN20" s="9"/>
-      <c r="JO20" s="9"/>
-      <c r="JP20" s="9"/>
-      <c r="JQ20" s="9"/>
-      <c r="JR20" s="9"/>
-      <c r="JS20" s="9"/>
-      <c r="JT20" s="9"/>
-      <c r="JU20" s="9"/>
-      <c r="JV20" s="9"/>
-      <c r="JW20" s="9"/>
-      <c r="JX20" s="9"/>
-      <c r="JY20" s="9"/>
-      <c r="JZ20" s="9"/>
-      <c r="KA20" s="9"/>
-      <c r="KB20" s="9"/>
-      <c r="KC20" s="9"/>
-      <c r="KD20" s="9"/>
-      <c r="KE20" s="9"/>
-      <c r="KF20" s="9"/>
-      <c r="KG20" s="9"/>
-      <c r="KH20" s="9"/>
-      <c r="KI20" s="9"/>
-      <c r="KJ20" s="9"/>
-      <c r="KK20" s="9"/>
-      <c r="KL20" s="9"/>
-      <c r="KM20" s="9"/>
-      <c r="KN20" s="9"/>
-      <c r="KO20" s="9"/>
-      <c r="KP20" s="9"/>
-      <c r="KQ20" s="9"/>
-      <c r="KR20" s="9"/>
-      <c r="KS20" s="9"/>
-      <c r="KT20" s="9"/>
-      <c r="KU20" s="9"/>
-      <c r="KV20" s="9"/>
-      <c r="KW20" s="9"/>
-      <c r="KX20" s="9"/>
-      <c r="KY20" s="9"/>
-      <c r="KZ20" s="9"/>
-      <c r="LA20" s="9"/>
-      <c r="LB20" s="9"/>
-      <c r="LC20" s="9"/>
-      <c r="LD20" s="9"/>
-      <c r="LE20" s="9"/>
-      <c r="LF20" s="9"/>
-      <c r="LG20" s="9"/>
-      <c r="LH20" s="9"/>
-      <c r="LI20" s="9"/>
-      <c r="LJ20" s="9"/>
-      <c r="LK20" s="9"/>
-      <c r="LL20" s="9"/>
-      <c r="LM20" s="9"/>
-      <c r="LN20" s="9"/>
-      <c r="LO20" s="9"/>
-      <c r="LP20" s="9"/>
-      <c r="LQ20" s="9"/>
-      <c r="LR20" s="9"/>
-      <c r="LS20" s="9"/>
-      <c r="LT20" s="9"/>
-      <c r="LU20" s="9"/>
-      <c r="LV20" s="9"/>
-      <c r="LW20" s="9"/>
-      <c r="LX20" s="9"/>
-      <c r="LY20" s="9"/>
-      <c r="LZ20" s="9"/>
-      <c r="MA20" s="9"/>
-      <c r="MB20" s="9"/>
-      <c r="MC20" s="9"/>
-      <c r="MD20" s="9"/>
-      <c r="ME20" s="9"/>
-      <c r="MF20" s="9"/>
-      <c r="MG20" s="9"/>
-      <c r="MH20" s="9"/>
-      <c r="MI20" s="9"/>
-      <c r="MJ20" s="9"/>
-      <c r="MK20" s="9"/>
-      <c r="ML20" s="9"/>
-      <c r="MM20" s="9"/>
-      <c r="MN20" s="9"/>
-      <c r="MO20" s="9"/>
-      <c r="MP20" s="9"/>
-      <c r="MQ20" s="9"/>
-      <c r="MR20" s="9"/>
-      <c r="MS20" s="9"/>
-      <c r="MT20" s="9"/>
-      <c r="MU20" s="9"/>
-      <c r="MV20" s="9"/>
-      <c r="MW20" s="9"/>
-      <c r="MX20" s="9"/>
-      <c r="MY20" s="9"/>
-      <c r="MZ20" s="9"/>
-      <c r="NA20" s="9"/>
-      <c r="NB20" s="9"/>
-      <c r="NC20" s="9"/>
-      <c r="ND20" s="9"/>
-      <c r="NE20" s="9"/>
-      <c r="NF20" s="9"/>
-      <c r="NG20" s="9"/>
-      <c r="NH20" s="9"/>
-      <c r="NI20" s="9"/>
-      <c r="NJ20" s="9"/>
-      <c r="NK20" s="9"/>
-      <c r="NL20" s="9"/>
-      <c r="NM20" s="9"/>
-      <c r="NN20" s="9"/>
-      <c r="NO20" s="9"/>
-      <c r="NP20" s="9"/>
-      <c r="NQ20" s="9"/>
-      <c r="NR20" s="9"/>
-      <c r="NS20" s="9"/>
-      <c r="NT20" s="9"/>
-      <c r="NU20" s="9"/>
-      <c r="NV20" s="9"/>
-      <c r="NW20" s="9"/>
-      <c r="NX20" s="9"/>
-      <c r="NY20" s="9"/>
-      <c r="NZ20" s="9"/>
-      <c r="OA20" s="9"/>
-      <c r="OB20" s="9"/>
-      <c r="OC20" s="9"/>
-      <c r="OD20" s="9"/>
-      <c r="OE20" s="9"/>
-      <c r="OF20" s="9"/>
-      <c r="OG20" s="9"/>
-      <c r="OH20" s="9"/>
-      <c r="OI20" s="9"/>
-      <c r="OJ20" s="9"/>
-      <c r="OK20" s="9"/>
-      <c r="OL20" s="9"/>
-      <c r="OM20" s="9"/>
-      <c r="ON20" s="9"/>
-      <c r="OO20" s="9"/>
-      <c r="OP20" s="9"/>
-      <c r="OQ20" s="9"/>
-      <c r="OR20" s="9"/>
-      <c r="OS20" s="9"/>
-      <c r="OT20" s="9"/>
-      <c r="OU20" s="9"/>
-      <c r="OV20" s="9"/>
-      <c r="OW20" s="9"/>
-      <c r="OX20" s="9"/>
-      <c r="OY20" s="9"/>
-      <c r="OZ20" s="9"/>
-      <c r="PA20" s="9"/>
-      <c r="PB20" s="9"/>
-      <c r="PC20" s="9"/>
-      <c r="PD20" s="9"/>
-      <c r="PE20" s="9"/>
-      <c r="PF20" s="9"/>
-      <c r="PG20" s="9"/>
-      <c r="PH20" s="9"/>
-      <c r="PI20" s="9"/>
-      <c r="PJ20" s="9"/>
-      <c r="PK20" s="9"/>
-      <c r="PL20" s="9"/>
-      <c r="PM20" s="9"/>
-      <c r="PN20" s="9"/>
-      <c r="PO20" s="9"/>
-      <c r="PP20" s="9"/>
-      <c r="PQ20" s="9"/>
-      <c r="PR20" s="9"/>
-      <c r="PS20" s="9"/>
-      <c r="PT20" s="9"/>
-      <c r="PU20" s="9"/>
-      <c r="PV20" s="9"/>
-      <c r="PW20" s="9"/>
-      <c r="PX20" s="9"/>
-      <c r="PY20" s="9"/>
-      <c r="PZ20" s="9"/>
-      <c r="QA20" s="9"/>
-      <c r="QB20" s="9"/>
-      <c r="QC20" s="9"/>
-      <c r="QD20" s="9"/>
-      <c r="QE20" s="9"/>
-      <c r="QF20" s="9"/>
-      <c r="QG20" s="9"/>
-      <c r="QH20" s="9"/>
-      <c r="QI20" s="9"/>
-      <c r="QJ20" s="9"/>
-      <c r="QK20" s="9"/>
-      <c r="QL20" s="9"/>
-      <c r="QM20" s="9"/>
-      <c r="QN20" s="9"/>
-      <c r="QO20" s="9"/>
-      <c r="QP20" s="9"/>
-      <c r="QQ20" s="9"/>
-      <c r="QR20" s="9"/>
-      <c r="QS20" s="9"/>
-      <c r="QT20" s="9"/>
-      <c r="QU20" s="9"/>
-      <c r="QV20" s="9"/>
-      <c r="QW20" s="9"/>
-      <c r="QX20" s="9"/>
-      <c r="QY20" s="9"/>
-      <c r="QZ20" s="9"/>
-      <c r="RA20" s="9"/>
-      <c r="RB20" s="9"/>
-      <c r="RC20" s="9"/>
-      <c r="RD20" s="9"/>
-      <c r="RE20" s="9"/>
-      <c r="RF20" s="9"/>
-      <c r="RG20" s="9"/>
-      <c r="RH20" s="9"/>
-      <c r="RI20" s="9"/>
-      <c r="RJ20" s="9"/>
-      <c r="RK20" s="9"/>
-      <c r="RL20" s="9"/>
-      <c r="RM20" s="9"/>
-      <c r="RN20" s="9"/>
-      <c r="RO20" s="9"/>
-      <c r="RP20" s="9"/>
-      <c r="RQ20" s="9"/>
-      <c r="RR20" s="9"/>
-      <c r="RS20" s="9"/>
-      <c r="RT20" s="9"/>
-      <c r="RU20" s="9"/>
-      <c r="RV20" s="9"/>
-      <c r="RW20" s="9"/>
-      <c r="RX20" s="9"/>
-      <c r="RY20" s="9"/>
-      <c r="RZ20" s="9"/>
-      <c r="SA20" s="9"/>
-      <c r="SB20" s="9"/>
-      <c r="SC20" s="9"/>
-      <c r="SD20" s="9"/>
-      <c r="SE20" s="9"/>
-      <c r="SF20" s="9"/>
-      <c r="SG20" s="9"/>
-      <c r="SH20" s="9"/>
-      <c r="SI20" s="9"/>
-      <c r="SJ20" s="9"/>
-      <c r="SK20" s="9"/>
-      <c r="SL20" s="9"/>
-      <c r="SM20" s="9"/>
-      <c r="SN20" s="9"/>
-      <c r="SO20" s="9"/>
-      <c r="SP20" s="9"/>
-      <c r="SQ20" s="9"/>
-      <c r="SR20" s="9"/>
-      <c r="SS20" s="9"/>
-      <c r="ST20" s="9"/>
-      <c r="SU20" s="9"/>
-      <c r="SV20" s="9"/>
-      <c r="SW20" s="9"/>
-      <c r="SX20" s="9"/>
-      <c r="SY20" s="9"/>
-      <c r="SZ20" s="9"/>
-      <c r="TA20" s="9"/>
-      <c r="TB20" s="9"/>
-      <c r="TC20" s="9"/>
-      <c r="TD20" s="9"/>
-      <c r="TE20" s="9"/>
-      <c r="TF20" s="9"/>
-      <c r="TG20" s="9"/>
-      <c r="TH20" s="9"/>
-      <c r="TI20" s="9"/>
-      <c r="TJ20" s="9"/>
-      <c r="TK20" s="9"/>
-      <c r="TL20" s="9"/>
-      <c r="TM20" s="9"/>
-      <c r="TN20" s="9"/>
-      <c r="TO20" s="9"/>
-      <c r="TP20" s="9"/>
-      <c r="TQ20" s="9"/>
-      <c r="TR20" s="9"/>
-      <c r="TS20" s="9"/>
-      <c r="TT20" s="9"/>
-      <c r="TU20" s="9"/>
-      <c r="TV20" s="9"/>
-      <c r="TW20" s="9"/>
-      <c r="TX20" s="9"/>
-      <c r="TY20" s="9"/>
-      <c r="TZ20" s="9"/>
-      <c r="UA20" s="9"/>
-      <c r="UB20" s="9"/>
-      <c r="UC20" s="9"/>
-      <c r="UD20" s="9"/>
-      <c r="UE20" s="9"/>
-      <c r="UF20" s="9"/>
-      <c r="UG20" s="9"/>
-      <c r="UH20" s="9"/>
-      <c r="UI20" s="9"/>
-      <c r="UJ20" s="9"/>
-      <c r="UK20" s="9"/>
-      <c r="UL20" s="9"/>
-      <c r="UM20" s="9"/>
-      <c r="UN20" s="9"/>
-      <c r="UO20" s="9"/>
-      <c r="UP20" s="9"/>
-      <c r="UQ20" s="9"/>
-      <c r="UR20" s="9"/>
-      <c r="US20" s="9"/>
-      <c r="UT20" s="9"/>
-      <c r="UU20" s="9"/>
-      <c r="UV20" s="9"/>
-      <c r="UW20" s="9"/>
-      <c r="UX20" s="9"/>
-      <c r="UY20" s="9"/>
-      <c r="UZ20" s="9"/>
-      <c r="VA20" s="9"/>
-      <c r="VB20" s="9"/>
-      <c r="VC20" s="9"/>
-      <c r="VD20" s="9"/>
-      <c r="VE20" s="9"/>
-      <c r="VF20" s="9"/>
-      <c r="VG20" s="9"/>
-      <c r="VH20" s="9"/>
-      <c r="VI20" s="9"/>
-      <c r="VJ20" s="9"/>
-      <c r="VK20" s="9"/>
-      <c r="VL20" s="9"/>
-      <c r="VM20" s="9"/>
-      <c r="VN20" s="9"/>
-      <c r="VO20" s="9"/>
-      <c r="VP20" s="9"/>
-      <c r="VQ20" s="9"/>
-      <c r="VR20" s="9"/>
-      <c r="VS20" s="9"/>
-      <c r="VT20" s="9"/>
-      <c r="VU20" s="9"/>
-      <c r="VV20" s="9"/>
-      <c r="VW20" s="9"/>
-      <c r="VX20" s="9"/>
-      <c r="VY20" s="9"/>
-      <c r="VZ20" s="9"/>
-      <c r="WA20" s="9"/>
-      <c r="WB20" s="9"/>
-      <c r="WC20" s="9"/>
-      <c r="WD20" s="9"/>
-      <c r="WE20" s="9"/>
-      <c r="WF20" s="9"/>
-      <c r="WG20" s="9"/>
-      <c r="WH20" s="9"/>
-      <c r="WI20" s="9"/>
-      <c r="WJ20" s="9"/>
-      <c r="WK20" s="9"/>
-      <c r="WL20" s="9"/>
-      <c r="WM20" s="9"/>
-      <c r="WN20" s="9"/>
-      <c r="WO20" s="9"/>
-      <c r="WP20" s="9"/>
-      <c r="WQ20" s="9"/>
-      <c r="WR20" s="9"/>
-      <c r="WS20" s="9"/>
-      <c r="WT20" s="9"/>
-      <c r="WU20" s="9"/>
+      <c r="AA20" s="10"/>
+      <c r="AB20" s="10"/>
+      <c r="AC20" s="10"/>
+      <c r="AD20" s="10"/>
+      <c r="AE20" s="10"/>
+      <c r="AF20" s="10"/>
+      <c r="AG20" s="10"/>
+      <c r="AH20" s="10"/>
+      <c r="AI20" s="10"/>
+      <c r="AJ20" s="10"/>
+      <c r="AK20" s="10"/>
+      <c r="AL20" s="10"/>
+      <c r="AM20" s="10"/>
+      <c r="AN20" s="10"/>
+      <c r="AO20" s="10"/>
+      <c r="AP20" s="10"/>
+      <c r="AQ20" s="10"/>
+      <c r="AR20" s="10"/>
+      <c r="AS20" s="10"/>
+      <c r="AT20" s="10"/>
+      <c r="AU20" s="10"/>
+      <c r="AV20" s="10"/>
+      <c r="AW20" s="10"/>
+      <c r="AX20" s="10"/>
+      <c r="AY20" s="10"/>
+      <c r="AZ20" s="10"/>
+      <c r="BA20" s="10"/>
+      <c r="BB20" s="10"/>
+      <c r="BC20" s="10"/>
+      <c r="BD20" s="10"/>
+      <c r="BE20" s="10"/>
+      <c r="BF20" s="10"/>
+      <c r="BG20" s="10"/>
+      <c r="BH20" s="10"/>
+      <c r="BI20" s="10"/>
+      <c r="BJ20" s="10"/>
+      <c r="BK20" s="10"/>
+      <c r="BL20" s="10"/>
+      <c r="BM20" s="10"/>
+      <c r="BN20" s="10"/>
+      <c r="BO20" s="10"/>
+      <c r="BP20" s="10"/>
+      <c r="BQ20" s="10"/>
+      <c r="BR20" s="10"/>
+      <c r="BS20" s="10"/>
+      <c r="BT20" s="10"/>
+      <c r="BU20" s="10"/>
+      <c r="BV20" s="10"/>
+      <c r="BW20" s="10"/>
+      <c r="BX20" s="10"/>
+      <c r="BY20" s="10"/>
+      <c r="BZ20" s="10"/>
+      <c r="CA20" s="10"/>
+      <c r="CB20" s="10"/>
+      <c r="CC20" s="10"/>
+      <c r="CD20" s="10"/>
+      <c r="CE20" s="10"/>
+      <c r="CF20" s="10"/>
+      <c r="CG20" s="10"/>
+      <c r="CH20" s="10"/>
+      <c r="CI20" s="10"/>
+      <c r="CJ20" s="10"/>
+      <c r="CK20" s="10"/>
+      <c r="CL20" s="10"/>
+      <c r="CM20" s="10"/>
+      <c r="CN20" s="10"/>
+      <c r="CO20" s="10"/>
+      <c r="CP20" s="10"/>
+      <c r="CQ20" s="10"/>
+      <c r="CR20" s="10"/>
+      <c r="CS20" s="10"/>
+      <c r="CT20" s="10"/>
+      <c r="CU20" s="10"/>
+      <c r="CV20" s="10"/>
+      <c r="CW20" s="10"/>
+      <c r="CX20" s="10"/>
+      <c r="CY20" s="10"/>
+      <c r="CZ20" s="10"/>
+      <c r="DA20" s="10"/>
+      <c r="DB20" s="10"/>
+      <c r="DC20" s="10"/>
+      <c r="DD20" s="10"/>
+      <c r="DE20" s="10"/>
+      <c r="DF20" s="10"/>
+      <c r="DG20" s="10"/>
+      <c r="DH20" s="10"/>
+      <c r="DI20" s="10"/>
+      <c r="DJ20" s="10"/>
+      <c r="DK20" s="10"/>
+      <c r="DL20" s="10"/>
+      <c r="DM20" s="10"/>
+      <c r="DN20" s="10"/>
+      <c r="DO20" s="10"/>
+      <c r="DP20" s="10"/>
+      <c r="DQ20" s="10"/>
+      <c r="DR20" s="10"/>
+      <c r="DS20" s="10"/>
+      <c r="DT20" s="10"/>
+      <c r="DU20" s="10"/>
+      <c r="DV20" s="10"/>
+      <c r="DW20" s="10"/>
+      <c r="DX20" s="10"/>
+      <c r="DY20" s="10"/>
+      <c r="DZ20" s="10"/>
+      <c r="EA20" s="10"/>
+      <c r="EB20" s="10"/>
+      <c r="EC20" s="10"/>
+      <c r="ED20" s="10"/>
+      <c r="EE20" s="10"/>
+      <c r="EF20" s="10"/>
+      <c r="EG20" s="10"/>
+      <c r="EH20" s="10"/>
+      <c r="EI20" s="10"/>
+      <c r="EJ20" s="10"/>
+      <c r="EK20" s="10"/>
+      <c r="EL20" s="10"/>
+      <c r="EM20" s="10"/>
+      <c r="EN20" s="10"/>
+      <c r="EO20" s="10"/>
+      <c r="EP20" s="10"/>
+      <c r="EQ20" s="10"/>
+      <c r="ER20" s="10"/>
+      <c r="ES20" s="10"/>
+      <c r="ET20" s="10"/>
+      <c r="EU20" s="10"/>
+      <c r="EV20" s="10"/>
+      <c r="EW20" s="10"/>
+      <c r="EX20" s="10"/>
+      <c r="EY20" s="10"/>
+      <c r="EZ20" s="10"/>
+      <c r="FA20" s="10"/>
+      <c r="FB20" s="10"/>
+      <c r="FC20" s="10"/>
+      <c r="FD20" s="10"/>
+      <c r="FE20" s="10"/>
+      <c r="FF20" s="10"/>
+      <c r="FG20" s="10"/>
+      <c r="FH20" s="10"/>
+      <c r="FI20" s="10"/>
+      <c r="FJ20" s="10"/>
+      <c r="FK20" s="10"/>
+      <c r="FL20" s="10"/>
+      <c r="FM20" s="10"/>
+      <c r="FN20" s="10"/>
+      <c r="FO20" s="10"/>
+      <c r="FP20" s="10"/>
+      <c r="FQ20" s="10"/>
+      <c r="FR20" s="10"/>
+      <c r="FS20" s="10"/>
+      <c r="FT20" s="10"/>
+      <c r="FU20" s="10"/>
+      <c r="FV20" s="10"/>
+      <c r="FW20" s="10"/>
+      <c r="FX20" s="10"/>
+      <c r="FY20" s="10"/>
+      <c r="FZ20" s="10"/>
+      <c r="GA20" s="10"/>
+      <c r="GB20" s="10"/>
+      <c r="GC20" s="10"/>
+      <c r="GD20" s="10"/>
+      <c r="GE20" s="10"/>
+      <c r="GF20" s="10"/>
+      <c r="GG20" s="10"/>
+      <c r="GH20" s="10"/>
+      <c r="GI20" s="10"/>
+      <c r="GJ20" s="10"/>
+      <c r="GK20" s="10"/>
+      <c r="GL20" s="10"/>
+      <c r="GM20" s="10"/>
+      <c r="GN20" s="10"/>
+      <c r="GO20" s="10"/>
+      <c r="GP20" s="10"/>
+      <c r="GQ20" s="10"/>
+      <c r="GR20" s="10"/>
+      <c r="GS20" s="10"/>
+      <c r="GT20" s="10"/>
+      <c r="GU20" s="10"/>
+      <c r="GV20" s="10"/>
+      <c r="GW20" s="10"/>
+      <c r="GX20" s="10"/>
+      <c r="GY20" s="10"/>
+      <c r="GZ20" s="10"/>
+      <c r="HA20" s="10"/>
+      <c r="HB20" s="10"/>
+      <c r="HC20" s="10"/>
+      <c r="HD20" s="10"/>
+      <c r="HE20" s="10"/>
+      <c r="HF20" s="10"/>
+      <c r="HG20" s="10"/>
+      <c r="HH20" s="10"/>
+      <c r="HI20" s="10"/>
+      <c r="HJ20" s="10"/>
+      <c r="HK20" s="10"/>
+      <c r="HL20" s="10"/>
+      <c r="HM20" s="10"/>
+      <c r="HN20" s="10"/>
+      <c r="HO20" s="10"/>
+      <c r="HP20" s="10"/>
+      <c r="HQ20" s="10"/>
+      <c r="HR20" s="10"/>
+      <c r="HS20" s="10"/>
+      <c r="HT20" s="10"/>
+      <c r="HU20" s="10"/>
+      <c r="HV20" s="10"/>
+      <c r="HW20" s="10"/>
+      <c r="HX20" s="10"/>
+      <c r="HY20" s="10"/>
+      <c r="HZ20" s="10"/>
+      <c r="IA20" s="10"/>
+      <c r="IB20" s="10"/>
+      <c r="IC20" s="10"/>
+      <c r="ID20" s="10"/>
+      <c r="IE20" s="10"/>
+      <c r="IF20" s="10"/>
+      <c r="IG20" s="10"/>
+      <c r="IH20" s="10"/>
+      <c r="II20" s="10"/>
+      <c r="IJ20" s="10"/>
+      <c r="IK20" s="10"/>
+      <c r="IL20" s="10"/>
+      <c r="IM20" s="10"/>
+      <c r="IN20" s="10"/>
+      <c r="IO20" s="10"/>
+      <c r="IP20" s="10"/>
+      <c r="IQ20" s="10"/>
+      <c r="IR20" s="10"/>
+      <c r="IS20" s="10"/>
+      <c r="IT20" s="10"/>
+      <c r="IU20" s="10"/>
+      <c r="IV20" s="10"/>
+      <c r="IW20" s="10"/>
+      <c r="IX20" s="10"/>
+      <c r="IY20" s="10"/>
+      <c r="IZ20" s="10"/>
+      <c r="JA20" s="10"/>
+      <c r="JB20" s="10"/>
+      <c r="JC20" s="10"/>
+      <c r="JD20" s="10"/>
+      <c r="JE20" s="10"/>
+      <c r="JF20" s="10"/>
+      <c r="JG20" s="10"/>
+      <c r="JH20" s="10"/>
+      <c r="JI20" s="10"/>
+      <c r="JJ20" s="10"/>
+      <c r="JK20" s="10"/>
+      <c r="JL20" s="10"/>
+      <c r="JM20" s="10"/>
+      <c r="JN20" s="10"/>
+      <c r="JO20" s="10"/>
+      <c r="JP20" s="10"/>
+      <c r="JQ20" s="10"/>
+      <c r="JR20" s="10"/>
+      <c r="JS20" s="10"/>
+      <c r="JT20" s="10"/>
+      <c r="JU20" s="10"/>
+      <c r="JV20" s="10"/>
+      <c r="JW20" s="10"/>
+      <c r="JX20" s="10"/>
+      <c r="JY20" s="10"/>
+      <c r="JZ20" s="10"/>
+      <c r="KA20" s="10"/>
+      <c r="KB20" s="10"/>
+      <c r="KC20" s="10"/>
+      <c r="KD20" s="10"/>
+      <c r="KE20" s="10"/>
+      <c r="KF20" s="10"/>
+      <c r="KG20" s="10"/>
+      <c r="KH20" s="10"/>
+      <c r="KI20" s="10"/>
+      <c r="KJ20" s="10"/>
+      <c r="KK20" s="10"/>
+      <c r="KL20" s="10"/>
+      <c r="KM20" s="10"/>
+      <c r="KN20" s="10"/>
+      <c r="KO20" s="10"/>
+      <c r="KP20" s="10"/>
+      <c r="KQ20" s="10"/>
+      <c r="KR20" s="10"/>
+      <c r="KS20" s="10"/>
+      <c r="KT20" s="10"/>
+      <c r="KU20" s="10"/>
+      <c r="KV20" s="10"/>
+      <c r="KW20" s="10"/>
+      <c r="KX20" s="10"/>
+      <c r="KY20" s="10"/>
+      <c r="KZ20" s="10"/>
+      <c r="LA20" s="10"/>
+      <c r="LB20" s="10"/>
+      <c r="LC20" s="10"/>
+      <c r="LD20" s="10"/>
+      <c r="LE20" s="10"/>
+      <c r="LF20" s="10"/>
+      <c r="LG20" s="10"/>
+      <c r="LH20" s="10"/>
+      <c r="LI20" s="10"/>
+      <c r="LJ20" s="10"/>
+      <c r="LK20" s="10"/>
+      <c r="LL20" s="10"/>
+      <c r="LM20" s="10"/>
+      <c r="LN20" s="10"/>
+      <c r="LO20" s="10"/>
+      <c r="LP20" s="10"/>
+      <c r="LQ20" s="10"/>
+      <c r="LR20" s="10"/>
+      <c r="LS20" s="10"/>
+      <c r="LT20" s="10"/>
+      <c r="LU20" s="10"/>
+      <c r="LV20" s="10"/>
+      <c r="LW20" s="10"/>
+      <c r="LX20" s="10"/>
+      <c r="LY20" s="10"/>
+      <c r="LZ20" s="10"/>
+      <c r="MA20" s="10"/>
+      <c r="MB20" s="10"/>
+      <c r="MC20" s="10"/>
+      <c r="MD20" s="10"/>
+      <c r="ME20" s="10"/>
+      <c r="MF20" s="10"/>
+      <c r="MG20" s="10"/>
+      <c r="MH20" s="10"/>
+      <c r="MI20" s="10"/>
+      <c r="MJ20" s="10"/>
+      <c r="MK20" s="10"/>
+      <c r="ML20" s="10"/>
+      <c r="MM20" s="10"/>
+      <c r="MN20" s="10"/>
+      <c r="MO20" s="10"/>
+      <c r="MP20" s="10"/>
+      <c r="MQ20" s="10"/>
+      <c r="MR20" s="10"/>
+      <c r="MS20" s="10"/>
+      <c r="MT20" s="10"/>
+      <c r="MU20" s="10"/>
+      <c r="MV20" s="10"/>
+      <c r="MW20" s="10"/>
+      <c r="MX20" s="10"/>
+      <c r="MY20" s="10"/>
+      <c r="MZ20" s="10"/>
+      <c r="NA20" s="10"/>
+      <c r="NB20" s="10"/>
+      <c r="NC20" s="10"/>
+      <c r="ND20" s="10"/>
+      <c r="NE20" s="10"/>
+      <c r="NF20" s="10"/>
+      <c r="NG20" s="10"/>
+      <c r="NH20" s="10"/>
+      <c r="NI20" s="10"/>
+      <c r="NJ20" s="10"/>
+      <c r="NK20" s="10"/>
+      <c r="NL20" s="10"/>
+      <c r="NM20" s="10"/>
+      <c r="NN20" s="10"/>
+      <c r="NO20" s="10"/>
+      <c r="NP20" s="10"/>
+      <c r="NQ20" s="10"/>
+      <c r="NR20" s="10"/>
+      <c r="NS20" s="10"/>
+      <c r="NT20" s="10"/>
+      <c r="NU20" s="10"/>
+      <c r="NV20" s="10"/>
+      <c r="NW20" s="10"/>
+      <c r="NX20" s="10"/>
+      <c r="NY20" s="10"/>
+      <c r="NZ20" s="10"/>
+      <c r="OA20" s="10"/>
+      <c r="OB20" s="10"/>
+      <c r="OC20" s="10"/>
+      <c r="OD20" s="10"/>
+      <c r="OE20" s="10"/>
+      <c r="OF20" s="10"/>
+      <c r="OG20" s="10"/>
+      <c r="OH20" s="10"/>
+      <c r="OI20" s="10"/>
+      <c r="OJ20" s="10"/>
+      <c r="OK20" s="10"/>
+      <c r="OL20" s="10"/>
+      <c r="OM20" s="10"/>
+      <c r="ON20" s="10"/>
+      <c r="OO20" s="10"/>
+      <c r="OP20" s="10"/>
+      <c r="OQ20" s="10"/>
+      <c r="OR20" s="10"/>
+      <c r="OS20" s="10"/>
+      <c r="OT20" s="10"/>
+      <c r="OU20" s="10"/>
+      <c r="OV20" s="10"/>
+      <c r="OW20" s="10"/>
+      <c r="OX20" s="10"/>
+      <c r="OY20" s="10"/>
+      <c r="OZ20" s="10"/>
+      <c r="PA20" s="10"/>
+      <c r="PB20" s="10"/>
+      <c r="PC20" s="10"/>
+      <c r="PD20" s="10"/>
+      <c r="PE20" s="10"/>
+      <c r="PF20" s="10"/>
+      <c r="PG20" s="10"/>
+      <c r="PH20" s="10"/>
+      <c r="PI20" s="10"/>
+      <c r="PJ20" s="10"/>
+      <c r="PK20" s="10"/>
+      <c r="PL20" s="10"/>
+      <c r="PM20" s="10"/>
+      <c r="PN20" s="10"/>
+      <c r="PO20" s="10"/>
+      <c r="PP20" s="10"/>
+      <c r="PQ20" s="10"/>
+      <c r="PR20" s="10"/>
+      <c r="PS20" s="10"/>
+      <c r="PT20" s="10"/>
+      <c r="PU20" s="10"/>
+      <c r="PV20" s="10"/>
+      <c r="PW20" s="10"/>
+      <c r="PX20" s="10"/>
+      <c r="PY20" s="10"/>
+      <c r="PZ20" s="10"/>
+      <c r="QA20" s="10"/>
+      <c r="QB20" s="10"/>
+      <c r="QC20" s="10"/>
+      <c r="QD20" s="10"/>
+      <c r="QE20" s="10"/>
+      <c r="QF20" s="10"/>
+      <c r="QG20" s="10"/>
+      <c r="QH20" s="10"/>
+      <c r="QI20" s="10"/>
+      <c r="QJ20" s="10"/>
+      <c r="QK20" s="10"/>
+      <c r="QL20" s="10"/>
+      <c r="QM20" s="10"/>
+      <c r="QN20" s="10"/>
+      <c r="QO20" s="10"/>
+      <c r="QP20" s="10"/>
+      <c r="QQ20" s="10"/>
+      <c r="QR20" s="10"/>
+      <c r="QS20" s="10"/>
+      <c r="QT20" s="10"/>
+      <c r="QU20" s="10"/>
+      <c r="QV20" s="10"/>
+      <c r="QW20" s="10"/>
+      <c r="QX20" s="10"/>
+      <c r="QY20" s="10"/>
+      <c r="QZ20" s="10"/>
+      <c r="RA20" s="10"/>
+      <c r="RB20" s="10"/>
+      <c r="RC20" s="10"/>
+      <c r="RD20" s="10"/>
+      <c r="RE20" s="10"/>
+      <c r="RF20" s="10"/>
+      <c r="RG20" s="10"/>
+      <c r="RH20" s="10"/>
+      <c r="RI20" s="10"/>
+      <c r="RJ20" s="10"/>
+      <c r="RK20" s="10"/>
+      <c r="RL20" s="10"/>
+      <c r="RM20" s="10"/>
+      <c r="RN20" s="10"/>
+      <c r="RO20" s="10"/>
+      <c r="RP20" s="10"/>
+      <c r="RQ20" s="10"/>
+      <c r="RR20" s="10"/>
+      <c r="RS20" s="10"/>
+      <c r="RT20" s="10"/>
+      <c r="RU20" s="10"/>
+      <c r="RV20" s="10"/>
+      <c r="RW20" s="10"/>
+      <c r="RX20" s="10"/>
+      <c r="RY20" s="10"/>
+      <c r="RZ20" s="10"/>
+      <c r="SA20" s="10"/>
+      <c r="SB20" s="10"/>
+      <c r="SC20" s="10"/>
+      <c r="SD20" s="10"/>
+      <c r="SE20" s="10"/>
+      <c r="SF20" s="10"/>
+      <c r="SG20" s="10"/>
+      <c r="SH20" s="10"/>
+      <c r="SI20" s="10"/>
+      <c r="SJ20" s="10"/>
+      <c r="SK20" s="10"/>
+      <c r="SL20" s="10"/>
+      <c r="SM20" s="10"/>
+      <c r="SN20" s="10"/>
+      <c r="SO20" s="10"/>
+      <c r="SP20" s="10"/>
+      <c r="SQ20" s="10"/>
+      <c r="SR20" s="10"/>
+      <c r="SS20" s="10"/>
+      <c r="ST20" s="10"/>
+      <c r="SU20" s="10"/>
+      <c r="SV20" s="10"/>
+      <c r="SW20" s="10"/>
+      <c r="SX20" s="10"/>
+      <c r="SY20" s="10"/>
+      <c r="SZ20" s="10"/>
+      <c r="TA20" s="10"/>
+      <c r="TB20" s="10"/>
+      <c r="TC20" s="10"/>
+      <c r="TD20" s="10"/>
+      <c r="TE20" s="10"/>
+      <c r="TF20" s="10"/>
+      <c r="TG20" s="10"/>
+      <c r="TH20" s="10"/>
+      <c r="TI20" s="10"/>
+      <c r="TJ20" s="10"/>
+      <c r="TK20" s="10"/>
+      <c r="TL20" s="10"/>
+      <c r="TM20" s="10"/>
+      <c r="TN20" s="10"/>
+      <c r="TO20" s="10"/>
+      <c r="TP20" s="10"/>
+      <c r="TQ20" s="10"/>
+      <c r="TR20" s="10"/>
+      <c r="TS20" s="10"/>
+      <c r="TT20" s="10"/>
+      <c r="TU20" s="10"/>
+      <c r="TV20" s="10"/>
+      <c r="TW20" s="10"/>
+      <c r="TX20" s="10"/>
+      <c r="TY20" s="10"/>
+      <c r="TZ20" s="10"/>
+      <c r="UA20" s="10"/>
+      <c r="UB20" s="10"/>
+      <c r="UC20" s="10"/>
+      <c r="UD20" s="10"/>
+      <c r="UE20" s="10"/>
+      <c r="UF20" s="10"/>
+      <c r="UG20" s="10"/>
+      <c r="UH20" s="10"/>
+      <c r="UI20" s="10"/>
+      <c r="UJ20" s="10"/>
+      <c r="UK20" s="10"/>
+      <c r="UL20" s="10"/>
+      <c r="UM20" s="10"/>
+      <c r="UN20" s="10"/>
+      <c r="UO20" s="10"/>
+      <c r="UP20" s="10"/>
+      <c r="UQ20" s="10"/>
+      <c r="UR20" s="10"/>
+      <c r="US20" s="10"/>
+      <c r="UT20" s="10"/>
+      <c r="UU20" s="10"/>
+      <c r="UV20" s="10"/>
+      <c r="UW20" s="10"/>
+      <c r="UX20" s="10"/>
+      <c r="UY20" s="10"/>
+      <c r="UZ20" s="10"/>
+      <c r="VA20" s="10"/>
+      <c r="VB20" s="10"/>
+      <c r="VC20" s="10"/>
+      <c r="VD20" s="10"/>
+      <c r="VE20" s="10"/>
+      <c r="VF20" s="10"/>
+      <c r="VG20" s="10"/>
+      <c r="VH20" s="10"/>
+      <c r="VI20" s="10"/>
+      <c r="VJ20" s="10"/>
+      <c r="VK20" s="10"/>
+      <c r="VL20" s="10"/>
+      <c r="VM20" s="10"/>
+      <c r="VN20" s="10"/>
+      <c r="VO20" s="10"/>
+      <c r="VP20" s="10"/>
+      <c r="VQ20" s="10"/>
+      <c r="VR20" s="10"/>
+      <c r="VS20" s="10"/>
+      <c r="VT20" s="10"/>
+      <c r="VU20" s="10"/>
+      <c r="VV20" s="10"/>
+      <c r="VW20" s="10"/>
+      <c r="VX20" s="10"/>
+      <c r="VY20" s="10"/>
+      <c r="VZ20" s="10"/>
+      <c r="WA20" s="10"/>
+      <c r="WB20" s="10"/>
+      <c r="WC20" s="10"/>
+      <c r="WD20" s="10"/>
+      <c r="WE20" s="10"/>
+      <c r="WF20" s="10"/>
+      <c r="WG20" s="10"/>
+      <c r="WH20" s="10"/>
+      <c r="WI20" s="10"/>
+      <c r="WJ20" s="10"/>
+      <c r="WK20" s="10"/>
+      <c r="WL20" s="10"/>
+      <c r="WM20" s="10"/>
+      <c r="WN20" s="10"/>
+      <c r="WO20" s="10"/>
+      <c r="WP20" s="10"/>
+      <c r="WQ20" s="10"/>
+      <c r="WR20" s="10"/>
+      <c r="WS20" s="10"/>
+      <c r="WT20" s="10"/>
+      <c r="WU20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G21" s="3"/>
       <c r="I21" s="1"/>
@@ -5357,616 +5413,616 @@
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
-      <c r="AA21" s="9"/>
-      <c r="AB21" s="9"/>
-      <c r="AC21" s="9"/>
-      <c r="AD21" s="9"/>
-      <c r="AE21" s="9"/>
-      <c r="AF21" s="9"/>
-      <c r="AG21" s="9"/>
-      <c r="AH21" s="9"/>
-      <c r="AI21" s="9"/>
-      <c r="AJ21" s="9"/>
-      <c r="AK21" s="9"/>
-      <c r="AL21" s="9"/>
-      <c r="AM21" s="9"/>
-      <c r="AN21" s="9"/>
-      <c r="AO21" s="9"/>
-      <c r="AP21" s="9"/>
-      <c r="AQ21" s="9"/>
-      <c r="AR21" s="9"/>
-      <c r="AS21" s="9"/>
-      <c r="AT21" s="9"/>
-      <c r="AU21" s="9"/>
-      <c r="AV21" s="9"/>
-      <c r="AW21" s="9"/>
-      <c r="AX21" s="9"/>
-      <c r="AY21" s="9"/>
-      <c r="AZ21" s="9"/>
-      <c r="BA21" s="9"/>
-      <c r="BB21" s="9"/>
-      <c r="BC21" s="9"/>
-      <c r="BD21" s="9"/>
-      <c r="BE21" s="9"/>
-      <c r="BF21" s="9"/>
-      <c r="BG21" s="9"/>
-      <c r="BH21" s="9"/>
-      <c r="BI21" s="9"/>
-      <c r="BJ21" s="9"/>
-      <c r="BK21" s="9"/>
-      <c r="BL21" s="9"/>
-      <c r="BM21" s="9"/>
-      <c r="BN21" s="9"/>
-      <c r="BO21" s="9"/>
-      <c r="BP21" s="9"/>
-      <c r="BQ21" s="9"/>
-      <c r="BR21" s="9"/>
-      <c r="BS21" s="9"/>
-      <c r="BT21" s="9"/>
-      <c r="BU21" s="9"/>
-      <c r="BV21" s="9"/>
-      <c r="BW21" s="9"/>
-      <c r="BX21" s="9"/>
-      <c r="BY21" s="9"/>
-      <c r="BZ21" s="9"/>
-      <c r="CA21" s="9"/>
-      <c r="CB21" s="9"/>
-      <c r="CC21" s="9"/>
-      <c r="CD21" s="9"/>
-      <c r="CE21" s="9"/>
-      <c r="CF21" s="9"/>
-      <c r="CG21" s="9"/>
-      <c r="CH21" s="9"/>
-      <c r="CI21" s="9"/>
-      <c r="CJ21" s="9"/>
-      <c r="CK21" s="9"/>
-      <c r="CL21" s="9"/>
-      <c r="CM21" s="9"/>
-      <c r="CN21" s="9"/>
-      <c r="CO21" s="9"/>
-      <c r="CP21" s="9"/>
-      <c r="CQ21" s="9"/>
-      <c r="CR21" s="9"/>
-      <c r="CS21" s="9"/>
-      <c r="CT21" s="9"/>
-      <c r="CU21" s="9"/>
-      <c r="CV21" s="9"/>
-      <c r="CW21" s="9"/>
-      <c r="CX21" s="9"/>
-      <c r="CY21" s="9"/>
-      <c r="CZ21" s="9"/>
-      <c r="DA21" s="9"/>
-      <c r="DB21" s="9"/>
-      <c r="DC21" s="9"/>
-      <c r="DD21" s="9"/>
-      <c r="DE21" s="9"/>
-      <c r="DF21" s="9"/>
-      <c r="DG21" s="9"/>
-      <c r="DH21" s="9"/>
-      <c r="DI21" s="9"/>
-      <c r="DJ21" s="9"/>
-      <c r="DK21" s="9"/>
-      <c r="DL21" s="9"/>
-      <c r="DM21" s="9"/>
-      <c r="DN21" s="9"/>
-      <c r="DO21" s="9"/>
-      <c r="DP21" s="9"/>
-      <c r="DQ21" s="9"/>
-      <c r="DR21" s="9"/>
-      <c r="DS21" s="9"/>
-      <c r="DT21" s="9"/>
-      <c r="DU21" s="9"/>
-      <c r="DV21" s="9"/>
-      <c r="DW21" s="9"/>
-      <c r="DX21" s="9"/>
-      <c r="DY21" s="9"/>
-      <c r="DZ21" s="9"/>
-      <c r="EA21" s="9"/>
-      <c r="EB21" s="9"/>
-      <c r="EC21" s="9"/>
-      <c r="ED21" s="9"/>
-      <c r="EE21" s="9"/>
-      <c r="EF21" s="9"/>
-      <c r="EG21" s="9"/>
-      <c r="EH21" s="9"/>
-      <c r="EI21" s="9"/>
-      <c r="EJ21" s="9"/>
-      <c r="EK21" s="9"/>
-      <c r="EL21" s="9"/>
-      <c r="EM21" s="9"/>
-      <c r="EN21" s="9"/>
-      <c r="EO21" s="9"/>
-      <c r="EP21" s="9"/>
-      <c r="EQ21" s="9"/>
-      <c r="ER21" s="9"/>
-      <c r="ES21" s="9"/>
-      <c r="ET21" s="9"/>
-      <c r="EU21" s="9"/>
-      <c r="EV21" s="9"/>
-      <c r="EW21" s="9"/>
-      <c r="EX21" s="9"/>
-      <c r="EY21" s="9"/>
-      <c r="EZ21" s="9"/>
-      <c r="FA21" s="9"/>
-      <c r="FB21" s="9"/>
-      <c r="FC21" s="9"/>
-      <c r="FD21" s="9"/>
-      <c r="FE21" s="9"/>
-      <c r="FF21" s="9"/>
-      <c r="FG21" s="9"/>
-      <c r="FH21" s="9"/>
-      <c r="FI21" s="9"/>
-      <c r="FJ21" s="9"/>
-      <c r="FK21" s="9"/>
-      <c r="FL21" s="9"/>
-      <c r="FM21" s="9"/>
-      <c r="FN21" s="9"/>
-      <c r="FO21" s="9"/>
-      <c r="FP21" s="9"/>
-      <c r="FQ21" s="9"/>
-      <c r="FR21" s="9"/>
-      <c r="FS21" s="9"/>
-      <c r="FT21" s="9"/>
-      <c r="FU21" s="9"/>
-      <c r="FV21" s="9"/>
-      <c r="FW21" s="9"/>
-      <c r="FX21" s="9"/>
-      <c r="FY21" s="9"/>
-      <c r="FZ21" s="9"/>
-      <c r="GA21" s="9"/>
-      <c r="GB21" s="9"/>
-      <c r="GC21" s="9"/>
-      <c r="GD21" s="9"/>
-      <c r="GE21" s="9"/>
-      <c r="GF21" s="9"/>
-      <c r="GG21" s="9"/>
-      <c r="GH21" s="9"/>
-      <c r="GI21" s="9"/>
-      <c r="GJ21" s="9"/>
-      <c r="GK21" s="9"/>
-      <c r="GL21" s="9"/>
-      <c r="GM21" s="9"/>
-      <c r="GN21" s="9"/>
-      <c r="GO21" s="9"/>
-      <c r="GP21" s="9"/>
-      <c r="GQ21" s="9"/>
-      <c r="GR21" s="9"/>
-      <c r="GS21" s="9"/>
-      <c r="GT21" s="9"/>
-      <c r="GU21" s="9"/>
-      <c r="GV21" s="9"/>
-      <c r="GW21" s="9"/>
-      <c r="GX21" s="9"/>
-      <c r="GY21" s="9"/>
-      <c r="GZ21" s="9"/>
-      <c r="HA21" s="9"/>
-      <c r="HB21" s="9"/>
-      <c r="HC21" s="9"/>
-      <c r="HD21" s="9"/>
-      <c r="HE21" s="9"/>
-      <c r="HF21" s="9"/>
-      <c r="HG21" s="9"/>
-      <c r="HH21" s="9"/>
-      <c r="HI21" s="9"/>
-      <c r="HJ21" s="9"/>
-      <c r="HK21" s="9"/>
-      <c r="HL21" s="9"/>
-      <c r="HM21" s="9"/>
-      <c r="HN21" s="9"/>
-      <c r="HO21" s="9"/>
-      <c r="HP21" s="9"/>
-      <c r="HQ21" s="9"/>
-      <c r="HR21" s="9"/>
-      <c r="HS21" s="9"/>
-      <c r="HT21" s="9"/>
-      <c r="HU21" s="9"/>
-      <c r="HV21" s="9"/>
-      <c r="HW21" s="9"/>
-      <c r="HX21" s="9"/>
-      <c r="HY21" s="9"/>
-      <c r="HZ21" s="9"/>
-      <c r="IA21" s="9"/>
-      <c r="IB21" s="9"/>
-      <c r="IC21" s="9"/>
-      <c r="ID21" s="9"/>
-      <c r="IE21" s="9"/>
-      <c r="IF21" s="9"/>
-      <c r="IG21" s="9"/>
-      <c r="IH21" s="9"/>
-      <c r="II21" s="9"/>
-      <c r="IJ21" s="9"/>
-      <c r="IK21" s="9"/>
-      <c r="IL21" s="9"/>
-      <c r="IM21" s="9"/>
-      <c r="IN21" s="9"/>
-      <c r="IO21" s="9"/>
-      <c r="IP21" s="9"/>
-      <c r="IQ21" s="9"/>
-      <c r="IR21" s="9"/>
-      <c r="IS21" s="9"/>
-      <c r="IT21" s="9"/>
-      <c r="IU21" s="9"/>
-      <c r="IV21" s="9"/>
-      <c r="IW21" s="9"/>
-      <c r="IX21" s="9"/>
-      <c r="IY21" s="9"/>
-      <c r="IZ21" s="9"/>
-      <c r="JA21" s="9"/>
-      <c r="JB21" s="9"/>
-      <c r="JC21" s="9"/>
-      <c r="JD21" s="9"/>
-      <c r="JE21" s="9"/>
-      <c r="JF21" s="9"/>
-      <c r="JG21" s="9"/>
-      <c r="JH21" s="9"/>
-      <c r="JI21" s="9"/>
-      <c r="JJ21" s="9"/>
-      <c r="JK21" s="9"/>
-      <c r="JL21" s="9"/>
-      <c r="JM21" s="9"/>
-      <c r="JN21" s="9"/>
-      <c r="JO21" s="9"/>
-      <c r="JP21" s="9"/>
-      <c r="JQ21" s="9"/>
-      <c r="JR21" s="9"/>
-      <c r="JS21" s="9"/>
-      <c r="JT21" s="9"/>
-      <c r="JU21" s="9"/>
-      <c r="JV21" s="9"/>
-      <c r="JW21" s="9"/>
-      <c r="JX21" s="9"/>
-      <c r="JY21" s="9"/>
-      <c r="JZ21" s="9"/>
-      <c r="KA21" s="9"/>
-      <c r="KB21" s="9"/>
-      <c r="KC21" s="9"/>
-      <c r="KD21" s="9"/>
-      <c r="KE21" s="9"/>
-      <c r="KF21" s="9"/>
-      <c r="KG21" s="9"/>
-      <c r="KH21" s="9"/>
-      <c r="KI21" s="9"/>
-      <c r="KJ21" s="9"/>
-      <c r="KK21" s="9"/>
-      <c r="KL21" s="9"/>
-      <c r="KM21" s="9"/>
-      <c r="KN21" s="9"/>
-      <c r="KO21" s="9"/>
-      <c r="KP21" s="9"/>
-      <c r="KQ21" s="9"/>
-      <c r="KR21" s="9"/>
-      <c r="KS21" s="9"/>
-      <c r="KT21" s="9"/>
-      <c r="KU21" s="9"/>
-      <c r="KV21" s="9"/>
-      <c r="KW21" s="9"/>
-      <c r="KX21" s="9"/>
-      <c r="KY21" s="9"/>
-      <c r="KZ21" s="9"/>
-      <c r="LA21" s="9"/>
-      <c r="LB21" s="9"/>
-      <c r="LC21" s="9"/>
-      <c r="LD21" s="9"/>
-      <c r="LE21" s="9"/>
-      <c r="LF21" s="9"/>
-      <c r="LG21" s="9"/>
-      <c r="LH21" s="9"/>
-      <c r="LI21" s="9"/>
-      <c r="LJ21" s="9"/>
-      <c r="LK21" s="9"/>
-      <c r="LL21" s="9"/>
-      <c r="LM21" s="9"/>
-      <c r="LN21" s="9"/>
-      <c r="LO21" s="9"/>
-      <c r="LP21" s="9"/>
-      <c r="LQ21" s="9"/>
-      <c r="LR21" s="9"/>
-      <c r="LS21" s="9"/>
-      <c r="LT21" s="9"/>
-      <c r="LU21" s="9"/>
-      <c r="LV21" s="9"/>
-      <c r="LW21" s="9"/>
-      <c r="LX21" s="9"/>
-      <c r="LY21" s="9"/>
-      <c r="LZ21" s="9"/>
-      <c r="MA21" s="9"/>
-      <c r="MB21" s="9"/>
-      <c r="MC21" s="9"/>
-      <c r="MD21" s="9"/>
-      <c r="ME21" s="9"/>
-      <c r="MF21" s="9"/>
-      <c r="MG21" s="9"/>
-      <c r="MH21" s="9"/>
-      <c r="MI21" s="9"/>
-      <c r="MJ21" s="9"/>
-      <c r="MK21" s="9"/>
-      <c r="ML21" s="9"/>
-      <c r="MM21" s="9"/>
-      <c r="MN21" s="9"/>
-      <c r="MO21" s="9"/>
-      <c r="MP21" s="9"/>
-      <c r="MQ21" s="9"/>
-      <c r="MR21" s="9"/>
-      <c r="MS21" s="9"/>
-      <c r="MT21" s="9"/>
-      <c r="MU21" s="9"/>
-      <c r="MV21" s="9"/>
-      <c r="MW21" s="9"/>
-      <c r="MX21" s="9"/>
-      <c r="MY21" s="9"/>
-      <c r="MZ21" s="9"/>
-      <c r="NA21" s="9"/>
-      <c r="NB21" s="9"/>
-      <c r="NC21" s="9"/>
-      <c r="ND21" s="9"/>
-      <c r="NE21" s="9"/>
-      <c r="NF21" s="9"/>
-      <c r="NG21" s="9"/>
-      <c r="NH21" s="9"/>
-      <c r="NI21" s="9"/>
-      <c r="NJ21" s="9"/>
-      <c r="NK21" s="9"/>
-      <c r="NL21" s="9"/>
-      <c r="NM21" s="9"/>
-      <c r="NN21" s="9"/>
-      <c r="NO21" s="9"/>
-      <c r="NP21" s="9"/>
-      <c r="NQ21" s="9"/>
-      <c r="NR21" s="9"/>
-      <c r="NS21" s="9"/>
-      <c r="NT21" s="9"/>
-      <c r="NU21" s="9"/>
-      <c r="NV21" s="9"/>
-      <c r="NW21" s="9"/>
-      <c r="NX21" s="9"/>
-      <c r="NY21" s="9"/>
-      <c r="NZ21" s="9"/>
-      <c r="OA21" s="9"/>
-      <c r="OB21" s="9"/>
-      <c r="OC21" s="9"/>
-      <c r="OD21" s="9"/>
-      <c r="OE21" s="9"/>
-      <c r="OF21" s="9"/>
-      <c r="OG21" s="9"/>
-      <c r="OH21" s="9"/>
-      <c r="OI21" s="9"/>
-      <c r="OJ21" s="9"/>
-      <c r="OK21" s="9"/>
-      <c r="OL21" s="9"/>
-      <c r="OM21" s="9"/>
-      <c r="ON21" s="9"/>
-      <c r="OO21" s="9"/>
-      <c r="OP21" s="9"/>
-      <c r="OQ21" s="9"/>
-      <c r="OR21" s="9"/>
-      <c r="OS21" s="9"/>
-      <c r="OT21" s="9"/>
-      <c r="OU21" s="9"/>
-      <c r="OV21" s="9"/>
-      <c r="OW21" s="9"/>
-      <c r="OX21" s="9"/>
-      <c r="OY21" s="9"/>
-      <c r="OZ21" s="9"/>
-      <c r="PA21" s="9"/>
-      <c r="PB21" s="9"/>
-      <c r="PC21" s="9"/>
-      <c r="PD21" s="9"/>
-      <c r="PE21" s="9"/>
-      <c r="PF21" s="9"/>
-      <c r="PG21" s="9"/>
-      <c r="PH21" s="9"/>
-      <c r="PI21" s="9"/>
-      <c r="PJ21" s="9"/>
-      <c r="PK21" s="9"/>
-      <c r="PL21" s="9"/>
-      <c r="PM21" s="9"/>
-      <c r="PN21" s="9"/>
-      <c r="PO21" s="9"/>
-      <c r="PP21" s="9"/>
-      <c r="PQ21" s="9"/>
-      <c r="PR21" s="9"/>
-      <c r="PS21" s="9"/>
-      <c r="PT21" s="9"/>
-      <c r="PU21" s="9"/>
-      <c r="PV21" s="9"/>
-      <c r="PW21" s="9"/>
-      <c r="PX21" s="9"/>
-      <c r="PY21" s="9"/>
-      <c r="PZ21" s="9"/>
-      <c r="QA21" s="9"/>
-      <c r="QB21" s="9"/>
-      <c r="QC21" s="9"/>
-      <c r="QD21" s="9"/>
-      <c r="QE21" s="9"/>
-      <c r="QF21" s="9"/>
-      <c r="QG21" s="9"/>
-      <c r="QH21" s="9"/>
-      <c r="QI21" s="9"/>
-      <c r="QJ21" s="9"/>
-      <c r="QK21" s="9"/>
-      <c r="QL21" s="9"/>
-      <c r="QM21" s="9"/>
-      <c r="QN21" s="9"/>
-      <c r="QO21" s="9"/>
-      <c r="QP21" s="9"/>
-      <c r="QQ21" s="9"/>
-      <c r="QR21" s="9"/>
-      <c r="QS21" s="9"/>
-      <c r="QT21" s="9"/>
-      <c r="QU21" s="9"/>
-      <c r="QV21" s="9"/>
-      <c r="QW21" s="9"/>
-      <c r="QX21" s="9"/>
-      <c r="QY21" s="9"/>
-      <c r="QZ21" s="9"/>
-      <c r="RA21" s="9"/>
-      <c r="RB21" s="9"/>
-      <c r="RC21" s="9"/>
-      <c r="RD21" s="9"/>
-      <c r="RE21" s="9"/>
-      <c r="RF21" s="9"/>
-      <c r="RG21" s="9"/>
-      <c r="RH21" s="9"/>
-      <c r="RI21" s="9"/>
-      <c r="RJ21" s="9"/>
-      <c r="RK21" s="9"/>
-      <c r="RL21" s="9"/>
-      <c r="RM21" s="9"/>
-      <c r="RN21" s="9"/>
-      <c r="RO21" s="9"/>
-      <c r="RP21" s="9"/>
-      <c r="RQ21" s="9"/>
-      <c r="RR21" s="9"/>
-      <c r="RS21" s="9"/>
-      <c r="RT21" s="9"/>
-      <c r="RU21" s="9"/>
-      <c r="RV21" s="9"/>
-      <c r="RW21" s="9"/>
-      <c r="RX21" s="9"/>
-      <c r="RY21" s="9"/>
-      <c r="RZ21" s="9"/>
-      <c r="SA21" s="9"/>
-      <c r="SB21" s="9"/>
-      <c r="SC21" s="9"/>
-      <c r="SD21" s="9"/>
-      <c r="SE21" s="9"/>
-      <c r="SF21" s="9"/>
-      <c r="SG21" s="9"/>
-      <c r="SH21" s="9"/>
-      <c r="SI21" s="9"/>
-      <c r="SJ21" s="9"/>
-      <c r="SK21" s="9"/>
-      <c r="SL21" s="9"/>
-      <c r="SM21" s="9"/>
-      <c r="SN21" s="9"/>
-      <c r="SO21" s="9"/>
-      <c r="SP21" s="9"/>
-      <c r="SQ21" s="9"/>
-      <c r="SR21" s="9"/>
-      <c r="SS21" s="9"/>
-      <c r="ST21" s="9"/>
-      <c r="SU21" s="9"/>
-      <c r="SV21" s="9"/>
-      <c r="SW21" s="9"/>
-      <c r="SX21" s="9"/>
-      <c r="SY21" s="9"/>
-      <c r="SZ21" s="9"/>
-      <c r="TA21" s="9"/>
-      <c r="TB21" s="9"/>
-      <c r="TC21" s="9"/>
-      <c r="TD21" s="9"/>
-      <c r="TE21" s="9"/>
-      <c r="TF21" s="9"/>
-      <c r="TG21" s="9"/>
-      <c r="TH21" s="9"/>
-      <c r="TI21" s="9"/>
-      <c r="TJ21" s="9"/>
-      <c r="TK21" s="9"/>
-      <c r="TL21" s="9"/>
-      <c r="TM21" s="9"/>
-      <c r="TN21" s="9"/>
-      <c r="TO21" s="9"/>
-      <c r="TP21" s="9"/>
-      <c r="TQ21" s="9"/>
-      <c r="TR21" s="9"/>
-      <c r="TS21" s="9"/>
-      <c r="TT21" s="9"/>
-      <c r="TU21" s="9"/>
-      <c r="TV21" s="9"/>
-      <c r="TW21" s="9"/>
-      <c r="TX21" s="9"/>
-      <c r="TY21" s="9"/>
-      <c r="TZ21" s="9"/>
-      <c r="UA21" s="9"/>
-      <c r="UB21" s="9"/>
-      <c r="UC21" s="9"/>
-      <c r="UD21" s="9"/>
-      <c r="UE21" s="9"/>
-      <c r="UF21" s="9"/>
-      <c r="UG21" s="9"/>
-      <c r="UH21" s="9"/>
-      <c r="UI21" s="9"/>
-      <c r="UJ21" s="9"/>
-      <c r="UK21" s="9"/>
-      <c r="UL21" s="9"/>
-      <c r="UM21" s="9"/>
-      <c r="UN21" s="9"/>
-      <c r="UO21" s="9"/>
-      <c r="UP21" s="9"/>
-      <c r="UQ21" s="9"/>
-      <c r="UR21" s="9"/>
-      <c r="US21" s="9"/>
-      <c r="UT21" s="9"/>
-      <c r="UU21" s="9"/>
-      <c r="UV21" s="9"/>
-      <c r="UW21" s="9"/>
-      <c r="UX21" s="9"/>
-      <c r="UY21" s="9"/>
-      <c r="UZ21" s="9"/>
-      <c r="VA21" s="9"/>
-      <c r="VB21" s="9"/>
-      <c r="VC21" s="9"/>
-      <c r="VD21" s="9"/>
-      <c r="VE21" s="9"/>
-      <c r="VF21" s="9"/>
-      <c r="VG21" s="9"/>
-      <c r="VH21" s="9"/>
-      <c r="VI21" s="9"/>
-      <c r="VJ21" s="9"/>
-      <c r="VK21" s="9"/>
-      <c r="VL21" s="9"/>
-      <c r="VM21" s="9"/>
-      <c r="VN21" s="9"/>
-      <c r="VO21" s="9"/>
-      <c r="VP21" s="9"/>
-      <c r="VQ21" s="9"/>
-      <c r="VR21" s="9"/>
-      <c r="VS21" s="9"/>
-      <c r="VT21" s="9"/>
-      <c r="VU21" s="9"/>
-      <c r="VV21" s="9"/>
-      <c r="VW21" s="9"/>
-      <c r="VX21" s="9"/>
-      <c r="VY21" s="9"/>
-      <c r="VZ21" s="9"/>
-      <c r="WA21" s="9"/>
-      <c r="WB21" s="9"/>
-      <c r="WC21" s="9"/>
-      <c r="WD21" s="9"/>
-      <c r="WE21" s="9"/>
-      <c r="WF21" s="9"/>
-      <c r="WG21" s="9"/>
-      <c r="WH21" s="9"/>
-      <c r="WI21" s="9"/>
-      <c r="WJ21" s="9"/>
-      <c r="WK21" s="9"/>
-      <c r="WL21" s="9"/>
-      <c r="WM21" s="9"/>
-      <c r="WN21" s="9"/>
-      <c r="WO21" s="9"/>
-      <c r="WP21" s="9"/>
-      <c r="WQ21" s="9"/>
-      <c r="WR21" s="9"/>
-      <c r="WS21" s="9"/>
-      <c r="WT21" s="9"/>
-      <c r="WU21" s="9"/>
+      <c r="AA21" s="10"/>
+      <c r="AB21" s="10"/>
+      <c r="AC21" s="10"/>
+      <c r="AD21" s="10"/>
+      <c r="AE21" s="10"/>
+      <c r="AF21" s="10"/>
+      <c r="AG21" s="10"/>
+      <c r="AH21" s="10"/>
+      <c r="AI21" s="10"/>
+      <c r="AJ21" s="10"/>
+      <c r="AK21" s="10"/>
+      <c r="AL21" s="10"/>
+      <c r="AM21" s="10"/>
+      <c r="AN21" s="10"/>
+      <c r="AO21" s="10"/>
+      <c r="AP21" s="10"/>
+      <c r="AQ21" s="10"/>
+      <c r="AR21" s="10"/>
+      <c r="AS21" s="10"/>
+      <c r="AT21" s="10"/>
+      <c r="AU21" s="10"/>
+      <c r="AV21" s="10"/>
+      <c r="AW21" s="10"/>
+      <c r="AX21" s="10"/>
+      <c r="AY21" s="10"/>
+      <c r="AZ21" s="10"/>
+      <c r="BA21" s="10"/>
+      <c r="BB21" s="10"/>
+      <c r="BC21" s="10"/>
+      <c r="BD21" s="10"/>
+      <c r="BE21" s="10"/>
+      <c r="BF21" s="10"/>
+      <c r="BG21" s="10"/>
+      <c r="BH21" s="10"/>
+      <c r="BI21" s="10"/>
+      <c r="BJ21" s="10"/>
+      <c r="BK21" s="10"/>
+      <c r="BL21" s="10"/>
+      <c r="BM21" s="10"/>
+      <c r="BN21" s="10"/>
+      <c r="BO21" s="10"/>
+      <c r="BP21" s="10"/>
+      <c r="BQ21" s="10"/>
+      <c r="BR21" s="10"/>
+      <c r="BS21" s="10"/>
+      <c r="BT21" s="10"/>
+      <c r="BU21" s="10"/>
+      <c r="BV21" s="10"/>
+      <c r="BW21" s="10"/>
+      <c r="BX21" s="10"/>
+      <c r="BY21" s="10"/>
+      <c r="BZ21" s="10"/>
+      <c r="CA21" s="10"/>
+      <c r="CB21" s="10"/>
+      <c r="CC21" s="10"/>
+      <c r="CD21" s="10"/>
+      <c r="CE21" s="10"/>
+      <c r="CF21" s="10"/>
+      <c r="CG21" s="10"/>
+      <c r="CH21" s="10"/>
+      <c r="CI21" s="10"/>
+      <c r="CJ21" s="10"/>
+      <c r="CK21" s="10"/>
+      <c r="CL21" s="10"/>
+      <c r="CM21" s="10"/>
+      <c r="CN21" s="10"/>
+      <c r="CO21" s="10"/>
+      <c r="CP21" s="10"/>
+      <c r="CQ21" s="10"/>
+      <c r="CR21" s="10"/>
+      <c r="CS21" s="10"/>
+      <c r="CT21" s="10"/>
+      <c r="CU21" s="10"/>
+      <c r="CV21" s="10"/>
+      <c r="CW21" s="10"/>
+      <c r="CX21" s="10"/>
+      <c r="CY21" s="10"/>
+      <c r="CZ21" s="10"/>
+      <c r="DA21" s="10"/>
+      <c r="DB21" s="10"/>
+      <c r="DC21" s="10"/>
+      <c r="DD21" s="10"/>
+      <c r="DE21" s="10"/>
+      <c r="DF21" s="10"/>
+      <c r="DG21" s="10"/>
+      <c r="DH21" s="10"/>
+      <c r="DI21" s="10"/>
+      <c r="DJ21" s="10"/>
+      <c r="DK21" s="10"/>
+      <c r="DL21" s="10"/>
+      <c r="DM21" s="10"/>
+      <c r="DN21" s="10"/>
+      <c r="DO21" s="10"/>
+      <c r="DP21" s="10"/>
+      <c r="DQ21" s="10"/>
+      <c r="DR21" s="10"/>
+      <c r="DS21" s="10"/>
+      <c r="DT21" s="10"/>
+      <c r="DU21" s="10"/>
+      <c r="DV21" s="10"/>
+      <c r="DW21" s="10"/>
+      <c r="DX21" s="10"/>
+      <c r="DY21" s="10"/>
+      <c r="DZ21" s="10"/>
+      <c r="EA21" s="10"/>
+      <c r="EB21" s="10"/>
+      <c r="EC21" s="10"/>
+      <c r="ED21" s="10"/>
+      <c r="EE21" s="10"/>
+      <c r="EF21" s="10"/>
+      <c r="EG21" s="10"/>
+      <c r="EH21" s="10"/>
+      <c r="EI21" s="10"/>
+      <c r="EJ21" s="10"/>
+      <c r="EK21" s="10"/>
+      <c r="EL21" s="10"/>
+      <c r="EM21" s="10"/>
+      <c r="EN21" s="10"/>
+      <c r="EO21" s="10"/>
+      <c r="EP21" s="10"/>
+      <c r="EQ21" s="10"/>
+      <c r="ER21" s="10"/>
+      <c r="ES21" s="10"/>
+      <c r="ET21" s="10"/>
+      <c r="EU21" s="10"/>
+      <c r="EV21" s="10"/>
+      <c r="EW21" s="10"/>
+      <c r="EX21" s="10"/>
+      <c r="EY21" s="10"/>
+      <c r="EZ21" s="10"/>
+      <c r="FA21" s="10"/>
+      <c r="FB21" s="10"/>
+      <c r="FC21" s="10"/>
+      <c r="FD21" s="10"/>
+      <c r="FE21" s="10"/>
+      <c r="FF21" s="10"/>
+      <c r="FG21" s="10"/>
+      <c r="FH21" s="10"/>
+      <c r="FI21" s="10"/>
+      <c r="FJ21" s="10"/>
+      <c r="FK21" s="10"/>
+      <c r="FL21" s="10"/>
+      <c r="FM21" s="10"/>
+      <c r="FN21" s="10"/>
+      <c r="FO21" s="10"/>
+      <c r="FP21" s="10"/>
+      <c r="FQ21" s="10"/>
+      <c r="FR21" s="10"/>
+      <c r="FS21" s="10"/>
+      <c r="FT21" s="10"/>
+      <c r="FU21" s="10"/>
+      <c r="FV21" s="10"/>
+      <c r="FW21" s="10"/>
+      <c r="FX21" s="10"/>
+      <c r="FY21" s="10"/>
+      <c r="FZ21" s="10"/>
+      <c r="GA21" s="10"/>
+      <c r="GB21" s="10"/>
+      <c r="GC21" s="10"/>
+      <c r="GD21" s="10"/>
+      <c r="GE21" s="10"/>
+      <c r="GF21" s="10"/>
+      <c r="GG21" s="10"/>
+      <c r="GH21" s="10"/>
+      <c r="GI21" s="10"/>
+      <c r="GJ21" s="10"/>
+      <c r="GK21" s="10"/>
+      <c r="GL21" s="10"/>
+      <c r="GM21" s="10"/>
+      <c r="GN21" s="10"/>
+      <c r="GO21" s="10"/>
+      <c r="GP21" s="10"/>
+      <c r="GQ21" s="10"/>
+      <c r="GR21" s="10"/>
+      <c r="GS21" s="10"/>
+      <c r="GT21" s="10"/>
+      <c r="GU21" s="10"/>
+      <c r="GV21" s="10"/>
+      <c r="GW21" s="10"/>
+      <c r="GX21" s="10"/>
+      <c r="GY21" s="10"/>
+      <c r="GZ21" s="10"/>
+      <c r="HA21" s="10"/>
+      <c r="HB21" s="10"/>
+      <c r="HC21" s="10"/>
+      <c r="HD21" s="10"/>
+      <c r="HE21" s="10"/>
+      <c r="HF21" s="10"/>
+      <c r="HG21" s="10"/>
+      <c r="HH21" s="10"/>
+      <c r="HI21" s="10"/>
+      <c r="HJ21" s="10"/>
+      <c r="HK21" s="10"/>
+      <c r="HL21" s="10"/>
+      <c r="HM21" s="10"/>
+      <c r="HN21" s="10"/>
+      <c r="HO21" s="10"/>
+      <c r="HP21" s="10"/>
+      <c r="HQ21" s="10"/>
+      <c r="HR21" s="10"/>
+      <c r="HS21" s="10"/>
+      <c r="HT21" s="10"/>
+      <c r="HU21" s="10"/>
+      <c r="HV21" s="10"/>
+      <c r="HW21" s="10"/>
+      <c r="HX21" s="10"/>
+      <c r="HY21" s="10"/>
+      <c r="HZ21" s="10"/>
+      <c r="IA21" s="10"/>
+      <c r="IB21" s="10"/>
+      <c r="IC21" s="10"/>
+      <c r="ID21" s="10"/>
+      <c r="IE21" s="10"/>
+      <c r="IF21" s="10"/>
+      <c r="IG21" s="10"/>
+      <c r="IH21" s="10"/>
+      <c r="II21" s="10"/>
+      <c r="IJ21" s="10"/>
+      <c r="IK21" s="10"/>
+      <c r="IL21" s="10"/>
+      <c r="IM21" s="10"/>
+      <c r="IN21" s="10"/>
+      <c r="IO21" s="10"/>
+      <c r="IP21" s="10"/>
+      <c r="IQ21" s="10"/>
+      <c r="IR21" s="10"/>
+      <c r="IS21" s="10"/>
+      <c r="IT21" s="10"/>
+      <c r="IU21" s="10"/>
+      <c r="IV21" s="10"/>
+      <c r="IW21" s="10"/>
+      <c r="IX21" s="10"/>
+      <c r="IY21" s="10"/>
+      <c r="IZ21" s="10"/>
+      <c r="JA21" s="10"/>
+      <c r="JB21" s="10"/>
+      <c r="JC21" s="10"/>
+      <c r="JD21" s="10"/>
+      <c r="JE21" s="10"/>
+      <c r="JF21" s="10"/>
+      <c r="JG21" s="10"/>
+      <c r="JH21" s="10"/>
+      <c r="JI21" s="10"/>
+      <c r="JJ21" s="10"/>
+      <c r="JK21" s="10"/>
+      <c r="JL21" s="10"/>
+      <c r="JM21" s="10"/>
+      <c r="JN21" s="10"/>
+      <c r="JO21" s="10"/>
+      <c r="JP21" s="10"/>
+      <c r="JQ21" s="10"/>
+      <c r="JR21" s="10"/>
+      <c r="JS21" s="10"/>
+      <c r="JT21" s="10"/>
+      <c r="JU21" s="10"/>
+      <c r="JV21" s="10"/>
+      <c r="JW21" s="10"/>
+      <c r="JX21" s="10"/>
+      <c r="JY21" s="10"/>
+      <c r="JZ21" s="10"/>
+      <c r="KA21" s="10"/>
+      <c r="KB21" s="10"/>
+      <c r="KC21" s="10"/>
+      <c r="KD21" s="10"/>
+      <c r="KE21" s="10"/>
+      <c r="KF21" s="10"/>
+      <c r="KG21" s="10"/>
+      <c r="KH21" s="10"/>
+      <c r="KI21" s="10"/>
+      <c r="KJ21" s="10"/>
+      <c r="KK21" s="10"/>
+      <c r="KL21" s="10"/>
+      <c r="KM21" s="10"/>
+      <c r="KN21" s="10"/>
+      <c r="KO21" s="10"/>
+      <c r="KP21" s="10"/>
+      <c r="KQ21" s="10"/>
+      <c r="KR21" s="10"/>
+      <c r="KS21" s="10"/>
+      <c r="KT21" s="10"/>
+      <c r="KU21" s="10"/>
+      <c r="KV21" s="10"/>
+      <c r="KW21" s="10"/>
+      <c r="KX21" s="10"/>
+      <c r="KY21" s="10"/>
+      <c r="KZ21" s="10"/>
+      <c r="LA21" s="10"/>
+      <c r="LB21" s="10"/>
+      <c r="LC21" s="10"/>
+      <c r="LD21" s="10"/>
+      <c r="LE21" s="10"/>
+      <c r="LF21" s="10"/>
+      <c r="LG21" s="10"/>
+      <c r="LH21" s="10"/>
+      <c r="LI21" s="10"/>
+      <c r="LJ21" s="10"/>
+      <c r="LK21" s="10"/>
+      <c r="LL21" s="10"/>
+      <c r="LM21" s="10"/>
+      <c r="LN21" s="10"/>
+      <c r="LO21" s="10"/>
+      <c r="LP21" s="10"/>
+      <c r="LQ21" s="10"/>
+      <c r="LR21" s="10"/>
+      <c r="LS21" s="10"/>
+      <c r="LT21" s="10"/>
+      <c r="LU21" s="10"/>
+      <c r="LV21" s="10"/>
+      <c r="LW21" s="10"/>
+      <c r="LX21" s="10"/>
+      <c r="LY21" s="10"/>
+      <c r="LZ21" s="10"/>
+      <c r="MA21" s="10"/>
+      <c r="MB21" s="10"/>
+      <c r="MC21" s="10"/>
+      <c r="MD21" s="10"/>
+      <c r="ME21" s="10"/>
+      <c r="MF21" s="10"/>
+      <c r="MG21" s="10"/>
+      <c r="MH21" s="10"/>
+      <c r="MI21" s="10"/>
+      <c r="MJ21" s="10"/>
+      <c r="MK21" s="10"/>
+      <c r="ML21" s="10"/>
+      <c r="MM21" s="10"/>
+      <c r="MN21" s="10"/>
+      <c r="MO21" s="10"/>
+      <c r="MP21" s="10"/>
+      <c r="MQ21" s="10"/>
+      <c r="MR21" s="10"/>
+      <c r="MS21" s="10"/>
+      <c r="MT21" s="10"/>
+      <c r="MU21" s="10"/>
+      <c r="MV21" s="10"/>
+      <c r="MW21" s="10"/>
+      <c r="MX21" s="10"/>
+      <c r="MY21" s="10"/>
+      <c r="MZ21" s="10"/>
+      <c r="NA21" s="10"/>
+      <c r="NB21" s="10"/>
+      <c r="NC21" s="10"/>
+      <c r="ND21" s="10"/>
+      <c r="NE21" s="10"/>
+      <c r="NF21" s="10"/>
+      <c r="NG21" s="10"/>
+      <c r="NH21" s="10"/>
+      <c r="NI21" s="10"/>
+      <c r="NJ21" s="10"/>
+      <c r="NK21" s="10"/>
+      <c r="NL21" s="10"/>
+      <c r="NM21" s="10"/>
+      <c r="NN21" s="10"/>
+      <c r="NO21" s="10"/>
+      <c r="NP21" s="10"/>
+      <c r="NQ21" s="10"/>
+      <c r="NR21" s="10"/>
+      <c r="NS21" s="10"/>
+      <c r="NT21" s="10"/>
+      <c r="NU21" s="10"/>
+      <c r="NV21" s="10"/>
+      <c r="NW21" s="10"/>
+      <c r="NX21" s="10"/>
+      <c r="NY21" s="10"/>
+      <c r="NZ21" s="10"/>
+      <c r="OA21" s="10"/>
+      <c r="OB21" s="10"/>
+      <c r="OC21" s="10"/>
+      <c r="OD21" s="10"/>
+      <c r="OE21" s="10"/>
+      <c r="OF21" s="10"/>
+      <c r="OG21" s="10"/>
+      <c r="OH21" s="10"/>
+      <c r="OI21" s="10"/>
+      <c r="OJ21" s="10"/>
+      <c r="OK21" s="10"/>
+      <c r="OL21" s="10"/>
+      <c r="OM21" s="10"/>
+      <c r="ON21" s="10"/>
+      <c r="OO21" s="10"/>
+      <c r="OP21" s="10"/>
+      <c r="OQ21" s="10"/>
+      <c r="OR21" s="10"/>
+      <c r="OS21" s="10"/>
+      <c r="OT21" s="10"/>
+      <c r="OU21" s="10"/>
+      <c r="OV21" s="10"/>
+      <c r="OW21" s="10"/>
+      <c r="OX21" s="10"/>
+      <c r="OY21" s="10"/>
+      <c r="OZ21" s="10"/>
+      <c r="PA21" s="10"/>
+      <c r="PB21" s="10"/>
+      <c r="PC21" s="10"/>
+      <c r="PD21" s="10"/>
+      <c r="PE21" s="10"/>
+      <c r="PF21" s="10"/>
+      <c r="PG21" s="10"/>
+      <c r="PH21" s="10"/>
+      <c r="PI21" s="10"/>
+      <c r="PJ21" s="10"/>
+      <c r="PK21" s="10"/>
+      <c r="PL21" s="10"/>
+      <c r="PM21" s="10"/>
+      <c r="PN21" s="10"/>
+      <c r="PO21" s="10"/>
+      <c r="PP21" s="10"/>
+      <c r="PQ21" s="10"/>
+      <c r="PR21" s="10"/>
+      <c r="PS21" s="10"/>
+      <c r="PT21" s="10"/>
+      <c r="PU21" s="10"/>
+      <c r="PV21" s="10"/>
+      <c r="PW21" s="10"/>
+      <c r="PX21" s="10"/>
+      <c r="PY21" s="10"/>
+      <c r="PZ21" s="10"/>
+      <c r="QA21" s="10"/>
+      <c r="QB21" s="10"/>
+      <c r="QC21" s="10"/>
+      <c r="QD21" s="10"/>
+      <c r="QE21" s="10"/>
+      <c r="QF21" s="10"/>
+      <c r="QG21" s="10"/>
+      <c r="QH21" s="10"/>
+      <c r="QI21" s="10"/>
+      <c r="QJ21" s="10"/>
+      <c r="QK21" s="10"/>
+      <c r="QL21" s="10"/>
+      <c r="QM21" s="10"/>
+      <c r="QN21" s="10"/>
+      <c r="QO21" s="10"/>
+      <c r="QP21" s="10"/>
+      <c r="QQ21" s="10"/>
+      <c r="QR21" s="10"/>
+      <c r="QS21" s="10"/>
+      <c r="QT21" s="10"/>
+      <c r="QU21" s="10"/>
+      <c r="QV21" s="10"/>
+      <c r="QW21" s="10"/>
+      <c r="QX21" s="10"/>
+      <c r="QY21" s="10"/>
+      <c r="QZ21" s="10"/>
+      <c r="RA21" s="10"/>
+      <c r="RB21" s="10"/>
+      <c r="RC21" s="10"/>
+      <c r="RD21" s="10"/>
+      <c r="RE21" s="10"/>
+      <c r="RF21" s="10"/>
+      <c r="RG21" s="10"/>
+      <c r="RH21" s="10"/>
+      <c r="RI21" s="10"/>
+      <c r="RJ21" s="10"/>
+      <c r="RK21" s="10"/>
+      <c r="RL21" s="10"/>
+      <c r="RM21" s="10"/>
+      <c r="RN21" s="10"/>
+      <c r="RO21" s="10"/>
+      <c r="RP21" s="10"/>
+      <c r="RQ21" s="10"/>
+      <c r="RR21" s="10"/>
+      <c r="RS21" s="10"/>
+      <c r="RT21" s="10"/>
+      <c r="RU21" s="10"/>
+      <c r="RV21" s="10"/>
+      <c r="RW21" s="10"/>
+      <c r="RX21" s="10"/>
+      <c r="RY21" s="10"/>
+      <c r="RZ21" s="10"/>
+      <c r="SA21" s="10"/>
+      <c r="SB21" s="10"/>
+      <c r="SC21" s="10"/>
+      <c r="SD21" s="10"/>
+      <c r="SE21" s="10"/>
+      <c r="SF21" s="10"/>
+      <c r="SG21" s="10"/>
+      <c r="SH21" s="10"/>
+      <c r="SI21" s="10"/>
+      <c r="SJ21" s="10"/>
+      <c r="SK21" s="10"/>
+      <c r="SL21" s="10"/>
+      <c r="SM21" s="10"/>
+      <c r="SN21" s="10"/>
+      <c r="SO21" s="10"/>
+      <c r="SP21" s="10"/>
+      <c r="SQ21" s="10"/>
+      <c r="SR21" s="10"/>
+      <c r="SS21" s="10"/>
+      <c r="ST21" s="10"/>
+      <c r="SU21" s="10"/>
+      <c r="SV21" s="10"/>
+      <c r="SW21" s="10"/>
+      <c r="SX21" s="10"/>
+      <c r="SY21" s="10"/>
+      <c r="SZ21" s="10"/>
+      <c r="TA21" s="10"/>
+      <c r="TB21" s="10"/>
+      <c r="TC21" s="10"/>
+      <c r="TD21" s="10"/>
+      <c r="TE21" s="10"/>
+      <c r="TF21" s="10"/>
+      <c r="TG21" s="10"/>
+      <c r="TH21" s="10"/>
+      <c r="TI21" s="10"/>
+      <c r="TJ21" s="10"/>
+      <c r="TK21" s="10"/>
+      <c r="TL21" s="10"/>
+      <c r="TM21" s="10"/>
+      <c r="TN21" s="10"/>
+      <c r="TO21" s="10"/>
+      <c r="TP21" s="10"/>
+      <c r="TQ21" s="10"/>
+      <c r="TR21" s="10"/>
+      <c r="TS21" s="10"/>
+      <c r="TT21" s="10"/>
+      <c r="TU21" s="10"/>
+      <c r="TV21" s="10"/>
+      <c r="TW21" s="10"/>
+      <c r="TX21" s="10"/>
+      <c r="TY21" s="10"/>
+      <c r="TZ21" s="10"/>
+      <c r="UA21" s="10"/>
+      <c r="UB21" s="10"/>
+      <c r="UC21" s="10"/>
+      <c r="UD21" s="10"/>
+      <c r="UE21" s="10"/>
+      <c r="UF21" s="10"/>
+      <c r="UG21" s="10"/>
+      <c r="UH21" s="10"/>
+      <c r="UI21" s="10"/>
+      <c r="UJ21" s="10"/>
+      <c r="UK21" s="10"/>
+      <c r="UL21" s="10"/>
+      <c r="UM21" s="10"/>
+      <c r="UN21" s="10"/>
+      <c r="UO21" s="10"/>
+      <c r="UP21" s="10"/>
+      <c r="UQ21" s="10"/>
+      <c r="UR21" s="10"/>
+      <c r="US21" s="10"/>
+      <c r="UT21" s="10"/>
+      <c r="UU21" s="10"/>
+      <c r="UV21" s="10"/>
+      <c r="UW21" s="10"/>
+      <c r="UX21" s="10"/>
+      <c r="UY21" s="10"/>
+      <c r="UZ21" s="10"/>
+      <c r="VA21" s="10"/>
+      <c r="VB21" s="10"/>
+      <c r="VC21" s="10"/>
+      <c r="VD21" s="10"/>
+      <c r="VE21" s="10"/>
+      <c r="VF21" s="10"/>
+      <c r="VG21" s="10"/>
+      <c r="VH21" s="10"/>
+      <c r="VI21" s="10"/>
+      <c r="VJ21" s="10"/>
+      <c r="VK21" s="10"/>
+      <c r="VL21" s="10"/>
+      <c r="VM21" s="10"/>
+      <c r="VN21" s="10"/>
+      <c r="VO21" s="10"/>
+      <c r="VP21" s="10"/>
+      <c r="VQ21" s="10"/>
+      <c r="VR21" s="10"/>
+      <c r="VS21" s="10"/>
+      <c r="VT21" s="10"/>
+      <c r="VU21" s="10"/>
+      <c r="VV21" s="10"/>
+      <c r="VW21" s="10"/>
+      <c r="VX21" s="10"/>
+      <c r="VY21" s="10"/>
+      <c r="VZ21" s="10"/>
+      <c r="WA21" s="10"/>
+      <c r="WB21" s="10"/>
+      <c r="WC21" s="10"/>
+      <c r="WD21" s="10"/>
+      <c r="WE21" s="10"/>
+      <c r="WF21" s="10"/>
+      <c r="WG21" s="10"/>
+      <c r="WH21" s="10"/>
+      <c r="WI21" s="10"/>
+      <c r="WJ21" s="10"/>
+      <c r="WK21" s="10"/>
+      <c r="WL21" s="10"/>
+      <c r="WM21" s="10"/>
+      <c r="WN21" s="10"/>
+      <c r="WO21" s="10"/>
+      <c r="WP21" s="10"/>
+      <c r="WQ21" s="10"/>
+      <c r="WR21" s="10"/>
+      <c r="WS21" s="10"/>
+      <c r="WT21" s="10"/>
+      <c r="WU21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G22" s="3"/>
       <c r="I22" s="1"/>
@@ -6583,20 +6639,20 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G23" s="3"/>
       <c r="I23" s="1"/>
@@ -7213,20 +7269,20 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G24" s="3"/>
       <c r="I24" s="1"/>
@@ -7843,20 +7899,20 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G25" s="3"/>
       <c r="I25" s="1"/>
@@ -8473,19 +8529,19 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -9103,17 +9159,17 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="11"/>
+        <v>73</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="12"/>
       <c r="E27" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F27" s="1"/>
       <c r="I27" s="1"/>
@@ -9730,20 +9786,20 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D28" s="11"/>
+        <v>75</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="12"/>
       <c r="E28" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -10359,20 +10415,20 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" s="11"/>
+        <v>76</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="12"/>
       <c r="E29" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F29" s="13" t="s">
-        <v>54</v>
+        <v>12</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>58</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -10987,18 +11043,18 @@
       <c r="WU29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" s="11"/>
+      <c r="A30" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="12"/>
       <c r="E30" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F30" s="1"/>
       <c r="I30" s="1"/>
@@ -11614,18 +11670,18 @@
       <c r="WU30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D31" s="11"/>
+      <c r="A31" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="12"/>
       <c r="E31" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F31" s="1"/>
       <c r="I31" s="1"/>
@@ -12241,20 +12297,20 @@
       <c r="WU31" s="1"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>11</v>
+      <c r="A32" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>12</v>
       </c>
       <c r="F32" s="1"/>
       <c r="I32" s="1"/>
@@ -12870,19 +12926,19 @@
       <c r="WU32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="11"/>
+      <c r="A33" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33" s="12"/>
       <c r="F33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -13497,19 +13553,19 @@
       <c r="WU33" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>9</v>
+      <c r="A34" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>10</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E34" s="11"/>
+        <v>37</v>
+      </c>
+      <c r="E34" s="12"/>
       <c r="F34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -14073,9 +14129,6 @@
       <c r="UV34" s="1"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0"/>
-      <c r="B35" s="0"/>
-      <c r="C35" s="0"/>
       <c r="D35" s="19"/>
       <c r="E35" s="20"/>
       <c r="F35" s="21"/>
@@ -14641,722 +14694,695 @@
       <c r="UV35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0"/>
-      <c r="B36" s="0"/>
-      <c r="C36" s="0"/>
       <c r="D36" s="19"/>
       <c r="E36" s="22"/>
       <c r="F36" s="23"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0"/>
-      <c r="B37" s="0"/>
-      <c r="C37" s="0"/>
       <c r="D37" s="19"/>
       <c r="F37" s="1"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0"/>
-      <c r="B38" s="0"/>
-      <c r="C38" s="0"/>
       <c r="D38" s="19"/>
       <c r="F38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0"/>
-      <c r="B39" s="0"/>
-      <c r="C39" s="0"/>
       <c r="D39" s="19"/>
-      <c r="E39" s="11"/>
+      <c r="E39" s="12"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0"/>
-      <c r="B40" s="0"/>
-      <c r="C40" s="0"/>
       <c r="D40" s="19"/>
-      <c r="E40" s="11"/>
+      <c r="E40" s="12"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0"/>
-      <c r="B41" s="0"/>
-      <c r="C41" s="0"/>
       <c r="D41" s="19"/>
-      <c r="E41" s="11"/>
+      <c r="E41" s="12"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0"/>
-      <c r="B42" s="0"/>
-      <c r="C42" s="0"/>
       <c r="D42" s="19"/>
-      <c r="E42" s="11"/>
+      <c r="E42" s="12"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0"/>
-      <c r="B43" s="0"/>
-      <c r="C43" s="0"/>
       <c r="D43" s="19"/>
-      <c r="E43" s="11"/>
+      <c r="E43" s="12"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0"/>
-      <c r="B44" s="0"/>
-      <c r="C44" s="0"/>
       <c r="D44" s="19"/>
-      <c r="E44" s="11"/>
+      <c r="E44" s="12"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C45" s="12"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C46" s="12"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C47" s="12"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C48" s="12"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C49" s="12"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C50" s="12"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C51" s="12"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C52" s="12"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C53" s="12"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="11"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C54" s="12"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="11"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C55" s="12"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="11"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C56" s="12"/>
-      <c r="D56" s="11"/>
-      <c r="E56" s="11"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C57" s="12"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="11"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C58" s="12"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="11"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C59" s="12"/>
-      <c r="D59" s="11"/>
-      <c r="E59" s="11"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C60" s="12"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="11"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C61" s="12"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C62" s="12"/>
-      <c r="D62" s="11"/>
-      <c r="E62" s="11"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C63" s="12"/>
-      <c r="D63" s="11"/>
-      <c r="E63" s="11"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C64" s="12"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="11"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C65" s="12"/>
-      <c r="D65" s="11"/>
-      <c r="E65" s="11"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C66" s="12"/>
-      <c r="D66" s="11"/>
-      <c r="E66" s="11"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="12"/>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C67" s="12"/>
-      <c r="D67" s="11"/>
-      <c r="E67" s="11"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C68" s="12"/>
-      <c r="D68" s="11"/>
-      <c r="E68" s="11"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12"/>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C69" s="12"/>
-      <c r="D69" s="11"/>
-      <c r="E69" s="11"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C70" s="12"/>
-      <c r="D70" s="11"/>
-      <c r="E70" s="11"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="12"/>
+      <c r="E70" s="12"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C71" s="12"/>
-      <c r="D71" s="11"/>
-      <c r="E71" s="11"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C72" s="12"/>
-      <c r="D72" s="11"/>
-      <c r="E72" s="11"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="12"/>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C73" s="12"/>
-      <c r="D73" s="11"/>
-      <c r="E73" s="11"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="12"/>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C74" s="12"/>
-      <c r="D74" s="11"/>
-      <c r="E74" s="11"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="12"/>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C75" s="12"/>
-      <c r="D75" s="11"/>
-      <c r="E75" s="11"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="12"/>
+      <c r="E75" s="12"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C76" s="12"/>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C77" s="12"/>
-      <c r="D77" s="11"/>
-      <c r="E77" s="11"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="12"/>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C78" s="12"/>
-      <c r="D78" s="11"/>
-      <c r="E78" s="11"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="12"/>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C79" s="12"/>
-      <c r="D79" s="11"/>
-      <c r="E79" s="11"/>
+      <c r="C79" s="13"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C80" s="12"/>
-      <c r="D80" s="11"/>
-      <c r="E80" s="11"/>
+      <c r="C80" s="13"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C81" s="12"/>
-      <c r="D81" s="11"/>
-      <c r="E81" s="11"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="12"/>
+      <c r="E81" s="12"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C82" s="12"/>
-      <c r="D82" s="11"/>
-      <c r="E82" s="11"/>
+      <c r="C82" s="13"/>
+      <c r="D82" s="12"/>
+      <c r="E82" s="12"/>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C83" s="12"/>
-      <c r="D83" s="11"/>
-      <c r="E83" s="11"/>
+      <c r="C83" s="13"/>
+      <c r="D83" s="12"/>
+      <c r="E83" s="12"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C84" s="12"/>
-      <c r="D84" s="11"/>
-      <c r="E84" s="11"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="12"/>
+      <c r="E84" s="12"/>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C85" s="12"/>
-      <c r="D85" s="11"/>
-      <c r="E85" s="11"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="12"/>
+      <c r="E85" s="12"/>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C86" s="12"/>
-      <c r="D86" s="11"/>
-      <c r="E86" s="11"/>
+      <c r="C86" s="13"/>
+      <c r="D86" s="12"/>
+      <c r="E86" s="12"/>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C87" s="12"/>
-      <c r="D87" s="11"/>
-      <c r="E87" s="11"/>
+      <c r="C87" s="13"/>
+      <c r="D87" s="12"/>
+      <c r="E87" s="12"/>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C88" s="12"/>
-      <c r="D88" s="11"/>
-      <c r="E88" s="11"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="12"/>
+      <c r="E88" s="12"/>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C89" s="12"/>
-      <c r="D89" s="11"/>
-      <c r="E89" s="11"/>
+      <c r="C89" s="13"/>
+      <c r="D89" s="12"/>
+      <c r="E89" s="12"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C90" s="12"/>
-      <c r="D90" s="11"/>
-      <c r="E90" s="11"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="12"/>
+      <c r="E90" s="12"/>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C91" s="12"/>
-      <c r="D91" s="11"/>
-      <c r="E91" s="11"/>
+      <c r="C91" s="13"/>
+      <c r="D91" s="12"/>
+      <c r="E91" s="12"/>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C92" s="12"/>
-      <c r="D92" s="11"/>
-      <c r="E92" s="11"/>
+      <c r="C92" s="13"/>
+      <c r="D92" s="12"/>
+      <c r="E92" s="12"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C93" s="12"/>
-      <c r="D93" s="11"/>
-      <c r="E93" s="11"/>
+      <c r="C93" s="13"/>
+      <c r="D93" s="12"/>
+      <c r="E93" s="12"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C94" s="12"/>
-      <c r="D94" s="11"/>
-      <c r="E94" s="11"/>
+      <c r="C94" s="13"/>
+      <c r="D94" s="12"/>
+      <c r="E94" s="12"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C95" s="12"/>
-      <c r="D95" s="11"/>
-      <c r="E95" s="11"/>
+      <c r="C95" s="13"/>
+      <c r="D95" s="12"/>
+      <c r="E95" s="12"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C96" s="12"/>
-      <c r="D96" s="11"/>
-      <c r="E96" s="11"/>
+      <c r="C96" s="13"/>
+      <c r="D96" s="12"/>
+      <c r="E96" s="12"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C97" s="12"/>
-      <c r="D97" s="11"/>
-      <c r="E97" s="11"/>
+      <c r="C97" s="13"/>
+      <c r="D97" s="12"/>
+      <c r="E97" s="12"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C98" s="12"/>
-      <c r="D98" s="11"/>
-      <c r="E98" s="11"/>
+      <c r="C98" s="13"/>
+      <c r="D98" s="12"/>
+      <c r="E98" s="12"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C99" s="12"/>
-      <c r="D99" s="11"/>
-      <c r="E99" s="11"/>
+      <c r="C99" s="13"/>
+      <c r="D99" s="12"/>
+      <c r="E99" s="12"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C100" s="12"/>
-      <c r="D100" s="11"/>
-      <c r="E100" s="11"/>
+      <c r="C100" s="13"/>
+      <c r="D100" s="12"/>
+      <c r="E100" s="12"/>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C101" s="12"/>
-      <c r="D101" s="11"/>
-      <c r="E101" s="11"/>
+      <c r="C101" s="13"/>
+      <c r="D101" s="12"/>
+      <c r="E101" s="12"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C102" s="12"/>
-      <c r="D102" s="11"/>
-      <c r="E102" s="11"/>
+      <c r="C102" s="13"/>
+      <c r="D102" s="12"/>
+      <c r="E102" s="12"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C103" s="12"/>
-      <c r="D103" s="11"/>
-      <c r="E103" s="11"/>
+      <c r="C103" s="13"/>
+      <c r="D103" s="12"/>
+      <c r="E103" s="12"/>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C104" s="12"/>
-      <c r="D104" s="11"/>
-      <c r="E104" s="11"/>
+      <c r="C104" s="13"/>
+      <c r="D104" s="12"/>
+      <c r="E104" s="12"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C105" s="12"/>
-      <c r="D105" s="11"/>
-      <c r="E105" s="11"/>
+      <c r="C105" s="13"/>
+      <c r="D105" s="12"/>
+      <c r="E105" s="12"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C106" s="12"/>
-      <c r="D106" s="11"/>
-      <c r="E106" s="11"/>
+      <c r="C106" s="13"/>
+      <c r="D106" s="12"/>
+      <c r="E106" s="12"/>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C107" s="12"/>
-      <c r="D107" s="11"/>
-      <c r="E107" s="11"/>
+      <c r="C107" s="13"/>
+      <c r="D107" s="12"/>
+      <c r="E107" s="12"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C108" s="12"/>
-      <c r="D108" s="11"/>
-      <c r="E108" s="11"/>
+      <c r="C108" s="13"/>
+      <c r="D108" s="12"/>
+      <c r="E108" s="12"/>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C109" s="12"/>
-      <c r="D109" s="11"/>
-      <c r="E109" s="11"/>
+      <c r="C109" s="13"/>
+      <c r="D109" s="12"/>
+      <c r="E109" s="12"/>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C110" s="12"/>
-      <c r="D110" s="11"/>
-      <c r="E110" s="11"/>
+      <c r="C110" s="13"/>
+      <c r="D110" s="12"/>
+      <c r="E110" s="12"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C111" s="12"/>
-      <c r="D111" s="11"/>
-      <c r="E111" s="11"/>
+      <c r="C111" s="13"/>
+      <c r="D111" s="12"/>
+      <c r="E111" s="12"/>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C112" s="12"/>
-      <c r="D112" s="11"/>
-      <c r="E112" s="11"/>
+      <c r="C112" s="13"/>
+      <c r="D112" s="12"/>
+      <c r="E112" s="12"/>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C113" s="12"/>
-      <c r="D113" s="11"/>
-      <c r="E113" s="11"/>
+      <c r="C113" s="13"/>
+      <c r="D113" s="12"/>
+      <c r="E113" s="12"/>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C114" s="12"/>
-      <c r="D114" s="11"/>
-      <c r="E114" s="11"/>
+      <c r="C114" s="13"/>
+      <c r="D114" s="12"/>
+      <c r="E114" s="12"/>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C115" s="12"/>
-      <c r="D115" s="11"/>
-      <c r="E115" s="11"/>
+      <c r="C115" s="13"/>
+      <c r="D115" s="12"/>
+      <c r="E115" s="12"/>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C116" s="12"/>
-      <c r="D116" s="11"/>
-      <c r="E116" s="11"/>
+      <c r="C116" s="13"/>
+      <c r="D116" s="12"/>
+      <c r="E116" s="12"/>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C117" s="12"/>
-      <c r="D117" s="11"/>
-      <c r="E117" s="11"/>
+      <c r="C117" s="13"/>
+      <c r="D117" s="12"/>
+      <c r="E117" s="12"/>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C118" s="12"/>
-      <c r="D118" s="11"/>
-      <c r="E118" s="11"/>
+      <c r="C118" s="13"/>
+      <c r="D118" s="12"/>
+      <c r="E118" s="12"/>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C119" s="12"/>
-      <c r="D119" s="11"/>
-      <c r="E119" s="11"/>
+      <c r="C119" s="13"/>
+      <c r="D119" s="12"/>
+      <c r="E119" s="12"/>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C120" s="12"/>
-      <c r="D120" s="11"/>
-      <c r="E120" s="11"/>
+      <c r="C120" s="13"/>
+      <c r="D120" s="12"/>
+      <c r="E120" s="12"/>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C121" s="12"/>
-      <c r="D121" s="11"/>
-      <c r="E121" s="11"/>
+      <c r="C121" s="13"/>
+      <c r="D121" s="12"/>
+      <c r="E121" s="12"/>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C122" s="12"/>
-      <c r="D122" s="11"/>
-      <c r="E122" s="11"/>
+      <c r="C122" s="13"/>
+      <c r="D122" s="12"/>
+      <c r="E122" s="12"/>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C123" s="12"/>
-      <c r="D123" s="11"/>
-      <c r="E123" s="11"/>
+      <c r="C123" s="13"/>
+      <c r="D123" s="12"/>
+      <c r="E123" s="12"/>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C124" s="12"/>
-      <c r="D124" s="11"/>
-      <c r="E124" s="11"/>
+      <c r="C124" s="13"/>
+      <c r="D124" s="12"/>
+      <c r="E124" s="12"/>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C125" s="12"/>
-      <c r="D125" s="11"/>
-      <c r="E125" s="11"/>
+      <c r="C125" s="13"/>
+      <c r="D125" s="12"/>
+      <c r="E125" s="12"/>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C126" s="12"/>
-      <c r="D126" s="11"/>
-      <c r="E126" s="11"/>
+      <c r="C126" s="13"/>
+      <c r="D126" s="12"/>
+      <c r="E126" s="12"/>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C127" s="12"/>
-      <c r="D127" s="11"/>
-      <c r="E127" s="11"/>
+      <c r="C127" s="13"/>
+      <c r="D127" s="12"/>
+      <c r="E127" s="12"/>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C128" s="12"/>
-      <c r="D128" s="11"/>
-      <c r="E128" s="11"/>
+      <c r="C128" s="13"/>
+      <c r="D128" s="12"/>
+      <c r="E128" s="12"/>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C129" s="12"/>
-      <c r="D129" s="11"/>
-      <c r="E129" s="11"/>
+      <c r="C129" s="13"/>
+      <c r="D129" s="12"/>
+      <c r="E129" s="12"/>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C130" s="12"/>
-      <c r="D130" s="11"/>
-      <c r="E130" s="11"/>
+      <c r="C130" s="13"/>
+      <c r="D130" s="12"/>
+      <c r="E130" s="12"/>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C131" s="12"/>
-      <c r="D131" s="11"/>
-      <c r="E131" s="11"/>
+      <c r="C131" s="13"/>
+      <c r="D131" s="12"/>
+      <c r="E131" s="12"/>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C132" s="12"/>
-      <c r="D132" s="11"/>
-      <c r="E132" s="11"/>
+      <c r="C132" s="13"/>
+      <c r="D132" s="12"/>
+      <c r="E132" s="12"/>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C133" s="12"/>
-      <c r="D133" s="11"/>
-      <c r="E133" s="11"/>
+      <c r="C133" s="13"/>
+      <c r="D133" s="12"/>
+      <c r="E133" s="12"/>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C134" s="12"/>
-      <c r="D134" s="11"/>
-      <c r="E134" s="11"/>
+      <c r="C134" s="13"/>
+      <c r="D134" s="12"/>
+      <c r="E134" s="12"/>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C135" s="12"/>
-      <c r="D135" s="11"/>
-      <c r="E135" s="11"/>
+      <c r="C135" s="13"/>
+      <c r="D135" s="12"/>
+      <c r="E135" s="12"/>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C136" s="12"/>
-      <c r="D136" s="11"/>
-      <c r="E136" s="11"/>
+      <c r="C136" s="13"/>
+      <c r="D136" s="12"/>
+      <c r="E136" s="12"/>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C137" s="12"/>
-      <c r="D137" s="11"/>
-      <c r="E137" s="11"/>
+      <c r="C137" s="13"/>
+      <c r="D137" s="12"/>
+      <c r="E137" s="12"/>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C138" s="12"/>
-      <c r="D138" s="11"/>
-      <c r="E138" s="11"/>
+      <c r="C138" s="13"/>
+      <c r="D138" s="12"/>
+      <c r="E138" s="12"/>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C139" s="12"/>
-      <c r="D139" s="11"/>
-      <c r="E139" s="11"/>
+      <c r="C139" s="13"/>
+      <c r="D139" s="12"/>
+      <c r="E139" s="12"/>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C140" s="12"/>
-      <c r="D140" s="11"/>
-      <c r="E140" s="11"/>
+      <c r="C140" s="13"/>
+      <c r="D140" s="12"/>
+      <c r="E140" s="12"/>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C141" s="12"/>
-      <c r="D141" s="11"/>
-      <c r="E141" s="11"/>
+      <c r="C141" s="13"/>
+      <c r="D141" s="12"/>
+      <c r="E141" s="12"/>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C142" s="12"/>
-      <c r="D142" s="11"/>
-      <c r="E142" s="11"/>
+      <c r="C142" s="13"/>
+      <c r="D142" s="12"/>
+      <c r="E142" s="12"/>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C143" s="12"/>
-      <c r="D143" s="11"/>
-      <c r="E143" s="11"/>
+      <c r="C143" s="13"/>
+      <c r="D143" s="12"/>
+      <c r="E143" s="12"/>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C144" s="12"/>
-      <c r="D144" s="11"/>
-      <c r="E144" s="11"/>
+      <c r="C144" s="13"/>
+      <c r="D144" s="12"/>
+      <c r="E144" s="12"/>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C145" s="12"/>
-      <c r="D145" s="11"/>
-      <c r="E145" s="11"/>
+      <c r="C145" s="13"/>
+      <c r="D145" s="12"/>
+      <c r="E145" s="12"/>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C146" s="12"/>
-      <c r="D146" s="11"/>
-      <c r="E146" s="11"/>
+      <c r="C146" s="13"/>
+      <c r="D146" s="12"/>
+      <c r="E146" s="12"/>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C147" s="12"/>
-      <c r="D147" s="11"/>
-      <c r="E147" s="11"/>
+      <c r="C147" s="13"/>
+      <c r="D147" s="12"/>
+      <c r="E147" s="12"/>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C148" s="12"/>
-      <c r="D148" s="11"/>
-      <c r="E148" s="11"/>
+      <c r="C148" s="13"/>
+      <c r="D148" s="12"/>
+      <c r="E148" s="12"/>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C149" s="12"/>
-      <c r="D149" s="11"/>
-      <c r="E149" s="11"/>
+      <c r="C149" s="13"/>
+      <c r="D149" s="12"/>
+      <c r="E149" s="12"/>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C150" s="12"/>
-      <c r="D150" s="11"/>
-      <c r="E150" s="11"/>
+      <c r="C150" s="13"/>
+      <c r="D150" s="12"/>
+      <c r="E150" s="12"/>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C151" s="12"/>
-      <c r="D151" s="11"/>
-      <c r="E151" s="11"/>
+      <c r="C151" s="13"/>
+      <c r="D151" s="12"/>
+      <c r="E151" s="12"/>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C152" s="12"/>
-      <c r="D152" s="11"/>
-      <c r="E152" s="11"/>
+      <c r="C152" s="13"/>
+      <c r="D152" s="12"/>
+      <c r="E152" s="12"/>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C153" s="12"/>
-      <c r="D153" s="11"/>
-      <c r="E153" s="11"/>
+      <c r="C153" s="13"/>
+      <c r="D153" s="12"/>
+      <c r="E153" s="12"/>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C154" s="12"/>
-      <c r="D154" s="11"/>
-      <c r="E154" s="11"/>
+      <c r="C154" s="13"/>
+      <c r="D154" s="12"/>
+      <c r="E154" s="12"/>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C155" s="12"/>
-      <c r="D155" s="11"/>
-      <c r="E155" s="11"/>
+      <c r="C155" s="13"/>
+      <c r="D155" s="12"/>
+      <c r="E155" s="12"/>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C156" s="12"/>
-      <c r="D156" s="11"/>
-      <c r="E156" s="11"/>
+      <c r="C156" s="13"/>
+      <c r="D156" s="12"/>
+      <c r="E156" s="12"/>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C157" s="12"/>
-      <c r="D157" s="11"/>
-      <c r="E157" s="11"/>
+      <c r="C157" s="13"/>
+      <c r="D157" s="12"/>
+      <c r="E157" s="12"/>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C158" s="12"/>
-      <c r="D158" s="11"/>
-      <c r="E158" s="11"/>
+      <c r="C158" s="13"/>
+      <c r="D158" s="12"/>
+      <c r="E158" s="12"/>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C159" s="12"/>
-      <c r="D159" s="11"/>
-      <c r="E159" s="11"/>
+      <c r="C159" s="13"/>
+      <c r="D159" s="12"/>
+      <c r="E159" s="12"/>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C160" s="12"/>
-      <c r="D160" s="11"/>
-      <c r="E160" s="11"/>
+      <c r="C160" s="13"/>
+      <c r="D160" s="12"/>
+      <c r="E160" s="12"/>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C161" s="12"/>
-      <c r="D161" s="11"/>
-      <c r="E161" s="11"/>
+      <c r="C161" s="13"/>
+      <c r="D161" s="12"/>
+      <c r="E161" s="12"/>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C162" s="12"/>
-      <c r="D162" s="11"/>
-      <c r="E162" s="11"/>
+      <c r="C162" s="13"/>
+      <c r="D162" s="12"/>
+      <c r="E162" s="12"/>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C163" s="12"/>
-      <c r="D163" s="11"/>
-      <c r="E163" s="11"/>
+      <c r="C163" s="13"/>
+      <c r="D163" s="12"/>
+      <c r="E163" s="12"/>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C164" s="12"/>
-      <c r="D164" s="11"/>
-      <c r="E164" s="11"/>
+      <c r="C164" s="13"/>
+      <c r="D164" s="12"/>
+      <c r="E164" s="12"/>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C165" s="12"/>
-      <c r="D165" s="11"/>
-      <c r="E165" s="11"/>
+      <c r="C165" s="13"/>
+      <c r="D165" s="12"/>
+      <c r="E165" s="12"/>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C166" s="12"/>
-      <c r="D166" s="11"/>
-      <c r="E166" s="11"/>
+      <c r="C166" s="13"/>
+      <c r="D166" s="12"/>
+      <c r="E166" s="12"/>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C167" s="12"/>
-      <c r="D167" s="11"/>
-      <c r="E167" s="11"/>
+      <c r="C167" s="13"/>
+      <c r="D167" s="12"/>
+      <c r="E167" s="12"/>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C168" s="12"/>
-      <c r="D168" s="11"/>
-      <c r="E168" s="11"/>
+      <c r="C168" s="13"/>
+      <c r="D168" s="12"/>
+      <c r="E168" s="12"/>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C169" s="12"/>
-      <c r="D169" s="11"/>
-      <c r="E169" s="11"/>
+      <c r="C169" s="13"/>
+      <c r="D169" s="12"/>
+      <c r="E169" s="12"/>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C170" s="12"/>
-      <c r="D170" s="11"/>
-      <c r="E170" s="11"/>
+      <c r="C170" s="13"/>
+      <c r="D170" s="12"/>
+      <c r="E170" s="12"/>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C171" s="12"/>
-      <c r="D171" s="11"/>
-      <c r="E171" s="11"/>
+      <c r="C171" s="13"/>
+      <c r="D171" s="12"/>
+      <c r="E171" s="12"/>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C172" s="12"/>
-      <c r="D172" s="11"/>
-      <c r="E172" s="11"/>
+      <c r="C172" s="13"/>
+      <c r="D172" s="12"/>
+      <c r="E172" s="12"/>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C173" s="12"/>
-      <c r="D173" s="11"/>
-      <c r="E173" s="11"/>
+      <c r="C173" s="13"/>
+      <c r="D173" s="12"/>
+      <c r="E173" s="12"/>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E174" s="11"/>
+      <c r="E174" s="12"/>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E175" s="11"/>
+      <c r="E175" s="12"/>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E176" s="11"/>
+      <c r="E176" s="12"/>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Transfer project improvements (#926)
* Remove Psc received from Project Transfer

* Add transferred_from on project

* Add annex groups in clusters and use in odsodp

* Add merge migration

* Labels for projects created through transfer

* Filter blends and substances by project id

---------

Co-authored-by: dana-cfc4 <dana.comiselu4@gmail.com>
</commit_message>
<xml_diff>
--- a/core/import_data/resources/projects_v2/project_clusters_06_05_2025.xlsx
+++ b/core/import_data/resources/projects_v2/project_clusters_06_05_2025.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="87">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -43,6 +43,9 @@
     <t xml:space="preserve">Old name</t>
   </si>
   <si>
+    <t xml:space="preserve">Annex groups</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kigali Implementation Plan Stage 1</t>
   </si>
   <si>
@@ -56,6 +59,9 @@
   </si>
   <si>
     <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
   </si>
   <si>
     <t xml:space="preserve">Kigali Implementation Plan Stage 2</t>
@@ -95,6 +101,9 @@
   </si>
   <si>
     <t xml:space="preserve">HPMP1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C/I</t>
   </si>
   <si>
     <t xml:space="preserve">HCFC phase-out management plan stage 2</t>
@@ -176,6 +185,9 @@
   </si>
   <si>
     <t xml:space="preserve">DISP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C/I,F</t>
   </si>
   <si>
     <t xml:space="preserve">CFC Individual</t>
@@ -279,7 +291,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -340,6 +352,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="0"/>
@@ -357,23 +375,11 @@
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -467,11 +473,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -483,27 +493,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -519,7 +525,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -775,8 +781,8 @@
   </sheetPr>
   <dimension ref="A1:WU1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -784,10 +790,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="49.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="25.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="21.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.8"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.04"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -812,7 +818,9 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6"/>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -834,250 +842,286 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>11</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
+      <c r="H3" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
+      <c r="H4" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
+      <c r="H5" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
+      <c r="H6" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
+      <c r="H7" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
+      <c r="H8" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
+      <c r="H9" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
+      <c r="H10" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
+      <c r="H11" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
+      <c r="H13" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
+      <c r="H14" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1641,22 +1685,25 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
+      <c r="H15" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -2220,22 +2267,25 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
+      <c r="H16" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -2799,22 +2849,25 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
+      <c r="H17" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -3429,25 +3482,25 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -4063,22 +4116,25 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
+      <c r="H19" s="9" t="s">
+        <v>55</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -4693,20 +4749,20 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G20" s="3"/>
       <c r="I20" s="1"/>
@@ -4727,616 +4783,616 @@
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
-      <c r="AA20" s="9"/>
-      <c r="AB20" s="9"/>
-      <c r="AC20" s="9"/>
-      <c r="AD20" s="9"/>
-      <c r="AE20" s="9"/>
-      <c r="AF20" s="9"/>
-      <c r="AG20" s="9"/>
-      <c r="AH20" s="9"/>
-      <c r="AI20" s="9"/>
-      <c r="AJ20" s="9"/>
-      <c r="AK20" s="9"/>
-      <c r="AL20" s="9"/>
-      <c r="AM20" s="9"/>
-      <c r="AN20" s="9"/>
-      <c r="AO20" s="9"/>
-      <c r="AP20" s="9"/>
-      <c r="AQ20" s="9"/>
-      <c r="AR20" s="9"/>
-      <c r="AS20" s="9"/>
-      <c r="AT20" s="9"/>
-      <c r="AU20" s="9"/>
-      <c r="AV20" s="9"/>
-      <c r="AW20" s="9"/>
-      <c r="AX20" s="9"/>
-      <c r="AY20" s="9"/>
-      <c r="AZ20" s="9"/>
-      <c r="BA20" s="9"/>
-      <c r="BB20" s="9"/>
-      <c r="BC20" s="9"/>
-      <c r="BD20" s="9"/>
-      <c r="BE20" s="9"/>
-      <c r="BF20" s="9"/>
-      <c r="BG20" s="9"/>
-      <c r="BH20" s="9"/>
-      <c r="BI20" s="9"/>
-      <c r="BJ20" s="9"/>
-      <c r="BK20" s="9"/>
-      <c r="BL20" s="9"/>
-      <c r="BM20" s="9"/>
-      <c r="BN20" s="9"/>
-      <c r="BO20" s="9"/>
-      <c r="BP20" s="9"/>
-      <c r="BQ20" s="9"/>
-      <c r="BR20" s="9"/>
-      <c r="BS20" s="9"/>
-      <c r="BT20" s="9"/>
-      <c r="BU20" s="9"/>
-      <c r="BV20" s="9"/>
-      <c r="BW20" s="9"/>
-      <c r="BX20" s="9"/>
-      <c r="BY20" s="9"/>
-      <c r="BZ20" s="9"/>
-      <c r="CA20" s="9"/>
-      <c r="CB20" s="9"/>
-      <c r="CC20" s="9"/>
-      <c r="CD20" s="9"/>
-      <c r="CE20" s="9"/>
-      <c r="CF20" s="9"/>
-      <c r="CG20" s="9"/>
-      <c r="CH20" s="9"/>
-      <c r="CI20" s="9"/>
-      <c r="CJ20" s="9"/>
-      <c r="CK20" s="9"/>
-      <c r="CL20" s="9"/>
-      <c r="CM20" s="9"/>
-      <c r="CN20" s="9"/>
-      <c r="CO20" s="9"/>
-      <c r="CP20" s="9"/>
-      <c r="CQ20" s="9"/>
-      <c r="CR20" s="9"/>
-      <c r="CS20" s="9"/>
-      <c r="CT20" s="9"/>
-      <c r="CU20" s="9"/>
-      <c r="CV20" s="9"/>
-      <c r="CW20" s="9"/>
-      <c r="CX20" s="9"/>
-      <c r="CY20" s="9"/>
-      <c r="CZ20" s="9"/>
-      <c r="DA20" s="9"/>
-      <c r="DB20" s="9"/>
-      <c r="DC20" s="9"/>
-      <c r="DD20" s="9"/>
-      <c r="DE20" s="9"/>
-      <c r="DF20" s="9"/>
-      <c r="DG20" s="9"/>
-      <c r="DH20" s="9"/>
-      <c r="DI20" s="9"/>
-      <c r="DJ20" s="9"/>
-      <c r="DK20" s="9"/>
-      <c r="DL20" s="9"/>
-      <c r="DM20" s="9"/>
-      <c r="DN20" s="9"/>
-      <c r="DO20" s="9"/>
-      <c r="DP20" s="9"/>
-      <c r="DQ20" s="9"/>
-      <c r="DR20" s="9"/>
-      <c r="DS20" s="9"/>
-      <c r="DT20" s="9"/>
-      <c r="DU20" s="9"/>
-      <c r="DV20" s="9"/>
-      <c r="DW20" s="9"/>
-      <c r="DX20" s="9"/>
-      <c r="DY20" s="9"/>
-      <c r="DZ20" s="9"/>
-      <c r="EA20" s="9"/>
-      <c r="EB20" s="9"/>
-      <c r="EC20" s="9"/>
-      <c r="ED20" s="9"/>
-      <c r="EE20" s="9"/>
-      <c r="EF20" s="9"/>
-      <c r="EG20" s="9"/>
-      <c r="EH20" s="9"/>
-      <c r="EI20" s="9"/>
-      <c r="EJ20" s="9"/>
-      <c r="EK20" s="9"/>
-      <c r="EL20" s="9"/>
-      <c r="EM20" s="9"/>
-      <c r="EN20" s="9"/>
-      <c r="EO20" s="9"/>
-      <c r="EP20" s="9"/>
-      <c r="EQ20" s="9"/>
-      <c r="ER20" s="9"/>
-      <c r="ES20" s="9"/>
-      <c r="ET20" s="9"/>
-      <c r="EU20" s="9"/>
-      <c r="EV20" s="9"/>
-      <c r="EW20" s="9"/>
-      <c r="EX20" s="9"/>
-      <c r="EY20" s="9"/>
-      <c r="EZ20" s="9"/>
-      <c r="FA20" s="9"/>
-      <c r="FB20" s="9"/>
-      <c r="FC20" s="9"/>
-      <c r="FD20" s="9"/>
-      <c r="FE20" s="9"/>
-      <c r="FF20" s="9"/>
-      <c r="FG20" s="9"/>
-      <c r="FH20" s="9"/>
-      <c r="FI20" s="9"/>
-      <c r="FJ20" s="9"/>
-      <c r="FK20" s="9"/>
-      <c r="FL20" s="9"/>
-      <c r="FM20" s="9"/>
-      <c r="FN20" s="9"/>
-      <c r="FO20" s="9"/>
-      <c r="FP20" s="9"/>
-      <c r="FQ20" s="9"/>
-      <c r="FR20" s="9"/>
-      <c r="FS20" s="9"/>
-      <c r="FT20" s="9"/>
-      <c r="FU20" s="9"/>
-      <c r="FV20" s="9"/>
-      <c r="FW20" s="9"/>
-      <c r="FX20" s="9"/>
-      <c r="FY20" s="9"/>
-      <c r="FZ20" s="9"/>
-      <c r="GA20" s="9"/>
-      <c r="GB20" s="9"/>
-      <c r="GC20" s="9"/>
-      <c r="GD20" s="9"/>
-      <c r="GE20" s="9"/>
-      <c r="GF20" s="9"/>
-      <c r="GG20" s="9"/>
-      <c r="GH20" s="9"/>
-      <c r="GI20" s="9"/>
-      <c r="GJ20" s="9"/>
-      <c r="GK20" s="9"/>
-      <c r="GL20" s="9"/>
-      <c r="GM20" s="9"/>
-      <c r="GN20" s="9"/>
-      <c r="GO20" s="9"/>
-      <c r="GP20" s="9"/>
-      <c r="GQ20" s="9"/>
-      <c r="GR20" s="9"/>
-      <c r="GS20" s="9"/>
-      <c r="GT20" s="9"/>
-      <c r="GU20" s="9"/>
-      <c r="GV20" s="9"/>
-      <c r="GW20" s="9"/>
-      <c r="GX20" s="9"/>
-      <c r="GY20" s="9"/>
-      <c r="GZ20" s="9"/>
-      <c r="HA20" s="9"/>
-      <c r="HB20" s="9"/>
-      <c r="HC20" s="9"/>
-      <c r="HD20" s="9"/>
-      <c r="HE20" s="9"/>
-      <c r="HF20" s="9"/>
-      <c r="HG20" s="9"/>
-      <c r="HH20" s="9"/>
-      <c r="HI20" s="9"/>
-      <c r="HJ20" s="9"/>
-      <c r="HK20" s="9"/>
-      <c r="HL20" s="9"/>
-      <c r="HM20" s="9"/>
-      <c r="HN20" s="9"/>
-      <c r="HO20" s="9"/>
-      <c r="HP20" s="9"/>
-      <c r="HQ20" s="9"/>
-      <c r="HR20" s="9"/>
-      <c r="HS20" s="9"/>
-      <c r="HT20" s="9"/>
-      <c r="HU20" s="9"/>
-      <c r="HV20" s="9"/>
-      <c r="HW20" s="9"/>
-      <c r="HX20" s="9"/>
-      <c r="HY20" s="9"/>
-      <c r="HZ20" s="9"/>
-      <c r="IA20" s="9"/>
-      <c r="IB20" s="9"/>
-      <c r="IC20" s="9"/>
-      <c r="ID20" s="9"/>
-      <c r="IE20" s="9"/>
-      <c r="IF20" s="9"/>
-      <c r="IG20" s="9"/>
-      <c r="IH20" s="9"/>
-      <c r="II20" s="9"/>
-      <c r="IJ20" s="9"/>
-      <c r="IK20" s="9"/>
-      <c r="IL20" s="9"/>
-      <c r="IM20" s="9"/>
-      <c r="IN20" s="9"/>
-      <c r="IO20" s="9"/>
-      <c r="IP20" s="9"/>
-      <c r="IQ20" s="9"/>
-      <c r="IR20" s="9"/>
-      <c r="IS20" s="9"/>
-      <c r="IT20" s="9"/>
-      <c r="IU20" s="9"/>
-      <c r="IV20" s="9"/>
-      <c r="IW20" s="9"/>
-      <c r="IX20" s="9"/>
-      <c r="IY20" s="9"/>
-      <c r="IZ20" s="9"/>
-      <c r="JA20" s="9"/>
-      <c r="JB20" s="9"/>
-      <c r="JC20" s="9"/>
-      <c r="JD20" s="9"/>
-      <c r="JE20" s="9"/>
-      <c r="JF20" s="9"/>
-      <c r="JG20" s="9"/>
-      <c r="JH20" s="9"/>
-      <c r="JI20" s="9"/>
-      <c r="JJ20" s="9"/>
-      <c r="JK20" s="9"/>
-      <c r="JL20" s="9"/>
-      <c r="JM20" s="9"/>
-      <c r="JN20" s="9"/>
-      <c r="JO20" s="9"/>
-      <c r="JP20" s="9"/>
-      <c r="JQ20" s="9"/>
-      <c r="JR20" s="9"/>
-      <c r="JS20" s="9"/>
-      <c r="JT20" s="9"/>
-      <c r="JU20" s="9"/>
-      <c r="JV20" s="9"/>
-      <c r="JW20" s="9"/>
-      <c r="JX20" s="9"/>
-      <c r="JY20" s="9"/>
-      <c r="JZ20" s="9"/>
-      <c r="KA20" s="9"/>
-      <c r="KB20" s="9"/>
-      <c r="KC20" s="9"/>
-      <c r="KD20" s="9"/>
-      <c r="KE20" s="9"/>
-      <c r="KF20" s="9"/>
-      <c r="KG20" s="9"/>
-      <c r="KH20" s="9"/>
-      <c r="KI20" s="9"/>
-      <c r="KJ20" s="9"/>
-      <c r="KK20" s="9"/>
-      <c r="KL20" s="9"/>
-      <c r="KM20" s="9"/>
-      <c r="KN20" s="9"/>
-      <c r="KO20" s="9"/>
-      <c r="KP20" s="9"/>
-      <c r="KQ20" s="9"/>
-      <c r="KR20" s="9"/>
-      <c r="KS20" s="9"/>
-      <c r="KT20" s="9"/>
-      <c r="KU20" s="9"/>
-      <c r="KV20" s="9"/>
-      <c r="KW20" s="9"/>
-      <c r="KX20" s="9"/>
-      <c r="KY20" s="9"/>
-      <c r="KZ20" s="9"/>
-      <c r="LA20" s="9"/>
-      <c r="LB20" s="9"/>
-      <c r="LC20" s="9"/>
-      <c r="LD20" s="9"/>
-      <c r="LE20" s="9"/>
-      <c r="LF20" s="9"/>
-      <c r="LG20" s="9"/>
-      <c r="LH20" s="9"/>
-      <c r="LI20" s="9"/>
-      <c r="LJ20" s="9"/>
-      <c r="LK20" s="9"/>
-      <c r="LL20" s="9"/>
-      <c r="LM20" s="9"/>
-      <c r="LN20" s="9"/>
-      <c r="LO20" s="9"/>
-      <c r="LP20" s="9"/>
-      <c r="LQ20" s="9"/>
-      <c r="LR20" s="9"/>
-      <c r="LS20" s="9"/>
-      <c r="LT20" s="9"/>
-      <c r="LU20" s="9"/>
-      <c r="LV20" s="9"/>
-      <c r="LW20" s="9"/>
-      <c r="LX20" s="9"/>
-      <c r="LY20" s="9"/>
-      <c r="LZ20" s="9"/>
-      <c r="MA20" s="9"/>
-      <c r="MB20" s="9"/>
-      <c r="MC20" s="9"/>
-      <c r="MD20" s="9"/>
-      <c r="ME20" s="9"/>
-      <c r="MF20" s="9"/>
-      <c r="MG20" s="9"/>
-      <c r="MH20" s="9"/>
-      <c r="MI20" s="9"/>
-      <c r="MJ20" s="9"/>
-      <c r="MK20" s="9"/>
-      <c r="ML20" s="9"/>
-      <c r="MM20" s="9"/>
-      <c r="MN20" s="9"/>
-      <c r="MO20" s="9"/>
-      <c r="MP20" s="9"/>
-      <c r="MQ20" s="9"/>
-      <c r="MR20" s="9"/>
-      <c r="MS20" s="9"/>
-      <c r="MT20" s="9"/>
-      <c r="MU20" s="9"/>
-      <c r="MV20" s="9"/>
-      <c r="MW20" s="9"/>
-      <c r="MX20" s="9"/>
-      <c r="MY20" s="9"/>
-      <c r="MZ20" s="9"/>
-      <c r="NA20" s="9"/>
-      <c r="NB20" s="9"/>
-      <c r="NC20" s="9"/>
-      <c r="ND20" s="9"/>
-      <c r="NE20" s="9"/>
-      <c r="NF20" s="9"/>
-      <c r="NG20" s="9"/>
-      <c r="NH20" s="9"/>
-      <c r="NI20" s="9"/>
-      <c r="NJ20" s="9"/>
-      <c r="NK20" s="9"/>
-      <c r="NL20" s="9"/>
-      <c r="NM20" s="9"/>
-      <c r="NN20" s="9"/>
-      <c r="NO20" s="9"/>
-      <c r="NP20" s="9"/>
-      <c r="NQ20" s="9"/>
-      <c r="NR20" s="9"/>
-      <c r="NS20" s="9"/>
-      <c r="NT20" s="9"/>
-      <c r="NU20" s="9"/>
-      <c r="NV20" s="9"/>
-      <c r="NW20" s="9"/>
-      <c r="NX20" s="9"/>
-      <c r="NY20" s="9"/>
-      <c r="NZ20" s="9"/>
-      <c r="OA20" s="9"/>
-      <c r="OB20" s="9"/>
-      <c r="OC20" s="9"/>
-      <c r="OD20" s="9"/>
-      <c r="OE20" s="9"/>
-      <c r="OF20" s="9"/>
-      <c r="OG20" s="9"/>
-      <c r="OH20" s="9"/>
-      <c r="OI20" s="9"/>
-      <c r="OJ20" s="9"/>
-      <c r="OK20" s="9"/>
-      <c r="OL20" s="9"/>
-      <c r="OM20" s="9"/>
-      <c r="ON20" s="9"/>
-      <c r="OO20" s="9"/>
-      <c r="OP20" s="9"/>
-      <c r="OQ20" s="9"/>
-      <c r="OR20" s="9"/>
-      <c r="OS20" s="9"/>
-      <c r="OT20" s="9"/>
-      <c r="OU20" s="9"/>
-      <c r="OV20" s="9"/>
-      <c r="OW20" s="9"/>
-      <c r="OX20" s="9"/>
-      <c r="OY20" s="9"/>
-      <c r="OZ20" s="9"/>
-      <c r="PA20" s="9"/>
-      <c r="PB20" s="9"/>
-      <c r="PC20" s="9"/>
-      <c r="PD20" s="9"/>
-      <c r="PE20" s="9"/>
-      <c r="PF20" s="9"/>
-      <c r="PG20" s="9"/>
-      <c r="PH20" s="9"/>
-      <c r="PI20" s="9"/>
-      <c r="PJ20" s="9"/>
-      <c r="PK20" s="9"/>
-      <c r="PL20" s="9"/>
-      <c r="PM20" s="9"/>
-      <c r="PN20" s="9"/>
-      <c r="PO20" s="9"/>
-      <c r="PP20" s="9"/>
-      <c r="PQ20" s="9"/>
-      <c r="PR20" s="9"/>
-      <c r="PS20" s="9"/>
-      <c r="PT20" s="9"/>
-      <c r="PU20" s="9"/>
-      <c r="PV20" s="9"/>
-      <c r="PW20" s="9"/>
-      <c r="PX20" s="9"/>
-      <c r="PY20" s="9"/>
-      <c r="PZ20" s="9"/>
-      <c r="QA20" s="9"/>
-      <c r="QB20" s="9"/>
-      <c r="QC20" s="9"/>
-      <c r="QD20" s="9"/>
-      <c r="QE20" s="9"/>
-      <c r="QF20" s="9"/>
-      <c r="QG20" s="9"/>
-      <c r="QH20" s="9"/>
-      <c r="QI20" s="9"/>
-      <c r="QJ20" s="9"/>
-      <c r="QK20" s="9"/>
-      <c r="QL20" s="9"/>
-      <c r="QM20" s="9"/>
-      <c r="QN20" s="9"/>
-      <c r="QO20" s="9"/>
-      <c r="QP20" s="9"/>
-      <c r="QQ20" s="9"/>
-      <c r="QR20" s="9"/>
-      <c r="QS20" s="9"/>
-      <c r="QT20" s="9"/>
-      <c r="QU20" s="9"/>
-      <c r="QV20" s="9"/>
-      <c r="QW20" s="9"/>
-      <c r="QX20" s="9"/>
-      <c r="QY20" s="9"/>
-      <c r="QZ20" s="9"/>
-      <c r="RA20" s="9"/>
-      <c r="RB20" s="9"/>
-      <c r="RC20" s="9"/>
-      <c r="RD20" s="9"/>
-      <c r="RE20" s="9"/>
-      <c r="RF20" s="9"/>
-      <c r="RG20" s="9"/>
-      <c r="RH20" s="9"/>
-      <c r="RI20" s="9"/>
-      <c r="RJ20" s="9"/>
-      <c r="RK20" s="9"/>
-      <c r="RL20" s="9"/>
-      <c r="RM20" s="9"/>
-      <c r="RN20" s="9"/>
-      <c r="RO20" s="9"/>
-      <c r="RP20" s="9"/>
-      <c r="RQ20" s="9"/>
-      <c r="RR20" s="9"/>
-      <c r="RS20" s="9"/>
-      <c r="RT20" s="9"/>
-      <c r="RU20" s="9"/>
-      <c r="RV20" s="9"/>
-      <c r="RW20" s="9"/>
-      <c r="RX20" s="9"/>
-      <c r="RY20" s="9"/>
-      <c r="RZ20" s="9"/>
-      <c r="SA20" s="9"/>
-      <c r="SB20" s="9"/>
-      <c r="SC20" s="9"/>
-      <c r="SD20" s="9"/>
-      <c r="SE20" s="9"/>
-      <c r="SF20" s="9"/>
-      <c r="SG20" s="9"/>
-      <c r="SH20" s="9"/>
-      <c r="SI20" s="9"/>
-      <c r="SJ20" s="9"/>
-      <c r="SK20" s="9"/>
-      <c r="SL20" s="9"/>
-      <c r="SM20" s="9"/>
-      <c r="SN20" s="9"/>
-      <c r="SO20" s="9"/>
-      <c r="SP20" s="9"/>
-      <c r="SQ20" s="9"/>
-      <c r="SR20" s="9"/>
-      <c r="SS20" s="9"/>
-      <c r="ST20" s="9"/>
-      <c r="SU20" s="9"/>
-      <c r="SV20" s="9"/>
-      <c r="SW20" s="9"/>
-      <c r="SX20" s="9"/>
-      <c r="SY20" s="9"/>
-      <c r="SZ20" s="9"/>
-      <c r="TA20" s="9"/>
-      <c r="TB20" s="9"/>
-      <c r="TC20" s="9"/>
-      <c r="TD20" s="9"/>
-      <c r="TE20" s="9"/>
-      <c r="TF20" s="9"/>
-      <c r="TG20" s="9"/>
-      <c r="TH20" s="9"/>
-      <c r="TI20" s="9"/>
-      <c r="TJ20" s="9"/>
-      <c r="TK20" s="9"/>
-      <c r="TL20" s="9"/>
-      <c r="TM20" s="9"/>
-      <c r="TN20" s="9"/>
-      <c r="TO20" s="9"/>
-      <c r="TP20" s="9"/>
-      <c r="TQ20" s="9"/>
-      <c r="TR20" s="9"/>
-      <c r="TS20" s="9"/>
-      <c r="TT20" s="9"/>
-      <c r="TU20" s="9"/>
-      <c r="TV20" s="9"/>
-      <c r="TW20" s="9"/>
-      <c r="TX20" s="9"/>
-      <c r="TY20" s="9"/>
-      <c r="TZ20" s="9"/>
-      <c r="UA20" s="9"/>
-      <c r="UB20" s="9"/>
-      <c r="UC20" s="9"/>
-      <c r="UD20" s="9"/>
-      <c r="UE20" s="9"/>
-      <c r="UF20" s="9"/>
-      <c r="UG20" s="9"/>
-      <c r="UH20" s="9"/>
-      <c r="UI20" s="9"/>
-      <c r="UJ20" s="9"/>
-      <c r="UK20" s="9"/>
-      <c r="UL20" s="9"/>
-      <c r="UM20" s="9"/>
-      <c r="UN20" s="9"/>
-      <c r="UO20" s="9"/>
-      <c r="UP20" s="9"/>
-      <c r="UQ20" s="9"/>
-      <c r="UR20" s="9"/>
-      <c r="US20" s="9"/>
-      <c r="UT20" s="9"/>
-      <c r="UU20" s="9"/>
-      <c r="UV20" s="9"/>
-      <c r="UW20" s="9"/>
-      <c r="UX20" s="9"/>
-      <c r="UY20" s="9"/>
-      <c r="UZ20" s="9"/>
-      <c r="VA20" s="9"/>
-      <c r="VB20" s="9"/>
-      <c r="VC20" s="9"/>
-      <c r="VD20" s="9"/>
-      <c r="VE20" s="9"/>
-      <c r="VF20" s="9"/>
-      <c r="VG20" s="9"/>
-      <c r="VH20" s="9"/>
-      <c r="VI20" s="9"/>
-      <c r="VJ20" s="9"/>
-      <c r="VK20" s="9"/>
-      <c r="VL20" s="9"/>
-      <c r="VM20" s="9"/>
-      <c r="VN20" s="9"/>
-      <c r="VO20" s="9"/>
-      <c r="VP20" s="9"/>
-      <c r="VQ20" s="9"/>
-      <c r="VR20" s="9"/>
-      <c r="VS20" s="9"/>
-      <c r="VT20" s="9"/>
-      <c r="VU20" s="9"/>
-      <c r="VV20" s="9"/>
-      <c r="VW20" s="9"/>
-      <c r="VX20" s="9"/>
-      <c r="VY20" s="9"/>
-      <c r="VZ20" s="9"/>
-      <c r="WA20" s="9"/>
-      <c r="WB20" s="9"/>
-      <c r="WC20" s="9"/>
-      <c r="WD20" s="9"/>
-      <c r="WE20" s="9"/>
-      <c r="WF20" s="9"/>
-      <c r="WG20" s="9"/>
-      <c r="WH20" s="9"/>
-      <c r="WI20" s="9"/>
-      <c r="WJ20" s="9"/>
-      <c r="WK20" s="9"/>
-      <c r="WL20" s="9"/>
-      <c r="WM20" s="9"/>
-      <c r="WN20" s="9"/>
-      <c r="WO20" s="9"/>
-      <c r="WP20" s="9"/>
-      <c r="WQ20" s="9"/>
-      <c r="WR20" s="9"/>
-      <c r="WS20" s="9"/>
-      <c r="WT20" s="9"/>
-      <c r="WU20" s="9"/>
+      <c r="AA20" s="10"/>
+      <c r="AB20" s="10"/>
+      <c r="AC20" s="10"/>
+      <c r="AD20" s="10"/>
+      <c r="AE20" s="10"/>
+      <c r="AF20" s="10"/>
+      <c r="AG20" s="10"/>
+      <c r="AH20" s="10"/>
+      <c r="AI20" s="10"/>
+      <c r="AJ20" s="10"/>
+      <c r="AK20" s="10"/>
+      <c r="AL20" s="10"/>
+      <c r="AM20" s="10"/>
+      <c r="AN20" s="10"/>
+      <c r="AO20" s="10"/>
+      <c r="AP20" s="10"/>
+      <c r="AQ20" s="10"/>
+      <c r="AR20" s="10"/>
+      <c r="AS20" s="10"/>
+      <c r="AT20" s="10"/>
+      <c r="AU20" s="10"/>
+      <c r="AV20" s="10"/>
+      <c r="AW20" s="10"/>
+      <c r="AX20" s="10"/>
+      <c r="AY20" s="10"/>
+      <c r="AZ20" s="10"/>
+      <c r="BA20" s="10"/>
+      <c r="BB20" s="10"/>
+      <c r="BC20" s="10"/>
+      <c r="BD20" s="10"/>
+      <c r="BE20" s="10"/>
+      <c r="BF20" s="10"/>
+      <c r="BG20" s="10"/>
+      <c r="BH20" s="10"/>
+      <c r="BI20" s="10"/>
+      <c r="BJ20" s="10"/>
+      <c r="BK20" s="10"/>
+      <c r="BL20" s="10"/>
+      <c r="BM20" s="10"/>
+      <c r="BN20" s="10"/>
+      <c r="BO20" s="10"/>
+      <c r="BP20" s="10"/>
+      <c r="BQ20" s="10"/>
+      <c r="BR20" s="10"/>
+      <c r="BS20" s="10"/>
+      <c r="BT20" s="10"/>
+      <c r="BU20" s="10"/>
+      <c r="BV20" s="10"/>
+      <c r="BW20" s="10"/>
+      <c r="BX20" s="10"/>
+      <c r="BY20" s="10"/>
+      <c r="BZ20" s="10"/>
+      <c r="CA20" s="10"/>
+      <c r="CB20" s="10"/>
+      <c r="CC20" s="10"/>
+      <c r="CD20" s="10"/>
+      <c r="CE20" s="10"/>
+      <c r="CF20" s="10"/>
+      <c r="CG20" s="10"/>
+      <c r="CH20" s="10"/>
+      <c r="CI20" s="10"/>
+      <c r="CJ20" s="10"/>
+      <c r="CK20" s="10"/>
+      <c r="CL20" s="10"/>
+      <c r="CM20" s="10"/>
+      <c r="CN20" s="10"/>
+      <c r="CO20" s="10"/>
+      <c r="CP20" s="10"/>
+      <c r="CQ20" s="10"/>
+      <c r="CR20" s="10"/>
+      <c r="CS20" s="10"/>
+      <c r="CT20" s="10"/>
+      <c r="CU20" s="10"/>
+      <c r="CV20" s="10"/>
+      <c r="CW20" s="10"/>
+      <c r="CX20" s="10"/>
+      <c r="CY20" s="10"/>
+      <c r="CZ20" s="10"/>
+      <c r="DA20" s="10"/>
+      <c r="DB20" s="10"/>
+      <c r="DC20" s="10"/>
+      <c r="DD20" s="10"/>
+      <c r="DE20" s="10"/>
+      <c r="DF20" s="10"/>
+      <c r="DG20" s="10"/>
+      <c r="DH20" s="10"/>
+      <c r="DI20" s="10"/>
+      <c r="DJ20" s="10"/>
+      <c r="DK20" s="10"/>
+      <c r="DL20" s="10"/>
+      <c r="DM20" s="10"/>
+      <c r="DN20" s="10"/>
+      <c r="DO20" s="10"/>
+      <c r="DP20" s="10"/>
+      <c r="DQ20" s="10"/>
+      <c r="DR20" s="10"/>
+      <c r="DS20" s="10"/>
+      <c r="DT20" s="10"/>
+      <c r="DU20" s="10"/>
+      <c r="DV20" s="10"/>
+      <c r="DW20" s="10"/>
+      <c r="DX20" s="10"/>
+      <c r="DY20" s="10"/>
+      <c r="DZ20" s="10"/>
+      <c r="EA20" s="10"/>
+      <c r="EB20" s="10"/>
+      <c r="EC20" s="10"/>
+      <c r="ED20" s="10"/>
+      <c r="EE20" s="10"/>
+      <c r="EF20" s="10"/>
+      <c r="EG20" s="10"/>
+      <c r="EH20" s="10"/>
+      <c r="EI20" s="10"/>
+      <c r="EJ20" s="10"/>
+      <c r="EK20" s="10"/>
+      <c r="EL20" s="10"/>
+      <c r="EM20" s="10"/>
+      <c r="EN20" s="10"/>
+      <c r="EO20" s="10"/>
+      <c r="EP20" s="10"/>
+      <c r="EQ20" s="10"/>
+      <c r="ER20" s="10"/>
+      <c r="ES20" s="10"/>
+      <c r="ET20" s="10"/>
+      <c r="EU20" s="10"/>
+      <c r="EV20" s="10"/>
+      <c r="EW20" s="10"/>
+      <c r="EX20" s="10"/>
+      <c r="EY20" s="10"/>
+      <c r="EZ20" s="10"/>
+      <c r="FA20" s="10"/>
+      <c r="FB20" s="10"/>
+      <c r="FC20" s="10"/>
+      <c r="FD20" s="10"/>
+      <c r="FE20" s="10"/>
+      <c r="FF20" s="10"/>
+      <c r="FG20" s="10"/>
+      <c r="FH20" s="10"/>
+      <c r="FI20" s="10"/>
+      <c r="FJ20" s="10"/>
+      <c r="FK20" s="10"/>
+      <c r="FL20" s="10"/>
+      <c r="FM20" s="10"/>
+      <c r="FN20" s="10"/>
+      <c r="FO20" s="10"/>
+      <c r="FP20" s="10"/>
+      <c r="FQ20" s="10"/>
+      <c r="FR20" s="10"/>
+      <c r="FS20" s="10"/>
+      <c r="FT20" s="10"/>
+      <c r="FU20" s="10"/>
+      <c r="FV20" s="10"/>
+      <c r="FW20" s="10"/>
+      <c r="FX20" s="10"/>
+      <c r="FY20" s="10"/>
+      <c r="FZ20" s="10"/>
+      <c r="GA20" s="10"/>
+      <c r="GB20" s="10"/>
+      <c r="GC20" s="10"/>
+      <c r="GD20" s="10"/>
+      <c r="GE20" s="10"/>
+      <c r="GF20" s="10"/>
+      <c r="GG20" s="10"/>
+      <c r="GH20" s="10"/>
+      <c r="GI20" s="10"/>
+      <c r="GJ20" s="10"/>
+      <c r="GK20" s="10"/>
+      <c r="GL20" s="10"/>
+      <c r="GM20" s="10"/>
+      <c r="GN20" s="10"/>
+      <c r="GO20" s="10"/>
+      <c r="GP20" s="10"/>
+      <c r="GQ20" s="10"/>
+      <c r="GR20" s="10"/>
+      <c r="GS20" s="10"/>
+      <c r="GT20" s="10"/>
+      <c r="GU20" s="10"/>
+      <c r="GV20" s="10"/>
+      <c r="GW20" s="10"/>
+      <c r="GX20" s="10"/>
+      <c r="GY20" s="10"/>
+      <c r="GZ20" s="10"/>
+      <c r="HA20" s="10"/>
+      <c r="HB20" s="10"/>
+      <c r="HC20" s="10"/>
+      <c r="HD20" s="10"/>
+      <c r="HE20" s="10"/>
+      <c r="HF20" s="10"/>
+      <c r="HG20" s="10"/>
+      <c r="HH20" s="10"/>
+      <c r="HI20" s="10"/>
+      <c r="HJ20" s="10"/>
+      <c r="HK20" s="10"/>
+      <c r="HL20" s="10"/>
+      <c r="HM20" s="10"/>
+      <c r="HN20" s="10"/>
+      <c r="HO20" s="10"/>
+      <c r="HP20" s="10"/>
+      <c r="HQ20" s="10"/>
+      <c r="HR20" s="10"/>
+      <c r="HS20" s="10"/>
+      <c r="HT20" s="10"/>
+      <c r="HU20" s="10"/>
+      <c r="HV20" s="10"/>
+      <c r="HW20" s="10"/>
+      <c r="HX20" s="10"/>
+      <c r="HY20" s="10"/>
+      <c r="HZ20" s="10"/>
+      <c r="IA20" s="10"/>
+      <c r="IB20" s="10"/>
+      <c r="IC20" s="10"/>
+      <c r="ID20" s="10"/>
+      <c r="IE20" s="10"/>
+      <c r="IF20" s="10"/>
+      <c r="IG20" s="10"/>
+      <c r="IH20" s="10"/>
+      <c r="II20" s="10"/>
+      <c r="IJ20" s="10"/>
+      <c r="IK20" s="10"/>
+      <c r="IL20" s="10"/>
+      <c r="IM20" s="10"/>
+      <c r="IN20" s="10"/>
+      <c r="IO20" s="10"/>
+      <c r="IP20" s="10"/>
+      <c r="IQ20" s="10"/>
+      <c r="IR20" s="10"/>
+      <c r="IS20" s="10"/>
+      <c r="IT20" s="10"/>
+      <c r="IU20" s="10"/>
+      <c r="IV20" s="10"/>
+      <c r="IW20" s="10"/>
+      <c r="IX20" s="10"/>
+      <c r="IY20" s="10"/>
+      <c r="IZ20" s="10"/>
+      <c r="JA20" s="10"/>
+      <c r="JB20" s="10"/>
+      <c r="JC20" s="10"/>
+      <c r="JD20" s="10"/>
+      <c r="JE20" s="10"/>
+      <c r="JF20" s="10"/>
+      <c r="JG20" s="10"/>
+      <c r="JH20" s="10"/>
+      <c r="JI20" s="10"/>
+      <c r="JJ20" s="10"/>
+      <c r="JK20" s="10"/>
+      <c r="JL20" s="10"/>
+      <c r="JM20" s="10"/>
+      <c r="JN20" s="10"/>
+      <c r="JO20" s="10"/>
+      <c r="JP20" s="10"/>
+      <c r="JQ20" s="10"/>
+      <c r="JR20" s="10"/>
+      <c r="JS20" s="10"/>
+      <c r="JT20" s="10"/>
+      <c r="JU20" s="10"/>
+      <c r="JV20" s="10"/>
+      <c r="JW20" s="10"/>
+      <c r="JX20" s="10"/>
+      <c r="JY20" s="10"/>
+      <c r="JZ20" s="10"/>
+      <c r="KA20" s="10"/>
+      <c r="KB20" s="10"/>
+      <c r="KC20" s="10"/>
+      <c r="KD20" s="10"/>
+      <c r="KE20" s="10"/>
+      <c r="KF20" s="10"/>
+      <c r="KG20" s="10"/>
+      <c r="KH20" s="10"/>
+      <c r="KI20" s="10"/>
+      <c r="KJ20" s="10"/>
+      <c r="KK20" s="10"/>
+      <c r="KL20" s="10"/>
+      <c r="KM20" s="10"/>
+      <c r="KN20" s="10"/>
+      <c r="KO20" s="10"/>
+      <c r="KP20" s="10"/>
+      <c r="KQ20" s="10"/>
+      <c r="KR20" s="10"/>
+      <c r="KS20" s="10"/>
+      <c r="KT20" s="10"/>
+      <c r="KU20" s="10"/>
+      <c r="KV20" s="10"/>
+      <c r="KW20" s="10"/>
+      <c r="KX20" s="10"/>
+      <c r="KY20" s="10"/>
+      <c r="KZ20" s="10"/>
+      <c r="LA20" s="10"/>
+      <c r="LB20" s="10"/>
+      <c r="LC20" s="10"/>
+      <c r="LD20" s="10"/>
+      <c r="LE20" s="10"/>
+      <c r="LF20" s="10"/>
+      <c r="LG20" s="10"/>
+      <c r="LH20" s="10"/>
+      <c r="LI20" s="10"/>
+      <c r="LJ20" s="10"/>
+      <c r="LK20" s="10"/>
+      <c r="LL20" s="10"/>
+      <c r="LM20" s="10"/>
+      <c r="LN20" s="10"/>
+      <c r="LO20" s="10"/>
+      <c r="LP20" s="10"/>
+      <c r="LQ20" s="10"/>
+      <c r="LR20" s="10"/>
+      <c r="LS20" s="10"/>
+      <c r="LT20" s="10"/>
+      <c r="LU20" s="10"/>
+      <c r="LV20" s="10"/>
+      <c r="LW20" s="10"/>
+      <c r="LX20" s="10"/>
+      <c r="LY20" s="10"/>
+      <c r="LZ20" s="10"/>
+      <c r="MA20" s="10"/>
+      <c r="MB20" s="10"/>
+      <c r="MC20" s="10"/>
+      <c r="MD20" s="10"/>
+      <c r="ME20" s="10"/>
+      <c r="MF20" s="10"/>
+      <c r="MG20" s="10"/>
+      <c r="MH20" s="10"/>
+      <c r="MI20" s="10"/>
+      <c r="MJ20" s="10"/>
+      <c r="MK20" s="10"/>
+      <c r="ML20" s="10"/>
+      <c r="MM20" s="10"/>
+      <c r="MN20" s="10"/>
+      <c r="MO20" s="10"/>
+      <c r="MP20" s="10"/>
+      <c r="MQ20" s="10"/>
+      <c r="MR20" s="10"/>
+      <c r="MS20" s="10"/>
+      <c r="MT20" s="10"/>
+      <c r="MU20" s="10"/>
+      <c r="MV20" s="10"/>
+      <c r="MW20" s="10"/>
+      <c r="MX20" s="10"/>
+      <c r="MY20" s="10"/>
+      <c r="MZ20" s="10"/>
+      <c r="NA20" s="10"/>
+      <c r="NB20" s="10"/>
+      <c r="NC20" s="10"/>
+      <c r="ND20" s="10"/>
+      <c r="NE20" s="10"/>
+      <c r="NF20" s="10"/>
+      <c r="NG20" s="10"/>
+      <c r="NH20" s="10"/>
+      <c r="NI20" s="10"/>
+      <c r="NJ20" s="10"/>
+      <c r="NK20" s="10"/>
+      <c r="NL20" s="10"/>
+      <c r="NM20" s="10"/>
+      <c r="NN20" s="10"/>
+      <c r="NO20" s="10"/>
+      <c r="NP20" s="10"/>
+      <c r="NQ20" s="10"/>
+      <c r="NR20" s="10"/>
+      <c r="NS20" s="10"/>
+      <c r="NT20" s="10"/>
+      <c r="NU20" s="10"/>
+      <c r="NV20" s="10"/>
+      <c r="NW20" s="10"/>
+      <c r="NX20" s="10"/>
+      <c r="NY20" s="10"/>
+      <c r="NZ20" s="10"/>
+      <c r="OA20" s="10"/>
+      <c r="OB20" s="10"/>
+      <c r="OC20" s="10"/>
+      <c r="OD20" s="10"/>
+      <c r="OE20" s="10"/>
+      <c r="OF20" s="10"/>
+      <c r="OG20" s="10"/>
+      <c r="OH20" s="10"/>
+      <c r="OI20" s="10"/>
+      <c r="OJ20" s="10"/>
+      <c r="OK20" s="10"/>
+      <c r="OL20" s="10"/>
+      <c r="OM20" s="10"/>
+      <c r="ON20" s="10"/>
+      <c r="OO20" s="10"/>
+      <c r="OP20" s="10"/>
+      <c r="OQ20" s="10"/>
+      <c r="OR20" s="10"/>
+      <c r="OS20" s="10"/>
+      <c r="OT20" s="10"/>
+      <c r="OU20" s="10"/>
+      <c r="OV20" s="10"/>
+      <c r="OW20" s="10"/>
+      <c r="OX20" s="10"/>
+      <c r="OY20" s="10"/>
+      <c r="OZ20" s="10"/>
+      <c r="PA20" s="10"/>
+      <c r="PB20" s="10"/>
+      <c r="PC20" s="10"/>
+      <c r="PD20" s="10"/>
+      <c r="PE20" s="10"/>
+      <c r="PF20" s="10"/>
+      <c r="PG20" s="10"/>
+      <c r="PH20" s="10"/>
+      <c r="PI20" s="10"/>
+      <c r="PJ20" s="10"/>
+      <c r="PK20" s="10"/>
+      <c r="PL20" s="10"/>
+      <c r="PM20" s="10"/>
+      <c r="PN20" s="10"/>
+      <c r="PO20" s="10"/>
+      <c r="PP20" s="10"/>
+      <c r="PQ20" s="10"/>
+      <c r="PR20" s="10"/>
+      <c r="PS20" s="10"/>
+      <c r="PT20" s="10"/>
+      <c r="PU20" s="10"/>
+      <c r="PV20" s="10"/>
+      <c r="PW20" s="10"/>
+      <c r="PX20" s="10"/>
+      <c r="PY20" s="10"/>
+      <c r="PZ20" s="10"/>
+      <c r="QA20" s="10"/>
+      <c r="QB20" s="10"/>
+      <c r="QC20" s="10"/>
+      <c r="QD20" s="10"/>
+      <c r="QE20" s="10"/>
+      <c r="QF20" s="10"/>
+      <c r="QG20" s="10"/>
+      <c r="QH20" s="10"/>
+      <c r="QI20" s="10"/>
+      <c r="QJ20" s="10"/>
+      <c r="QK20" s="10"/>
+      <c r="QL20" s="10"/>
+      <c r="QM20" s="10"/>
+      <c r="QN20" s="10"/>
+      <c r="QO20" s="10"/>
+      <c r="QP20" s="10"/>
+      <c r="QQ20" s="10"/>
+      <c r="QR20" s="10"/>
+      <c r="QS20" s="10"/>
+      <c r="QT20" s="10"/>
+      <c r="QU20" s="10"/>
+      <c r="QV20" s="10"/>
+      <c r="QW20" s="10"/>
+      <c r="QX20" s="10"/>
+      <c r="QY20" s="10"/>
+      <c r="QZ20" s="10"/>
+      <c r="RA20" s="10"/>
+      <c r="RB20" s="10"/>
+      <c r="RC20" s="10"/>
+      <c r="RD20" s="10"/>
+      <c r="RE20" s="10"/>
+      <c r="RF20" s="10"/>
+      <c r="RG20" s="10"/>
+      <c r="RH20" s="10"/>
+      <c r="RI20" s="10"/>
+      <c r="RJ20" s="10"/>
+      <c r="RK20" s="10"/>
+      <c r="RL20" s="10"/>
+      <c r="RM20" s="10"/>
+      <c r="RN20" s="10"/>
+      <c r="RO20" s="10"/>
+      <c r="RP20" s="10"/>
+      <c r="RQ20" s="10"/>
+      <c r="RR20" s="10"/>
+      <c r="RS20" s="10"/>
+      <c r="RT20" s="10"/>
+      <c r="RU20" s="10"/>
+      <c r="RV20" s="10"/>
+      <c r="RW20" s="10"/>
+      <c r="RX20" s="10"/>
+      <c r="RY20" s="10"/>
+      <c r="RZ20" s="10"/>
+      <c r="SA20" s="10"/>
+      <c r="SB20" s="10"/>
+      <c r="SC20" s="10"/>
+      <c r="SD20" s="10"/>
+      <c r="SE20" s="10"/>
+      <c r="SF20" s="10"/>
+      <c r="SG20" s="10"/>
+      <c r="SH20" s="10"/>
+      <c r="SI20" s="10"/>
+      <c r="SJ20" s="10"/>
+      <c r="SK20" s="10"/>
+      <c r="SL20" s="10"/>
+      <c r="SM20" s="10"/>
+      <c r="SN20" s="10"/>
+      <c r="SO20" s="10"/>
+      <c r="SP20" s="10"/>
+      <c r="SQ20" s="10"/>
+      <c r="SR20" s="10"/>
+      <c r="SS20" s="10"/>
+      <c r="ST20" s="10"/>
+      <c r="SU20" s="10"/>
+      <c r="SV20" s="10"/>
+      <c r="SW20" s="10"/>
+      <c r="SX20" s="10"/>
+      <c r="SY20" s="10"/>
+      <c r="SZ20" s="10"/>
+      <c r="TA20" s="10"/>
+      <c r="TB20" s="10"/>
+      <c r="TC20" s="10"/>
+      <c r="TD20" s="10"/>
+      <c r="TE20" s="10"/>
+      <c r="TF20" s="10"/>
+      <c r="TG20" s="10"/>
+      <c r="TH20" s="10"/>
+      <c r="TI20" s="10"/>
+      <c r="TJ20" s="10"/>
+      <c r="TK20" s="10"/>
+      <c r="TL20" s="10"/>
+      <c r="TM20" s="10"/>
+      <c r="TN20" s="10"/>
+      <c r="TO20" s="10"/>
+      <c r="TP20" s="10"/>
+      <c r="TQ20" s="10"/>
+      <c r="TR20" s="10"/>
+      <c r="TS20" s="10"/>
+      <c r="TT20" s="10"/>
+      <c r="TU20" s="10"/>
+      <c r="TV20" s="10"/>
+      <c r="TW20" s="10"/>
+      <c r="TX20" s="10"/>
+      <c r="TY20" s="10"/>
+      <c r="TZ20" s="10"/>
+      <c r="UA20" s="10"/>
+      <c r="UB20" s="10"/>
+      <c r="UC20" s="10"/>
+      <c r="UD20" s="10"/>
+      <c r="UE20" s="10"/>
+      <c r="UF20" s="10"/>
+      <c r="UG20" s="10"/>
+      <c r="UH20" s="10"/>
+      <c r="UI20" s="10"/>
+      <c r="UJ20" s="10"/>
+      <c r="UK20" s="10"/>
+      <c r="UL20" s="10"/>
+      <c r="UM20" s="10"/>
+      <c r="UN20" s="10"/>
+      <c r="UO20" s="10"/>
+      <c r="UP20" s="10"/>
+      <c r="UQ20" s="10"/>
+      <c r="UR20" s="10"/>
+      <c r="US20" s="10"/>
+      <c r="UT20" s="10"/>
+      <c r="UU20" s="10"/>
+      <c r="UV20" s="10"/>
+      <c r="UW20" s="10"/>
+      <c r="UX20" s="10"/>
+      <c r="UY20" s="10"/>
+      <c r="UZ20" s="10"/>
+      <c r="VA20" s="10"/>
+      <c r="VB20" s="10"/>
+      <c r="VC20" s="10"/>
+      <c r="VD20" s="10"/>
+      <c r="VE20" s="10"/>
+      <c r="VF20" s="10"/>
+      <c r="VG20" s="10"/>
+      <c r="VH20" s="10"/>
+      <c r="VI20" s="10"/>
+      <c r="VJ20" s="10"/>
+      <c r="VK20" s="10"/>
+      <c r="VL20" s="10"/>
+      <c r="VM20" s="10"/>
+      <c r="VN20" s="10"/>
+      <c r="VO20" s="10"/>
+      <c r="VP20" s="10"/>
+      <c r="VQ20" s="10"/>
+      <c r="VR20" s="10"/>
+      <c r="VS20" s="10"/>
+      <c r="VT20" s="10"/>
+      <c r="VU20" s="10"/>
+      <c r="VV20" s="10"/>
+      <c r="VW20" s="10"/>
+      <c r="VX20" s="10"/>
+      <c r="VY20" s="10"/>
+      <c r="VZ20" s="10"/>
+      <c r="WA20" s="10"/>
+      <c r="WB20" s="10"/>
+      <c r="WC20" s="10"/>
+      <c r="WD20" s="10"/>
+      <c r="WE20" s="10"/>
+      <c r="WF20" s="10"/>
+      <c r="WG20" s="10"/>
+      <c r="WH20" s="10"/>
+      <c r="WI20" s="10"/>
+      <c r="WJ20" s="10"/>
+      <c r="WK20" s="10"/>
+      <c r="WL20" s="10"/>
+      <c r="WM20" s="10"/>
+      <c r="WN20" s="10"/>
+      <c r="WO20" s="10"/>
+      <c r="WP20" s="10"/>
+      <c r="WQ20" s="10"/>
+      <c r="WR20" s="10"/>
+      <c r="WS20" s="10"/>
+      <c r="WT20" s="10"/>
+      <c r="WU20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G21" s="3"/>
       <c r="I21" s="1"/>
@@ -5357,616 +5413,616 @@
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
-      <c r="AA21" s="9"/>
-      <c r="AB21" s="9"/>
-      <c r="AC21" s="9"/>
-      <c r="AD21" s="9"/>
-      <c r="AE21" s="9"/>
-      <c r="AF21" s="9"/>
-      <c r="AG21" s="9"/>
-      <c r="AH21" s="9"/>
-      <c r="AI21" s="9"/>
-      <c r="AJ21" s="9"/>
-      <c r="AK21" s="9"/>
-      <c r="AL21" s="9"/>
-      <c r="AM21" s="9"/>
-      <c r="AN21" s="9"/>
-      <c r="AO21" s="9"/>
-      <c r="AP21" s="9"/>
-      <c r="AQ21" s="9"/>
-      <c r="AR21" s="9"/>
-      <c r="AS21" s="9"/>
-      <c r="AT21" s="9"/>
-      <c r="AU21" s="9"/>
-      <c r="AV21" s="9"/>
-      <c r="AW21" s="9"/>
-      <c r="AX21" s="9"/>
-      <c r="AY21" s="9"/>
-      <c r="AZ21" s="9"/>
-      <c r="BA21" s="9"/>
-      <c r="BB21" s="9"/>
-      <c r="BC21" s="9"/>
-      <c r="BD21" s="9"/>
-      <c r="BE21" s="9"/>
-      <c r="BF21" s="9"/>
-      <c r="BG21" s="9"/>
-      <c r="BH21" s="9"/>
-      <c r="BI21" s="9"/>
-      <c r="BJ21" s="9"/>
-      <c r="BK21" s="9"/>
-      <c r="BL21" s="9"/>
-      <c r="BM21" s="9"/>
-      <c r="BN21" s="9"/>
-      <c r="BO21" s="9"/>
-      <c r="BP21" s="9"/>
-      <c r="BQ21" s="9"/>
-      <c r="BR21" s="9"/>
-      <c r="BS21" s="9"/>
-      <c r="BT21" s="9"/>
-      <c r="BU21" s="9"/>
-      <c r="BV21" s="9"/>
-      <c r="BW21" s="9"/>
-      <c r="BX21" s="9"/>
-      <c r="BY21" s="9"/>
-      <c r="BZ21" s="9"/>
-      <c r="CA21" s="9"/>
-      <c r="CB21" s="9"/>
-      <c r="CC21" s="9"/>
-      <c r="CD21" s="9"/>
-      <c r="CE21" s="9"/>
-      <c r="CF21" s="9"/>
-      <c r="CG21" s="9"/>
-      <c r="CH21" s="9"/>
-      <c r="CI21" s="9"/>
-      <c r="CJ21" s="9"/>
-      <c r="CK21" s="9"/>
-      <c r="CL21" s="9"/>
-      <c r="CM21" s="9"/>
-      <c r="CN21" s="9"/>
-      <c r="CO21" s="9"/>
-      <c r="CP21" s="9"/>
-      <c r="CQ21" s="9"/>
-      <c r="CR21" s="9"/>
-      <c r="CS21" s="9"/>
-      <c r="CT21" s="9"/>
-      <c r="CU21" s="9"/>
-      <c r="CV21" s="9"/>
-      <c r="CW21" s="9"/>
-      <c r="CX21" s="9"/>
-      <c r="CY21" s="9"/>
-      <c r="CZ21" s="9"/>
-      <c r="DA21" s="9"/>
-      <c r="DB21" s="9"/>
-      <c r="DC21" s="9"/>
-      <c r="DD21" s="9"/>
-      <c r="DE21" s="9"/>
-      <c r="DF21" s="9"/>
-      <c r="DG21" s="9"/>
-      <c r="DH21" s="9"/>
-      <c r="DI21" s="9"/>
-      <c r="DJ21" s="9"/>
-      <c r="DK21" s="9"/>
-      <c r="DL21" s="9"/>
-      <c r="DM21" s="9"/>
-      <c r="DN21" s="9"/>
-      <c r="DO21" s="9"/>
-      <c r="DP21" s="9"/>
-      <c r="DQ21" s="9"/>
-      <c r="DR21" s="9"/>
-      <c r="DS21" s="9"/>
-      <c r="DT21" s="9"/>
-      <c r="DU21" s="9"/>
-      <c r="DV21" s="9"/>
-      <c r="DW21" s="9"/>
-      <c r="DX21" s="9"/>
-      <c r="DY21" s="9"/>
-      <c r="DZ21" s="9"/>
-      <c r="EA21" s="9"/>
-      <c r="EB21" s="9"/>
-      <c r="EC21" s="9"/>
-      <c r="ED21" s="9"/>
-      <c r="EE21" s="9"/>
-      <c r="EF21" s="9"/>
-      <c r="EG21" s="9"/>
-      <c r="EH21" s="9"/>
-      <c r="EI21" s="9"/>
-      <c r="EJ21" s="9"/>
-      <c r="EK21" s="9"/>
-      <c r="EL21" s="9"/>
-      <c r="EM21" s="9"/>
-      <c r="EN21" s="9"/>
-      <c r="EO21" s="9"/>
-      <c r="EP21" s="9"/>
-      <c r="EQ21" s="9"/>
-      <c r="ER21" s="9"/>
-      <c r="ES21" s="9"/>
-      <c r="ET21" s="9"/>
-      <c r="EU21" s="9"/>
-      <c r="EV21" s="9"/>
-      <c r="EW21" s="9"/>
-      <c r="EX21" s="9"/>
-      <c r="EY21" s="9"/>
-      <c r="EZ21" s="9"/>
-      <c r="FA21" s="9"/>
-      <c r="FB21" s="9"/>
-      <c r="FC21" s="9"/>
-      <c r="FD21" s="9"/>
-      <c r="FE21" s="9"/>
-      <c r="FF21" s="9"/>
-      <c r="FG21" s="9"/>
-      <c r="FH21" s="9"/>
-      <c r="FI21" s="9"/>
-      <c r="FJ21" s="9"/>
-      <c r="FK21" s="9"/>
-      <c r="FL21" s="9"/>
-      <c r="FM21" s="9"/>
-      <c r="FN21" s="9"/>
-      <c r="FO21" s="9"/>
-      <c r="FP21" s="9"/>
-      <c r="FQ21" s="9"/>
-      <c r="FR21" s="9"/>
-      <c r="FS21" s="9"/>
-      <c r="FT21" s="9"/>
-      <c r="FU21" s="9"/>
-      <c r="FV21" s="9"/>
-      <c r="FW21" s="9"/>
-      <c r="FX21" s="9"/>
-      <c r="FY21" s="9"/>
-      <c r="FZ21" s="9"/>
-      <c r="GA21" s="9"/>
-      <c r="GB21" s="9"/>
-      <c r="GC21" s="9"/>
-      <c r="GD21" s="9"/>
-      <c r="GE21" s="9"/>
-      <c r="GF21" s="9"/>
-      <c r="GG21" s="9"/>
-      <c r="GH21" s="9"/>
-      <c r="GI21" s="9"/>
-      <c r="GJ21" s="9"/>
-      <c r="GK21" s="9"/>
-      <c r="GL21" s="9"/>
-      <c r="GM21" s="9"/>
-      <c r="GN21" s="9"/>
-      <c r="GO21" s="9"/>
-      <c r="GP21" s="9"/>
-      <c r="GQ21" s="9"/>
-      <c r="GR21" s="9"/>
-      <c r="GS21" s="9"/>
-      <c r="GT21" s="9"/>
-      <c r="GU21" s="9"/>
-      <c r="GV21" s="9"/>
-      <c r="GW21" s="9"/>
-      <c r="GX21" s="9"/>
-      <c r="GY21" s="9"/>
-      <c r="GZ21" s="9"/>
-      <c r="HA21" s="9"/>
-      <c r="HB21" s="9"/>
-      <c r="HC21" s="9"/>
-      <c r="HD21" s="9"/>
-      <c r="HE21" s="9"/>
-      <c r="HF21" s="9"/>
-      <c r="HG21" s="9"/>
-      <c r="HH21" s="9"/>
-      <c r="HI21" s="9"/>
-      <c r="HJ21" s="9"/>
-      <c r="HK21" s="9"/>
-      <c r="HL21" s="9"/>
-      <c r="HM21" s="9"/>
-      <c r="HN21" s="9"/>
-      <c r="HO21" s="9"/>
-      <c r="HP21" s="9"/>
-      <c r="HQ21" s="9"/>
-      <c r="HR21" s="9"/>
-      <c r="HS21" s="9"/>
-      <c r="HT21" s="9"/>
-      <c r="HU21" s="9"/>
-      <c r="HV21" s="9"/>
-      <c r="HW21" s="9"/>
-      <c r="HX21" s="9"/>
-      <c r="HY21" s="9"/>
-      <c r="HZ21" s="9"/>
-      <c r="IA21" s="9"/>
-      <c r="IB21" s="9"/>
-      <c r="IC21" s="9"/>
-      <c r="ID21" s="9"/>
-      <c r="IE21" s="9"/>
-      <c r="IF21" s="9"/>
-      <c r="IG21" s="9"/>
-      <c r="IH21" s="9"/>
-      <c r="II21" s="9"/>
-      <c r="IJ21" s="9"/>
-      <c r="IK21" s="9"/>
-      <c r="IL21" s="9"/>
-      <c r="IM21" s="9"/>
-      <c r="IN21" s="9"/>
-      <c r="IO21" s="9"/>
-      <c r="IP21" s="9"/>
-      <c r="IQ21" s="9"/>
-      <c r="IR21" s="9"/>
-      <c r="IS21" s="9"/>
-      <c r="IT21" s="9"/>
-      <c r="IU21" s="9"/>
-      <c r="IV21" s="9"/>
-      <c r="IW21" s="9"/>
-      <c r="IX21" s="9"/>
-      <c r="IY21" s="9"/>
-      <c r="IZ21" s="9"/>
-      <c r="JA21" s="9"/>
-      <c r="JB21" s="9"/>
-      <c r="JC21" s="9"/>
-      <c r="JD21" s="9"/>
-      <c r="JE21" s="9"/>
-      <c r="JF21" s="9"/>
-      <c r="JG21" s="9"/>
-      <c r="JH21" s="9"/>
-      <c r="JI21" s="9"/>
-      <c r="JJ21" s="9"/>
-      <c r="JK21" s="9"/>
-      <c r="JL21" s="9"/>
-      <c r="JM21" s="9"/>
-      <c r="JN21" s="9"/>
-      <c r="JO21" s="9"/>
-      <c r="JP21" s="9"/>
-      <c r="JQ21" s="9"/>
-      <c r="JR21" s="9"/>
-      <c r="JS21" s="9"/>
-      <c r="JT21" s="9"/>
-      <c r="JU21" s="9"/>
-      <c r="JV21" s="9"/>
-      <c r="JW21" s="9"/>
-      <c r="JX21" s="9"/>
-      <c r="JY21" s="9"/>
-      <c r="JZ21" s="9"/>
-      <c r="KA21" s="9"/>
-      <c r="KB21" s="9"/>
-      <c r="KC21" s="9"/>
-      <c r="KD21" s="9"/>
-      <c r="KE21" s="9"/>
-      <c r="KF21" s="9"/>
-      <c r="KG21" s="9"/>
-      <c r="KH21" s="9"/>
-      <c r="KI21" s="9"/>
-      <c r="KJ21" s="9"/>
-      <c r="KK21" s="9"/>
-      <c r="KL21" s="9"/>
-      <c r="KM21" s="9"/>
-      <c r="KN21" s="9"/>
-      <c r="KO21" s="9"/>
-      <c r="KP21" s="9"/>
-      <c r="KQ21" s="9"/>
-      <c r="KR21" s="9"/>
-      <c r="KS21" s="9"/>
-      <c r="KT21" s="9"/>
-      <c r="KU21" s="9"/>
-      <c r="KV21" s="9"/>
-      <c r="KW21" s="9"/>
-      <c r="KX21" s="9"/>
-      <c r="KY21" s="9"/>
-      <c r="KZ21" s="9"/>
-      <c r="LA21" s="9"/>
-      <c r="LB21" s="9"/>
-      <c r="LC21" s="9"/>
-      <c r="LD21" s="9"/>
-      <c r="LE21" s="9"/>
-      <c r="LF21" s="9"/>
-      <c r="LG21" s="9"/>
-      <c r="LH21" s="9"/>
-      <c r="LI21" s="9"/>
-      <c r="LJ21" s="9"/>
-      <c r="LK21" s="9"/>
-      <c r="LL21" s="9"/>
-      <c r="LM21" s="9"/>
-      <c r="LN21" s="9"/>
-      <c r="LO21" s="9"/>
-      <c r="LP21" s="9"/>
-      <c r="LQ21" s="9"/>
-      <c r="LR21" s="9"/>
-      <c r="LS21" s="9"/>
-      <c r="LT21" s="9"/>
-      <c r="LU21" s="9"/>
-      <c r="LV21" s="9"/>
-      <c r="LW21" s="9"/>
-      <c r="LX21" s="9"/>
-      <c r="LY21" s="9"/>
-      <c r="LZ21" s="9"/>
-      <c r="MA21" s="9"/>
-      <c r="MB21" s="9"/>
-      <c r="MC21" s="9"/>
-      <c r="MD21" s="9"/>
-      <c r="ME21" s="9"/>
-      <c r="MF21" s="9"/>
-      <c r="MG21" s="9"/>
-      <c r="MH21" s="9"/>
-      <c r="MI21" s="9"/>
-      <c r="MJ21" s="9"/>
-      <c r="MK21" s="9"/>
-      <c r="ML21" s="9"/>
-      <c r="MM21" s="9"/>
-      <c r="MN21" s="9"/>
-      <c r="MO21" s="9"/>
-      <c r="MP21" s="9"/>
-      <c r="MQ21" s="9"/>
-      <c r="MR21" s="9"/>
-      <c r="MS21" s="9"/>
-      <c r="MT21" s="9"/>
-      <c r="MU21" s="9"/>
-      <c r="MV21" s="9"/>
-      <c r="MW21" s="9"/>
-      <c r="MX21" s="9"/>
-      <c r="MY21" s="9"/>
-      <c r="MZ21" s="9"/>
-      <c r="NA21" s="9"/>
-      <c r="NB21" s="9"/>
-      <c r="NC21" s="9"/>
-      <c r="ND21" s="9"/>
-      <c r="NE21" s="9"/>
-      <c r="NF21" s="9"/>
-      <c r="NG21" s="9"/>
-      <c r="NH21" s="9"/>
-      <c r="NI21" s="9"/>
-      <c r="NJ21" s="9"/>
-      <c r="NK21" s="9"/>
-      <c r="NL21" s="9"/>
-      <c r="NM21" s="9"/>
-      <c r="NN21" s="9"/>
-      <c r="NO21" s="9"/>
-      <c r="NP21" s="9"/>
-      <c r="NQ21" s="9"/>
-      <c r="NR21" s="9"/>
-      <c r="NS21" s="9"/>
-      <c r="NT21" s="9"/>
-      <c r="NU21" s="9"/>
-      <c r="NV21" s="9"/>
-      <c r="NW21" s="9"/>
-      <c r="NX21" s="9"/>
-      <c r="NY21" s="9"/>
-      <c r="NZ21" s="9"/>
-      <c r="OA21" s="9"/>
-      <c r="OB21" s="9"/>
-      <c r="OC21" s="9"/>
-      <c r="OD21" s="9"/>
-      <c r="OE21" s="9"/>
-      <c r="OF21" s="9"/>
-      <c r="OG21" s="9"/>
-      <c r="OH21" s="9"/>
-      <c r="OI21" s="9"/>
-      <c r="OJ21" s="9"/>
-      <c r="OK21" s="9"/>
-      <c r="OL21" s="9"/>
-      <c r="OM21" s="9"/>
-      <c r="ON21" s="9"/>
-      <c r="OO21" s="9"/>
-      <c r="OP21" s="9"/>
-      <c r="OQ21" s="9"/>
-      <c r="OR21" s="9"/>
-      <c r="OS21" s="9"/>
-      <c r="OT21" s="9"/>
-      <c r="OU21" s="9"/>
-      <c r="OV21" s="9"/>
-      <c r="OW21" s="9"/>
-      <c r="OX21" s="9"/>
-      <c r="OY21" s="9"/>
-      <c r="OZ21" s="9"/>
-      <c r="PA21" s="9"/>
-      <c r="PB21" s="9"/>
-      <c r="PC21" s="9"/>
-      <c r="PD21" s="9"/>
-      <c r="PE21" s="9"/>
-      <c r="PF21" s="9"/>
-      <c r="PG21" s="9"/>
-      <c r="PH21" s="9"/>
-      <c r="PI21" s="9"/>
-      <c r="PJ21" s="9"/>
-      <c r="PK21" s="9"/>
-      <c r="PL21" s="9"/>
-      <c r="PM21" s="9"/>
-      <c r="PN21" s="9"/>
-      <c r="PO21" s="9"/>
-      <c r="PP21" s="9"/>
-      <c r="PQ21" s="9"/>
-      <c r="PR21" s="9"/>
-      <c r="PS21" s="9"/>
-      <c r="PT21" s="9"/>
-      <c r="PU21" s="9"/>
-      <c r="PV21" s="9"/>
-      <c r="PW21" s="9"/>
-      <c r="PX21" s="9"/>
-      <c r="PY21" s="9"/>
-      <c r="PZ21" s="9"/>
-      <c r="QA21" s="9"/>
-      <c r="QB21" s="9"/>
-      <c r="QC21" s="9"/>
-      <c r="QD21" s="9"/>
-      <c r="QE21" s="9"/>
-      <c r="QF21" s="9"/>
-      <c r="QG21" s="9"/>
-      <c r="QH21" s="9"/>
-      <c r="QI21" s="9"/>
-      <c r="QJ21" s="9"/>
-      <c r="QK21" s="9"/>
-      <c r="QL21" s="9"/>
-      <c r="QM21" s="9"/>
-      <c r="QN21" s="9"/>
-      <c r="QO21" s="9"/>
-      <c r="QP21" s="9"/>
-      <c r="QQ21" s="9"/>
-      <c r="QR21" s="9"/>
-      <c r="QS21" s="9"/>
-      <c r="QT21" s="9"/>
-      <c r="QU21" s="9"/>
-      <c r="QV21" s="9"/>
-      <c r="QW21" s="9"/>
-      <c r="QX21" s="9"/>
-      <c r="QY21" s="9"/>
-      <c r="QZ21" s="9"/>
-      <c r="RA21" s="9"/>
-      <c r="RB21" s="9"/>
-      <c r="RC21" s="9"/>
-      <c r="RD21" s="9"/>
-      <c r="RE21" s="9"/>
-      <c r="RF21" s="9"/>
-      <c r="RG21" s="9"/>
-      <c r="RH21" s="9"/>
-      <c r="RI21" s="9"/>
-      <c r="RJ21" s="9"/>
-      <c r="RK21" s="9"/>
-      <c r="RL21" s="9"/>
-      <c r="RM21" s="9"/>
-      <c r="RN21" s="9"/>
-      <c r="RO21" s="9"/>
-      <c r="RP21" s="9"/>
-      <c r="RQ21" s="9"/>
-      <c r="RR21" s="9"/>
-      <c r="RS21" s="9"/>
-      <c r="RT21" s="9"/>
-      <c r="RU21" s="9"/>
-      <c r="RV21" s="9"/>
-      <c r="RW21" s="9"/>
-      <c r="RX21" s="9"/>
-      <c r="RY21" s="9"/>
-      <c r="RZ21" s="9"/>
-      <c r="SA21" s="9"/>
-      <c r="SB21" s="9"/>
-      <c r="SC21" s="9"/>
-      <c r="SD21" s="9"/>
-      <c r="SE21" s="9"/>
-      <c r="SF21" s="9"/>
-      <c r="SG21" s="9"/>
-      <c r="SH21" s="9"/>
-      <c r="SI21" s="9"/>
-      <c r="SJ21" s="9"/>
-      <c r="SK21" s="9"/>
-      <c r="SL21" s="9"/>
-      <c r="SM21" s="9"/>
-      <c r="SN21" s="9"/>
-      <c r="SO21" s="9"/>
-      <c r="SP21" s="9"/>
-      <c r="SQ21" s="9"/>
-      <c r="SR21" s="9"/>
-      <c r="SS21" s="9"/>
-      <c r="ST21" s="9"/>
-      <c r="SU21" s="9"/>
-      <c r="SV21" s="9"/>
-      <c r="SW21" s="9"/>
-      <c r="SX21" s="9"/>
-      <c r="SY21" s="9"/>
-      <c r="SZ21" s="9"/>
-      <c r="TA21" s="9"/>
-      <c r="TB21" s="9"/>
-      <c r="TC21" s="9"/>
-      <c r="TD21" s="9"/>
-      <c r="TE21" s="9"/>
-      <c r="TF21" s="9"/>
-      <c r="TG21" s="9"/>
-      <c r="TH21" s="9"/>
-      <c r="TI21" s="9"/>
-      <c r="TJ21" s="9"/>
-      <c r="TK21" s="9"/>
-      <c r="TL21" s="9"/>
-      <c r="TM21" s="9"/>
-      <c r="TN21" s="9"/>
-      <c r="TO21" s="9"/>
-      <c r="TP21" s="9"/>
-      <c r="TQ21" s="9"/>
-      <c r="TR21" s="9"/>
-      <c r="TS21" s="9"/>
-      <c r="TT21" s="9"/>
-      <c r="TU21" s="9"/>
-      <c r="TV21" s="9"/>
-      <c r="TW21" s="9"/>
-      <c r="TX21" s="9"/>
-      <c r="TY21" s="9"/>
-      <c r="TZ21" s="9"/>
-      <c r="UA21" s="9"/>
-      <c r="UB21" s="9"/>
-      <c r="UC21" s="9"/>
-      <c r="UD21" s="9"/>
-      <c r="UE21" s="9"/>
-      <c r="UF21" s="9"/>
-      <c r="UG21" s="9"/>
-      <c r="UH21" s="9"/>
-      <c r="UI21" s="9"/>
-      <c r="UJ21" s="9"/>
-      <c r="UK21" s="9"/>
-      <c r="UL21" s="9"/>
-      <c r="UM21" s="9"/>
-      <c r="UN21" s="9"/>
-      <c r="UO21" s="9"/>
-      <c r="UP21" s="9"/>
-      <c r="UQ21" s="9"/>
-      <c r="UR21" s="9"/>
-      <c r="US21" s="9"/>
-      <c r="UT21" s="9"/>
-      <c r="UU21" s="9"/>
-      <c r="UV21" s="9"/>
-      <c r="UW21" s="9"/>
-      <c r="UX21" s="9"/>
-      <c r="UY21" s="9"/>
-      <c r="UZ21" s="9"/>
-      <c r="VA21" s="9"/>
-      <c r="VB21" s="9"/>
-      <c r="VC21" s="9"/>
-      <c r="VD21" s="9"/>
-      <c r="VE21" s="9"/>
-      <c r="VF21" s="9"/>
-      <c r="VG21" s="9"/>
-      <c r="VH21" s="9"/>
-      <c r="VI21" s="9"/>
-      <c r="VJ21" s="9"/>
-      <c r="VK21" s="9"/>
-      <c r="VL21" s="9"/>
-      <c r="VM21" s="9"/>
-      <c r="VN21" s="9"/>
-      <c r="VO21" s="9"/>
-      <c r="VP21" s="9"/>
-      <c r="VQ21" s="9"/>
-      <c r="VR21" s="9"/>
-      <c r="VS21" s="9"/>
-      <c r="VT21" s="9"/>
-      <c r="VU21" s="9"/>
-      <c r="VV21" s="9"/>
-      <c r="VW21" s="9"/>
-      <c r="VX21" s="9"/>
-      <c r="VY21" s="9"/>
-      <c r="VZ21" s="9"/>
-      <c r="WA21" s="9"/>
-      <c r="WB21" s="9"/>
-      <c r="WC21" s="9"/>
-      <c r="WD21" s="9"/>
-      <c r="WE21" s="9"/>
-      <c r="WF21" s="9"/>
-      <c r="WG21" s="9"/>
-      <c r="WH21" s="9"/>
-      <c r="WI21" s="9"/>
-      <c r="WJ21" s="9"/>
-      <c r="WK21" s="9"/>
-      <c r="WL21" s="9"/>
-      <c r="WM21" s="9"/>
-      <c r="WN21" s="9"/>
-      <c r="WO21" s="9"/>
-      <c r="WP21" s="9"/>
-      <c r="WQ21" s="9"/>
-      <c r="WR21" s="9"/>
-      <c r="WS21" s="9"/>
-      <c r="WT21" s="9"/>
-      <c r="WU21" s="9"/>
+      <c r="AA21" s="10"/>
+      <c r="AB21" s="10"/>
+      <c r="AC21" s="10"/>
+      <c r="AD21" s="10"/>
+      <c r="AE21" s="10"/>
+      <c r="AF21" s="10"/>
+      <c r="AG21" s="10"/>
+      <c r="AH21" s="10"/>
+      <c r="AI21" s="10"/>
+      <c r="AJ21" s="10"/>
+      <c r="AK21" s="10"/>
+      <c r="AL21" s="10"/>
+      <c r="AM21" s="10"/>
+      <c r="AN21" s="10"/>
+      <c r="AO21" s="10"/>
+      <c r="AP21" s="10"/>
+      <c r="AQ21" s="10"/>
+      <c r="AR21" s="10"/>
+      <c r="AS21" s="10"/>
+      <c r="AT21" s="10"/>
+      <c r="AU21" s="10"/>
+      <c r="AV21" s="10"/>
+      <c r="AW21" s="10"/>
+      <c r="AX21" s="10"/>
+      <c r="AY21" s="10"/>
+      <c r="AZ21" s="10"/>
+      <c r="BA21" s="10"/>
+      <c r="BB21" s="10"/>
+      <c r="BC21" s="10"/>
+      <c r="BD21" s="10"/>
+      <c r="BE21" s="10"/>
+      <c r="BF21" s="10"/>
+      <c r="BG21" s="10"/>
+      <c r="BH21" s="10"/>
+      <c r="BI21" s="10"/>
+      <c r="BJ21" s="10"/>
+      <c r="BK21" s="10"/>
+      <c r="BL21" s="10"/>
+      <c r="BM21" s="10"/>
+      <c r="BN21" s="10"/>
+      <c r="BO21" s="10"/>
+      <c r="BP21" s="10"/>
+      <c r="BQ21" s="10"/>
+      <c r="BR21" s="10"/>
+      <c r="BS21" s="10"/>
+      <c r="BT21" s="10"/>
+      <c r="BU21" s="10"/>
+      <c r="BV21" s="10"/>
+      <c r="BW21" s="10"/>
+      <c r="BX21" s="10"/>
+      <c r="BY21" s="10"/>
+      <c r="BZ21" s="10"/>
+      <c r="CA21" s="10"/>
+      <c r="CB21" s="10"/>
+      <c r="CC21" s="10"/>
+      <c r="CD21" s="10"/>
+      <c r="CE21" s="10"/>
+      <c r="CF21" s="10"/>
+      <c r="CG21" s="10"/>
+      <c r="CH21" s="10"/>
+      <c r="CI21" s="10"/>
+      <c r="CJ21" s="10"/>
+      <c r="CK21" s="10"/>
+      <c r="CL21" s="10"/>
+      <c r="CM21" s="10"/>
+      <c r="CN21" s="10"/>
+      <c r="CO21" s="10"/>
+      <c r="CP21" s="10"/>
+      <c r="CQ21" s="10"/>
+      <c r="CR21" s="10"/>
+      <c r="CS21" s="10"/>
+      <c r="CT21" s="10"/>
+      <c r="CU21" s="10"/>
+      <c r="CV21" s="10"/>
+      <c r="CW21" s="10"/>
+      <c r="CX21" s="10"/>
+      <c r="CY21" s="10"/>
+      <c r="CZ21" s="10"/>
+      <c r="DA21" s="10"/>
+      <c r="DB21" s="10"/>
+      <c r="DC21" s="10"/>
+      <c r="DD21" s="10"/>
+      <c r="DE21" s="10"/>
+      <c r="DF21" s="10"/>
+      <c r="DG21" s="10"/>
+      <c r="DH21" s="10"/>
+      <c r="DI21" s="10"/>
+      <c r="DJ21" s="10"/>
+      <c r="DK21" s="10"/>
+      <c r="DL21" s="10"/>
+      <c r="DM21" s="10"/>
+      <c r="DN21" s="10"/>
+      <c r="DO21" s="10"/>
+      <c r="DP21" s="10"/>
+      <c r="DQ21" s="10"/>
+      <c r="DR21" s="10"/>
+      <c r="DS21" s="10"/>
+      <c r="DT21" s="10"/>
+      <c r="DU21" s="10"/>
+      <c r="DV21" s="10"/>
+      <c r="DW21" s="10"/>
+      <c r="DX21" s="10"/>
+      <c r="DY21" s="10"/>
+      <c r="DZ21" s="10"/>
+      <c r="EA21" s="10"/>
+      <c r="EB21" s="10"/>
+      <c r="EC21" s="10"/>
+      <c r="ED21" s="10"/>
+      <c r="EE21" s="10"/>
+      <c r="EF21" s="10"/>
+      <c r="EG21" s="10"/>
+      <c r="EH21" s="10"/>
+      <c r="EI21" s="10"/>
+      <c r="EJ21" s="10"/>
+      <c r="EK21" s="10"/>
+      <c r="EL21" s="10"/>
+      <c r="EM21" s="10"/>
+      <c r="EN21" s="10"/>
+      <c r="EO21" s="10"/>
+      <c r="EP21" s="10"/>
+      <c r="EQ21" s="10"/>
+      <c r="ER21" s="10"/>
+      <c r="ES21" s="10"/>
+      <c r="ET21" s="10"/>
+      <c r="EU21" s="10"/>
+      <c r="EV21" s="10"/>
+      <c r="EW21" s="10"/>
+      <c r="EX21" s="10"/>
+      <c r="EY21" s="10"/>
+      <c r="EZ21" s="10"/>
+      <c r="FA21" s="10"/>
+      <c r="FB21" s="10"/>
+      <c r="FC21" s="10"/>
+      <c r="FD21" s="10"/>
+      <c r="FE21" s="10"/>
+      <c r="FF21" s="10"/>
+      <c r="FG21" s="10"/>
+      <c r="FH21" s="10"/>
+      <c r="FI21" s="10"/>
+      <c r="FJ21" s="10"/>
+      <c r="FK21" s="10"/>
+      <c r="FL21" s="10"/>
+      <c r="FM21" s="10"/>
+      <c r="FN21" s="10"/>
+      <c r="FO21" s="10"/>
+      <c r="FP21" s="10"/>
+      <c r="FQ21" s="10"/>
+      <c r="FR21" s="10"/>
+      <c r="FS21" s="10"/>
+      <c r="FT21" s="10"/>
+      <c r="FU21" s="10"/>
+      <c r="FV21" s="10"/>
+      <c r="FW21" s="10"/>
+      <c r="FX21" s="10"/>
+      <c r="FY21" s="10"/>
+      <c r="FZ21" s="10"/>
+      <c r="GA21" s="10"/>
+      <c r="GB21" s="10"/>
+      <c r="GC21" s="10"/>
+      <c r="GD21" s="10"/>
+      <c r="GE21" s="10"/>
+      <c r="GF21" s="10"/>
+      <c r="GG21" s="10"/>
+      <c r="GH21" s="10"/>
+      <c r="GI21" s="10"/>
+      <c r="GJ21" s="10"/>
+      <c r="GK21" s="10"/>
+      <c r="GL21" s="10"/>
+      <c r="GM21" s="10"/>
+      <c r="GN21" s="10"/>
+      <c r="GO21" s="10"/>
+      <c r="GP21" s="10"/>
+      <c r="GQ21" s="10"/>
+      <c r="GR21" s="10"/>
+      <c r="GS21" s="10"/>
+      <c r="GT21" s="10"/>
+      <c r="GU21" s="10"/>
+      <c r="GV21" s="10"/>
+      <c r="GW21" s="10"/>
+      <c r="GX21" s="10"/>
+      <c r="GY21" s="10"/>
+      <c r="GZ21" s="10"/>
+      <c r="HA21" s="10"/>
+      <c r="HB21" s="10"/>
+      <c r="HC21" s="10"/>
+      <c r="HD21" s="10"/>
+      <c r="HE21" s="10"/>
+      <c r="HF21" s="10"/>
+      <c r="HG21" s="10"/>
+      <c r="HH21" s="10"/>
+      <c r="HI21" s="10"/>
+      <c r="HJ21" s="10"/>
+      <c r="HK21" s="10"/>
+      <c r="HL21" s="10"/>
+      <c r="HM21" s="10"/>
+      <c r="HN21" s="10"/>
+      <c r="HO21" s="10"/>
+      <c r="HP21" s="10"/>
+      <c r="HQ21" s="10"/>
+      <c r="HR21" s="10"/>
+      <c r="HS21" s="10"/>
+      <c r="HT21" s="10"/>
+      <c r="HU21" s="10"/>
+      <c r="HV21" s="10"/>
+      <c r="HW21" s="10"/>
+      <c r="HX21" s="10"/>
+      <c r="HY21" s="10"/>
+      <c r="HZ21" s="10"/>
+      <c r="IA21" s="10"/>
+      <c r="IB21" s="10"/>
+      <c r="IC21" s="10"/>
+      <c r="ID21" s="10"/>
+      <c r="IE21" s="10"/>
+      <c r="IF21" s="10"/>
+      <c r="IG21" s="10"/>
+      <c r="IH21" s="10"/>
+      <c r="II21" s="10"/>
+      <c r="IJ21" s="10"/>
+      <c r="IK21" s="10"/>
+      <c r="IL21" s="10"/>
+      <c r="IM21" s="10"/>
+      <c r="IN21" s="10"/>
+      <c r="IO21" s="10"/>
+      <c r="IP21" s="10"/>
+      <c r="IQ21" s="10"/>
+      <c r="IR21" s="10"/>
+      <c r="IS21" s="10"/>
+      <c r="IT21" s="10"/>
+      <c r="IU21" s="10"/>
+      <c r="IV21" s="10"/>
+      <c r="IW21" s="10"/>
+      <c r="IX21" s="10"/>
+      <c r="IY21" s="10"/>
+      <c r="IZ21" s="10"/>
+      <c r="JA21" s="10"/>
+      <c r="JB21" s="10"/>
+      <c r="JC21" s="10"/>
+      <c r="JD21" s="10"/>
+      <c r="JE21" s="10"/>
+      <c r="JF21" s="10"/>
+      <c r="JG21" s="10"/>
+      <c r="JH21" s="10"/>
+      <c r="JI21" s="10"/>
+      <c r="JJ21" s="10"/>
+      <c r="JK21" s="10"/>
+      <c r="JL21" s="10"/>
+      <c r="JM21" s="10"/>
+      <c r="JN21" s="10"/>
+      <c r="JO21" s="10"/>
+      <c r="JP21" s="10"/>
+      <c r="JQ21" s="10"/>
+      <c r="JR21" s="10"/>
+      <c r="JS21" s="10"/>
+      <c r="JT21" s="10"/>
+      <c r="JU21" s="10"/>
+      <c r="JV21" s="10"/>
+      <c r="JW21" s="10"/>
+      <c r="JX21" s="10"/>
+      <c r="JY21" s="10"/>
+      <c r="JZ21" s="10"/>
+      <c r="KA21" s="10"/>
+      <c r="KB21" s="10"/>
+      <c r="KC21" s="10"/>
+      <c r="KD21" s="10"/>
+      <c r="KE21" s="10"/>
+      <c r="KF21" s="10"/>
+      <c r="KG21" s="10"/>
+      <c r="KH21" s="10"/>
+      <c r="KI21" s="10"/>
+      <c r="KJ21" s="10"/>
+      <c r="KK21" s="10"/>
+      <c r="KL21" s="10"/>
+      <c r="KM21" s="10"/>
+      <c r="KN21" s="10"/>
+      <c r="KO21" s="10"/>
+      <c r="KP21" s="10"/>
+      <c r="KQ21" s="10"/>
+      <c r="KR21" s="10"/>
+      <c r="KS21" s="10"/>
+      <c r="KT21" s="10"/>
+      <c r="KU21" s="10"/>
+      <c r="KV21" s="10"/>
+      <c r="KW21" s="10"/>
+      <c r="KX21" s="10"/>
+      <c r="KY21" s="10"/>
+      <c r="KZ21" s="10"/>
+      <c r="LA21" s="10"/>
+      <c r="LB21" s="10"/>
+      <c r="LC21" s="10"/>
+      <c r="LD21" s="10"/>
+      <c r="LE21" s="10"/>
+      <c r="LF21" s="10"/>
+      <c r="LG21" s="10"/>
+      <c r="LH21" s="10"/>
+      <c r="LI21" s="10"/>
+      <c r="LJ21" s="10"/>
+      <c r="LK21" s="10"/>
+      <c r="LL21" s="10"/>
+      <c r="LM21" s="10"/>
+      <c r="LN21" s="10"/>
+      <c r="LO21" s="10"/>
+      <c r="LP21" s="10"/>
+      <c r="LQ21" s="10"/>
+      <c r="LR21" s="10"/>
+      <c r="LS21" s="10"/>
+      <c r="LT21" s="10"/>
+      <c r="LU21" s="10"/>
+      <c r="LV21" s="10"/>
+      <c r="LW21" s="10"/>
+      <c r="LX21" s="10"/>
+      <c r="LY21" s="10"/>
+      <c r="LZ21" s="10"/>
+      <c r="MA21" s="10"/>
+      <c r="MB21" s="10"/>
+      <c r="MC21" s="10"/>
+      <c r="MD21" s="10"/>
+      <c r="ME21" s="10"/>
+      <c r="MF21" s="10"/>
+      <c r="MG21" s="10"/>
+      <c r="MH21" s="10"/>
+      <c r="MI21" s="10"/>
+      <c r="MJ21" s="10"/>
+      <c r="MK21" s="10"/>
+      <c r="ML21" s="10"/>
+      <c r="MM21" s="10"/>
+      <c r="MN21" s="10"/>
+      <c r="MO21" s="10"/>
+      <c r="MP21" s="10"/>
+      <c r="MQ21" s="10"/>
+      <c r="MR21" s="10"/>
+      <c r="MS21" s="10"/>
+      <c r="MT21" s="10"/>
+      <c r="MU21" s="10"/>
+      <c r="MV21" s="10"/>
+      <c r="MW21" s="10"/>
+      <c r="MX21" s="10"/>
+      <c r="MY21" s="10"/>
+      <c r="MZ21" s="10"/>
+      <c r="NA21" s="10"/>
+      <c r="NB21" s="10"/>
+      <c r="NC21" s="10"/>
+      <c r="ND21" s="10"/>
+      <c r="NE21" s="10"/>
+      <c r="NF21" s="10"/>
+      <c r="NG21" s="10"/>
+      <c r="NH21" s="10"/>
+      <c r="NI21" s="10"/>
+      <c r="NJ21" s="10"/>
+      <c r="NK21" s="10"/>
+      <c r="NL21" s="10"/>
+      <c r="NM21" s="10"/>
+      <c r="NN21" s="10"/>
+      <c r="NO21" s="10"/>
+      <c r="NP21" s="10"/>
+      <c r="NQ21" s="10"/>
+      <c r="NR21" s="10"/>
+      <c r="NS21" s="10"/>
+      <c r="NT21" s="10"/>
+      <c r="NU21" s="10"/>
+      <c r="NV21" s="10"/>
+      <c r="NW21" s="10"/>
+      <c r="NX21" s="10"/>
+      <c r="NY21" s="10"/>
+      <c r="NZ21" s="10"/>
+      <c r="OA21" s="10"/>
+      <c r="OB21" s="10"/>
+      <c r="OC21" s="10"/>
+      <c r="OD21" s="10"/>
+      <c r="OE21" s="10"/>
+      <c r="OF21" s="10"/>
+      <c r="OG21" s="10"/>
+      <c r="OH21" s="10"/>
+      <c r="OI21" s="10"/>
+      <c r="OJ21" s="10"/>
+      <c r="OK21" s="10"/>
+      <c r="OL21" s="10"/>
+      <c r="OM21" s="10"/>
+      <c r="ON21" s="10"/>
+      <c r="OO21" s="10"/>
+      <c r="OP21" s="10"/>
+      <c r="OQ21" s="10"/>
+      <c r="OR21" s="10"/>
+      <c r="OS21" s="10"/>
+      <c r="OT21" s="10"/>
+      <c r="OU21" s="10"/>
+      <c r="OV21" s="10"/>
+      <c r="OW21" s="10"/>
+      <c r="OX21" s="10"/>
+      <c r="OY21" s="10"/>
+      <c r="OZ21" s="10"/>
+      <c r="PA21" s="10"/>
+      <c r="PB21" s="10"/>
+      <c r="PC21" s="10"/>
+      <c r="PD21" s="10"/>
+      <c r="PE21" s="10"/>
+      <c r="PF21" s="10"/>
+      <c r="PG21" s="10"/>
+      <c r="PH21" s="10"/>
+      <c r="PI21" s="10"/>
+      <c r="PJ21" s="10"/>
+      <c r="PK21" s="10"/>
+      <c r="PL21" s="10"/>
+      <c r="PM21" s="10"/>
+      <c r="PN21" s="10"/>
+      <c r="PO21" s="10"/>
+      <c r="PP21" s="10"/>
+      <c r="PQ21" s="10"/>
+      <c r="PR21" s="10"/>
+      <c r="PS21" s="10"/>
+      <c r="PT21" s="10"/>
+      <c r="PU21" s="10"/>
+      <c r="PV21" s="10"/>
+      <c r="PW21" s="10"/>
+      <c r="PX21" s="10"/>
+      <c r="PY21" s="10"/>
+      <c r="PZ21" s="10"/>
+      <c r="QA21" s="10"/>
+      <c r="QB21" s="10"/>
+      <c r="QC21" s="10"/>
+      <c r="QD21" s="10"/>
+      <c r="QE21" s="10"/>
+      <c r="QF21" s="10"/>
+      <c r="QG21" s="10"/>
+      <c r="QH21" s="10"/>
+      <c r="QI21" s="10"/>
+      <c r="QJ21" s="10"/>
+      <c r="QK21" s="10"/>
+      <c r="QL21" s="10"/>
+      <c r="QM21" s="10"/>
+      <c r="QN21" s="10"/>
+      <c r="QO21" s="10"/>
+      <c r="QP21" s="10"/>
+      <c r="QQ21" s="10"/>
+      <c r="QR21" s="10"/>
+      <c r="QS21" s="10"/>
+      <c r="QT21" s="10"/>
+      <c r="QU21" s="10"/>
+      <c r="QV21" s="10"/>
+      <c r="QW21" s="10"/>
+      <c r="QX21" s="10"/>
+      <c r="QY21" s="10"/>
+      <c r="QZ21" s="10"/>
+      <c r="RA21" s="10"/>
+      <c r="RB21" s="10"/>
+      <c r="RC21" s="10"/>
+      <c r="RD21" s="10"/>
+      <c r="RE21" s="10"/>
+      <c r="RF21" s="10"/>
+      <c r="RG21" s="10"/>
+      <c r="RH21" s="10"/>
+      <c r="RI21" s="10"/>
+      <c r="RJ21" s="10"/>
+      <c r="RK21" s="10"/>
+      <c r="RL21" s="10"/>
+      <c r="RM21" s="10"/>
+      <c r="RN21" s="10"/>
+      <c r="RO21" s="10"/>
+      <c r="RP21" s="10"/>
+      <c r="RQ21" s="10"/>
+      <c r="RR21" s="10"/>
+      <c r="RS21" s="10"/>
+      <c r="RT21" s="10"/>
+      <c r="RU21" s="10"/>
+      <c r="RV21" s="10"/>
+      <c r="RW21" s="10"/>
+      <c r="RX21" s="10"/>
+      <c r="RY21" s="10"/>
+      <c r="RZ21" s="10"/>
+      <c r="SA21" s="10"/>
+      <c r="SB21" s="10"/>
+      <c r="SC21" s="10"/>
+      <c r="SD21" s="10"/>
+      <c r="SE21" s="10"/>
+      <c r="SF21" s="10"/>
+      <c r="SG21" s="10"/>
+      <c r="SH21" s="10"/>
+      <c r="SI21" s="10"/>
+      <c r="SJ21" s="10"/>
+      <c r="SK21" s="10"/>
+      <c r="SL21" s="10"/>
+      <c r="SM21" s="10"/>
+      <c r="SN21" s="10"/>
+      <c r="SO21" s="10"/>
+      <c r="SP21" s="10"/>
+      <c r="SQ21" s="10"/>
+      <c r="SR21" s="10"/>
+      <c r="SS21" s="10"/>
+      <c r="ST21" s="10"/>
+      <c r="SU21" s="10"/>
+      <c r="SV21" s="10"/>
+      <c r="SW21" s="10"/>
+      <c r="SX21" s="10"/>
+      <c r="SY21" s="10"/>
+      <c r="SZ21" s="10"/>
+      <c r="TA21" s="10"/>
+      <c r="TB21" s="10"/>
+      <c r="TC21" s="10"/>
+      <c r="TD21" s="10"/>
+      <c r="TE21" s="10"/>
+      <c r="TF21" s="10"/>
+      <c r="TG21" s="10"/>
+      <c r="TH21" s="10"/>
+      <c r="TI21" s="10"/>
+      <c r="TJ21" s="10"/>
+      <c r="TK21" s="10"/>
+      <c r="TL21" s="10"/>
+      <c r="TM21" s="10"/>
+      <c r="TN21" s="10"/>
+      <c r="TO21" s="10"/>
+      <c r="TP21" s="10"/>
+      <c r="TQ21" s="10"/>
+      <c r="TR21" s="10"/>
+      <c r="TS21" s="10"/>
+      <c r="TT21" s="10"/>
+      <c r="TU21" s="10"/>
+      <c r="TV21" s="10"/>
+      <c r="TW21" s="10"/>
+      <c r="TX21" s="10"/>
+      <c r="TY21" s="10"/>
+      <c r="TZ21" s="10"/>
+      <c r="UA21" s="10"/>
+      <c r="UB21" s="10"/>
+      <c r="UC21" s="10"/>
+      <c r="UD21" s="10"/>
+      <c r="UE21" s="10"/>
+      <c r="UF21" s="10"/>
+      <c r="UG21" s="10"/>
+      <c r="UH21" s="10"/>
+      <c r="UI21" s="10"/>
+      <c r="UJ21" s="10"/>
+      <c r="UK21" s="10"/>
+      <c r="UL21" s="10"/>
+      <c r="UM21" s="10"/>
+      <c r="UN21" s="10"/>
+      <c r="UO21" s="10"/>
+      <c r="UP21" s="10"/>
+      <c r="UQ21" s="10"/>
+      <c r="UR21" s="10"/>
+      <c r="US21" s="10"/>
+      <c r="UT21" s="10"/>
+      <c r="UU21" s="10"/>
+      <c r="UV21" s="10"/>
+      <c r="UW21" s="10"/>
+      <c r="UX21" s="10"/>
+      <c r="UY21" s="10"/>
+      <c r="UZ21" s="10"/>
+      <c r="VA21" s="10"/>
+      <c r="VB21" s="10"/>
+      <c r="VC21" s="10"/>
+      <c r="VD21" s="10"/>
+      <c r="VE21" s="10"/>
+      <c r="VF21" s="10"/>
+      <c r="VG21" s="10"/>
+      <c r="VH21" s="10"/>
+      <c r="VI21" s="10"/>
+      <c r="VJ21" s="10"/>
+      <c r="VK21" s="10"/>
+      <c r="VL21" s="10"/>
+      <c r="VM21" s="10"/>
+      <c r="VN21" s="10"/>
+      <c r="VO21" s="10"/>
+      <c r="VP21" s="10"/>
+      <c r="VQ21" s="10"/>
+      <c r="VR21" s="10"/>
+      <c r="VS21" s="10"/>
+      <c r="VT21" s="10"/>
+      <c r="VU21" s="10"/>
+      <c r="VV21" s="10"/>
+      <c r="VW21" s="10"/>
+      <c r="VX21" s="10"/>
+      <c r="VY21" s="10"/>
+      <c r="VZ21" s="10"/>
+      <c r="WA21" s="10"/>
+      <c r="WB21" s="10"/>
+      <c r="WC21" s="10"/>
+      <c r="WD21" s="10"/>
+      <c r="WE21" s="10"/>
+      <c r="WF21" s="10"/>
+      <c r="WG21" s="10"/>
+      <c r="WH21" s="10"/>
+      <c r="WI21" s="10"/>
+      <c r="WJ21" s="10"/>
+      <c r="WK21" s="10"/>
+      <c r="WL21" s="10"/>
+      <c r="WM21" s="10"/>
+      <c r="WN21" s="10"/>
+      <c r="WO21" s="10"/>
+      <c r="WP21" s="10"/>
+      <c r="WQ21" s="10"/>
+      <c r="WR21" s="10"/>
+      <c r="WS21" s="10"/>
+      <c r="WT21" s="10"/>
+      <c r="WU21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G22" s="3"/>
       <c r="I22" s="1"/>
@@ -6583,20 +6639,20 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G23" s="3"/>
       <c r="I23" s="1"/>
@@ -7213,20 +7269,20 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G24" s="3"/>
       <c r="I24" s="1"/>
@@ -7843,20 +7899,20 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G25" s="3"/>
       <c r="I25" s="1"/>
@@ -8473,19 +8529,19 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -9103,17 +9159,17 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="11"/>
+        <v>73</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="12"/>
       <c r="E27" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F27" s="1"/>
       <c r="I27" s="1"/>
@@ -9730,20 +9786,20 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D28" s="11"/>
+        <v>75</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="12"/>
       <c r="E28" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -10359,20 +10415,20 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" s="11"/>
+        <v>76</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="12"/>
       <c r="E29" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F29" s="13" t="s">
-        <v>54</v>
+        <v>12</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>58</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -10987,18 +11043,18 @@
       <c r="WU29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" s="11"/>
+      <c r="A30" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="12"/>
       <c r="E30" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F30" s="1"/>
       <c r="I30" s="1"/>
@@ -11614,18 +11670,18 @@
       <c r="WU30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D31" s="11"/>
+      <c r="A31" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="12"/>
       <c r="E31" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F31" s="1"/>
       <c r="I31" s="1"/>
@@ -12241,20 +12297,20 @@
       <c r="WU31" s="1"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>11</v>
+      <c r="A32" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>12</v>
       </c>
       <c r="F32" s="1"/>
       <c r="I32" s="1"/>
@@ -12870,19 +12926,19 @@
       <c r="WU32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="11"/>
+      <c r="A33" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33" s="12"/>
       <c r="F33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -13497,19 +13553,19 @@
       <c r="WU33" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>9</v>
+      <c r="A34" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>10</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E34" s="11"/>
+        <v>37</v>
+      </c>
+      <c r="E34" s="12"/>
       <c r="F34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -14073,9 +14129,6 @@
       <c r="UV34" s="1"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0"/>
-      <c r="B35" s="0"/>
-      <c r="C35" s="0"/>
       <c r="D35" s="19"/>
       <c r="E35" s="20"/>
       <c r="F35" s="21"/>
@@ -14641,722 +14694,695 @@
       <c r="UV35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0"/>
-      <c r="B36" s="0"/>
-      <c r="C36" s="0"/>
       <c r="D36" s="19"/>
       <c r="E36" s="22"/>
       <c r="F36" s="23"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0"/>
-      <c r="B37" s="0"/>
-      <c r="C37" s="0"/>
       <c r="D37" s="19"/>
       <c r="F37" s="1"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0"/>
-      <c r="B38" s="0"/>
-      <c r="C38" s="0"/>
       <c r="D38" s="19"/>
       <c r="F38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0"/>
-      <c r="B39" s="0"/>
-      <c r="C39" s="0"/>
       <c r="D39" s="19"/>
-      <c r="E39" s="11"/>
+      <c r="E39" s="12"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0"/>
-      <c r="B40" s="0"/>
-      <c r="C40" s="0"/>
       <c r="D40" s="19"/>
-      <c r="E40" s="11"/>
+      <c r="E40" s="12"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0"/>
-      <c r="B41" s="0"/>
-      <c r="C41" s="0"/>
       <c r="D41" s="19"/>
-      <c r="E41" s="11"/>
+      <c r="E41" s="12"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0"/>
-      <c r="B42" s="0"/>
-      <c r="C42" s="0"/>
       <c r="D42" s="19"/>
-      <c r="E42" s="11"/>
+      <c r="E42" s="12"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0"/>
-      <c r="B43" s="0"/>
-      <c r="C43" s="0"/>
       <c r="D43" s="19"/>
-      <c r="E43" s="11"/>
+      <c r="E43" s="12"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0"/>
-      <c r="B44" s="0"/>
-      <c r="C44" s="0"/>
       <c r="D44" s="19"/>
-      <c r="E44" s="11"/>
+      <c r="E44" s="12"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C45" s="12"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C46" s="12"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C47" s="12"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C48" s="12"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C49" s="12"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C50" s="12"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C51" s="12"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C52" s="12"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C53" s="12"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="11"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C54" s="12"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="11"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C55" s="12"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="11"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C56" s="12"/>
-      <c r="D56" s="11"/>
-      <c r="E56" s="11"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C57" s="12"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="11"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C58" s="12"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="11"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C59" s="12"/>
-      <c r="D59" s="11"/>
-      <c r="E59" s="11"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C60" s="12"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="11"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C61" s="12"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C62" s="12"/>
-      <c r="D62" s="11"/>
-      <c r="E62" s="11"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C63" s="12"/>
-      <c r="D63" s="11"/>
-      <c r="E63" s="11"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C64" s="12"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="11"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C65" s="12"/>
-      <c r="D65" s="11"/>
-      <c r="E65" s="11"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C66" s="12"/>
-      <c r="D66" s="11"/>
-      <c r="E66" s="11"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="12"/>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C67" s="12"/>
-      <c r="D67" s="11"/>
-      <c r="E67" s="11"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C68" s="12"/>
-      <c r="D68" s="11"/>
-      <c r="E68" s="11"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12"/>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C69" s="12"/>
-      <c r="D69" s="11"/>
-      <c r="E69" s="11"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C70" s="12"/>
-      <c r="D70" s="11"/>
-      <c r="E70" s="11"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="12"/>
+      <c r="E70" s="12"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C71" s="12"/>
-      <c r="D71" s="11"/>
-      <c r="E71" s="11"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C72" s="12"/>
-      <c r="D72" s="11"/>
-      <c r="E72" s="11"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="12"/>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C73" s="12"/>
-      <c r="D73" s="11"/>
-      <c r="E73" s="11"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="12"/>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C74" s="12"/>
-      <c r="D74" s="11"/>
-      <c r="E74" s="11"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="12"/>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C75" s="12"/>
-      <c r="D75" s="11"/>
-      <c r="E75" s="11"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="12"/>
+      <c r="E75" s="12"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C76" s="12"/>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C77" s="12"/>
-      <c r="D77" s="11"/>
-      <c r="E77" s="11"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="12"/>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C78" s="12"/>
-      <c r="D78" s="11"/>
-      <c r="E78" s="11"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="12"/>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C79" s="12"/>
-      <c r="D79" s="11"/>
-      <c r="E79" s="11"/>
+      <c r="C79" s="13"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C80" s="12"/>
-      <c r="D80" s="11"/>
-      <c r="E80" s="11"/>
+      <c r="C80" s="13"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C81" s="12"/>
-      <c r="D81" s="11"/>
-      <c r="E81" s="11"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="12"/>
+      <c r="E81" s="12"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C82" s="12"/>
-      <c r="D82" s="11"/>
-      <c r="E82" s="11"/>
+      <c r="C82" s="13"/>
+      <c r="D82" s="12"/>
+      <c r="E82" s="12"/>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C83" s="12"/>
-      <c r="D83" s="11"/>
-      <c r="E83" s="11"/>
+      <c r="C83" s="13"/>
+      <c r="D83" s="12"/>
+      <c r="E83" s="12"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C84" s="12"/>
-      <c r="D84" s="11"/>
-      <c r="E84" s="11"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="12"/>
+      <c r="E84" s="12"/>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C85" s="12"/>
-      <c r="D85" s="11"/>
-      <c r="E85" s="11"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="12"/>
+      <c r="E85" s="12"/>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C86" s="12"/>
-      <c r="D86" s="11"/>
-      <c r="E86" s="11"/>
+      <c r="C86" s="13"/>
+      <c r="D86" s="12"/>
+      <c r="E86" s="12"/>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C87" s="12"/>
-      <c r="D87" s="11"/>
-      <c r="E87" s="11"/>
+      <c r="C87" s="13"/>
+      <c r="D87" s="12"/>
+      <c r="E87" s="12"/>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C88" s="12"/>
-      <c r="D88" s="11"/>
-      <c r="E88" s="11"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="12"/>
+      <c r="E88" s="12"/>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C89" s="12"/>
-      <c r="D89" s="11"/>
-      <c r="E89" s="11"/>
+      <c r="C89" s="13"/>
+      <c r="D89" s="12"/>
+      <c r="E89" s="12"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C90" s="12"/>
-      <c r="D90" s="11"/>
-      <c r="E90" s="11"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="12"/>
+      <c r="E90" s="12"/>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C91" s="12"/>
-      <c r="D91" s="11"/>
-      <c r="E91" s="11"/>
+      <c r="C91" s="13"/>
+      <c r="D91" s="12"/>
+      <c r="E91" s="12"/>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C92" s="12"/>
-      <c r="D92" s="11"/>
-      <c r="E92" s="11"/>
+      <c r="C92" s="13"/>
+      <c r="D92" s="12"/>
+      <c r="E92" s="12"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C93" s="12"/>
-      <c r="D93" s="11"/>
-      <c r="E93" s="11"/>
+      <c r="C93" s="13"/>
+      <c r="D93" s="12"/>
+      <c r="E93" s="12"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C94" s="12"/>
-      <c r="D94" s="11"/>
-      <c r="E94" s="11"/>
+      <c r="C94" s="13"/>
+      <c r="D94" s="12"/>
+      <c r="E94" s="12"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C95" s="12"/>
-      <c r="D95" s="11"/>
-      <c r="E95" s="11"/>
+      <c r="C95" s="13"/>
+      <c r="D95" s="12"/>
+      <c r="E95" s="12"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C96" s="12"/>
-      <c r="D96" s="11"/>
-      <c r="E96" s="11"/>
+      <c r="C96" s="13"/>
+      <c r="D96" s="12"/>
+      <c r="E96" s="12"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C97" s="12"/>
-      <c r="D97" s="11"/>
-      <c r="E97" s="11"/>
+      <c r="C97" s="13"/>
+      <c r="D97" s="12"/>
+      <c r="E97" s="12"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C98" s="12"/>
-      <c r="D98" s="11"/>
-      <c r="E98" s="11"/>
+      <c r="C98" s="13"/>
+      <c r="D98" s="12"/>
+      <c r="E98" s="12"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C99" s="12"/>
-      <c r="D99" s="11"/>
-      <c r="E99" s="11"/>
+      <c r="C99" s="13"/>
+      <c r="D99" s="12"/>
+      <c r="E99" s="12"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C100" s="12"/>
-      <c r="D100" s="11"/>
-      <c r="E100" s="11"/>
+      <c r="C100" s="13"/>
+      <c r="D100" s="12"/>
+      <c r="E100" s="12"/>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C101" s="12"/>
-      <c r="D101" s="11"/>
-      <c r="E101" s="11"/>
+      <c r="C101" s="13"/>
+      <c r="D101" s="12"/>
+      <c r="E101" s="12"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C102" s="12"/>
-      <c r="D102" s="11"/>
-      <c r="E102" s="11"/>
+      <c r="C102" s="13"/>
+      <c r="D102" s="12"/>
+      <c r="E102" s="12"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C103" s="12"/>
-      <c r="D103" s="11"/>
-      <c r="E103" s="11"/>
+      <c r="C103" s="13"/>
+      <c r="D103" s="12"/>
+      <c r="E103" s="12"/>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C104" s="12"/>
-      <c r="D104" s="11"/>
-      <c r="E104" s="11"/>
+      <c r="C104" s="13"/>
+      <c r="D104" s="12"/>
+      <c r="E104" s="12"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C105" s="12"/>
-      <c r="D105" s="11"/>
-      <c r="E105" s="11"/>
+      <c r="C105" s="13"/>
+      <c r="D105" s="12"/>
+      <c r="E105" s="12"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C106" s="12"/>
-      <c r="D106" s="11"/>
-      <c r="E106" s="11"/>
+      <c r="C106" s="13"/>
+      <c r="D106" s="12"/>
+      <c r="E106" s="12"/>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C107" s="12"/>
-      <c r="D107" s="11"/>
-      <c r="E107" s="11"/>
+      <c r="C107" s="13"/>
+      <c r="D107" s="12"/>
+      <c r="E107" s="12"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C108" s="12"/>
-      <c r="D108" s="11"/>
-      <c r="E108" s="11"/>
+      <c r="C108" s="13"/>
+      <c r="D108" s="12"/>
+      <c r="E108" s="12"/>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C109" s="12"/>
-      <c r="D109" s="11"/>
-      <c r="E109" s="11"/>
+      <c r="C109" s="13"/>
+      <c r="D109" s="12"/>
+      <c r="E109" s="12"/>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C110" s="12"/>
-      <c r="D110" s="11"/>
-      <c r="E110" s="11"/>
+      <c r="C110" s="13"/>
+      <c r="D110" s="12"/>
+      <c r="E110" s="12"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C111" s="12"/>
-      <c r="D111" s="11"/>
-      <c r="E111" s="11"/>
+      <c r="C111" s="13"/>
+      <c r="D111" s="12"/>
+      <c r="E111" s="12"/>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C112" s="12"/>
-      <c r="D112" s="11"/>
-      <c r="E112" s="11"/>
+      <c r="C112" s="13"/>
+      <c r="D112" s="12"/>
+      <c r="E112" s="12"/>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C113" s="12"/>
-      <c r="D113" s="11"/>
-      <c r="E113" s="11"/>
+      <c r="C113" s="13"/>
+      <c r="D113" s="12"/>
+      <c r="E113" s="12"/>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C114" s="12"/>
-      <c r="D114" s="11"/>
-      <c r="E114" s="11"/>
+      <c r="C114" s="13"/>
+      <c r="D114" s="12"/>
+      <c r="E114" s="12"/>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C115" s="12"/>
-      <c r="D115" s="11"/>
-      <c r="E115" s="11"/>
+      <c r="C115" s="13"/>
+      <c r="D115" s="12"/>
+      <c r="E115" s="12"/>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C116" s="12"/>
-      <c r="D116" s="11"/>
-      <c r="E116" s="11"/>
+      <c r="C116" s="13"/>
+      <c r="D116" s="12"/>
+      <c r="E116" s="12"/>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C117" s="12"/>
-      <c r="D117" s="11"/>
-      <c r="E117" s="11"/>
+      <c r="C117" s="13"/>
+      <c r="D117" s="12"/>
+      <c r="E117" s="12"/>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C118" s="12"/>
-      <c r="D118" s="11"/>
-      <c r="E118" s="11"/>
+      <c r="C118" s="13"/>
+      <c r="D118" s="12"/>
+      <c r="E118" s="12"/>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C119" s="12"/>
-      <c r="D119" s="11"/>
-      <c r="E119" s="11"/>
+      <c r="C119" s="13"/>
+      <c r="D119" s="12"/>
+      <c r="E119" s="12"/>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C120" s="12"/>
-      <c r="D120" s="11"/>
-      <c r="E120" s="11"/>
+      <c r="C120" s="13"/>
+      <c r="D120" s="12"/>
+      <c r="E120" s="12"/>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C121" s="12"/>
-      <c r="D121" s="11"/>
-      <c r="E121" s="11"/>
+      <c r="C121" s="13"/>
+      <c r="D121" s="12"/>
+      <c r="E121" s="12"/>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C122" s="12"/>
-      <c r="D122" s="11"/>
-      <c r="E122" s="11"/>
+      <c r="C122" s="13"/>
+      <c r="D122" s="12"/>
+      <c r="E122" s="12"/>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C123" s="12"/>
-      <c r="D123" s="11"/>
-      <c r="E123" s="11"/>
+      <c r="C123" s="13"/>
+      <c r="D123" s="12"/>
+      <c r="E123" s="12"/>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C124" s="12"/>
-      <c r="D124" s="11"/>
-      <c r="E124" s="11"/>
+      <c r="C124" s="13"/>
+      <c r="D124" s="12"/>
+      <c r="E124" s="12"/>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C125" s="12"/>
-      <c r="D125" s="11"/>
-      <c r="E125" s="11"/>
+      <c r="C125" s="13"/>
+      <c r="D125" s="12"/>
+      <c r="E125" s="12"/>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C126" s="12"/>
-      <c r="D126" s="11"/>
-      <c r="E126" s="11"/>
+      <c r="C126" s="13"/>
+      <c r="D126" s="12"/>
+      <c r="E126" s="12"/>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C127" s="12"/>
-      <c r="D127" s="11"/>
-      <c r="E127" s="11"/>
+      <c r="C127" s="13"/>
+      <c r="D127" s="12"/>
+      <c r="E127" s="12"/>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C128" s="12"/>
-      <c r="D128" s="11"/>
-      <c r="E128" s="11"/>
+      <c r="C128" s="13"/>
+      <c r="D128" s="12"/>
+      <c r="E128" s="12"/>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C129" s="12"/>
-      <c r="D129" s="11"/>
-      <c r="E129" s="11"/>
+      <c r="C129" s="13"/>
+      <c r="D129" s="12"/>
+      <c r="E129" s="12"/>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C130" s="12"/>
-      <c r="D130" s="11"/>
-      <c r="E130" s="11"/>
+      <c r="C130" s="13"/>
+      <c r="D130" s="12"/>
+      <c r="E130" s="12"/>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C131" s="12"/>
-      <c r="D131" s="11"/>
-      <c r="E131" s="11"/>
+      <c r="C131" s="13"/>
+      <c r="D131" s="12"/>
+      <c r="E131" s="12"/>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C132" s="12"/>
-      <c r="D132" s="11"/>
-      <c r="E132" s="11"/>
+      <c r="C132" s="13"/>
+      <c r="D132" s="12"/>
+      <c r="E132" s="12"/>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C133" s="12"/>
-      <c r="D133" s="11"/>
-      <c r="E133" s="11"/>
+      <c r="C133" s="13"/>
+      <c r="D133" s="12"/>
+      <c r="E133" s="12"/>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C134" s="12"/>
-      <c r="D134" s="11"/>
-      <c r="E134" s="11"/>
+      <c r="C134" s="13"/>
+      <c r="D134" s="12"/>
+      <c r="E134" s="12"/>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C135" s="12"/>
-      <c r="D135" s="11"/>
-      <c r="E135" s="11"/>
+      <c r="C135" s="13"/>
+      <c r="D135" s="12"/>
+      <c r="E135" s="12"/>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C136" s="12"/>
-      <c r="D136" s="11"/>
-      <c r="E136" s="11"/>
+      <c r="C136" s="13"/>
+      <c r="D136" s="12"/>
+      <c r="E136" s="12"/>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C137" s="12"/>
-      <c r="D137" s="11"/>
-      <c r="E137" s="11"/>
+      <c r="C137" s="13"/>
+      <c r="D137" s="12"/>
+      <c r="E137" s="12"/>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C138" s="12"/>
-      <c r="D138" s="11"/>
-      <c r="E138" s="11"/>
+      <c r="C138" s="13"/>
+      <c r="D138" s="12"/>
+      <c r="E138" s="12"/>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C139" s="12"/>
-      <c r="D139" s="11"/>
-      <c r="E139" s="11"/>
+      <c r="C139" s="13"/>
+      <c r="D139" s="12"/>
+      <c r="E139" s="12"/>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C140" s="12"/>
-      <c r="D140" s="11"/>
-      <c r="E140" s="11"/>
+      <c r="C140" s="13"/>
+      <c r="D140" s="12"/>
+      <c r="E140" s="12"/>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C141" s="12"/>
-      <c r="D141" s="11"/>
-      <c r="E141" s="11"/>
+      <c r="C141" s="13"/>
+      <c r="D141" s="12"/>
+      <c r="E141" s="12"/>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C142" s="12"/>
-      <c r="D142" s="11"/>
-      <c r="E142" s="11"/>
+      <c r="C142" s="13"/>
+      <c r="D142" s="12"/>
+      <c r="E142" s="12"/>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C143" s="12"/>
-      <c r="D143" s="11"/>
-      <c r="E143" s="11"/>
+      <c r="C143" s="13"/>
+      <c r="D143" s="12"/>
+      <c r="E143" s="12"/>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C144" s="12"/>
-      <c r="D144" s="11"/>
-      <c r="E144" s="11"/>
+      <c r="C144" s="13"/>
+      <c r="D144" s="12"/>
+      <c r="E144" s="12"/>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C145" s="12"/>
-      <c r="D145" s="11"/>
-      <c r="E145" s="11"/>
+      <c r="C145" s="13"/>
+      <c r="D145" s="12"/>
+      <c r="E145" s="12"/>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C146" s="12"/>
-      <c r="D146" s="11"/>
-      <c r="E146" s="11"/>
+      <c r="C146" s="13"/>
+      <c r="D146" s="12"/>
+      <c r="E146" s="12"/>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C147" s="12"/>
-      <c r="D147" s="11"/>
-      <c r="E147" s="11"/>
+      <c r="C147" s="13"/>
+      <c r="D147" s="12"/>
+      <c r="E147" s="12"/>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C148" s="12"/>
-      <c r="D148" s="11"/>
-      <c r="E148" s="11"/>
+      <c r="C148" s="13"/>
+      <c r="D148" s="12"/>
+      <c r="E148" s="12"/>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C149" s="12"/>
-      <c r="D149" s="11"/>
-      <c r="E149" s="11"/>
+      <c r="C149" s="13"/>
+      <c r="D149" s="12"/>
+      <c r="E149" s="12"/>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C150" s="12"/>
-      <c r="D150" s="11"/>
-      <c r="E150" s="11"/>
+      <c r="C150" s="13"/>
+      <c r="D150" s="12"/>
+      <c r="E150" s="12"/>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C151" s="12"/>
-      <c r="D151" s="11"/>
-      <c r="E151" s="11"/>
+      <c r="C151" s="13"/>
+      <c r="D151" s="12"/>
+      <c r="E151" s="12"/>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C152" s="12"/>
-      <c r="D152" s="11"/>
-      <c r="E152" s="11"/>
+      <c r="C152" s="13"/>
+      <c r="D152" s="12"/>
+      <c r="E152" s="12"/>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C153" s="12"/>
-      <c r="D153" s="11"/>
-      <c r="E153" s="11"/>
+      <c r="C153" s="13"/>
+      <c r="D153" s="12"/>
+      <c r="E153" s="12"/>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C154" s="12"/>
-      <c r="D154" s="11"/>
-      <c r="E154" s="11"/>
+      <c r="C154" s="13"/>
+      <c r="D154" s="12"/>
+      <c r="E154" s="12"/>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C155" s="12"/>
-      <c r="D155" s="11"/>
-      <c r="E155" s="11"/>
+      <c r="C155" s="13"/>
+      <c r="D155" s="12"/>
+      <c r="E155" s="12"/>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C156" s="12"/>
-      <c r="D156" s="11"/>
-      <c r="E156" s="11"/>
+      <c r="C156" s="13"/>
+      <c r="D156" s="12"/>
+      <c r="E156" s="12"/>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C157" s="12"/>
-      <c r="D157" s="11"/>
-      <c r="E157" s="11"/>
+      <c r="C157" s="13"/>
+      <c r="D157" s="12"/>
+      <c r="E157" s="12"/>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C158" s="12"/>
-      <c r="D158" s="11"/>
-      <c r="E158" s="11"/>
+      <c r="C158" s="13"/>
+      <c r="D158" s="12"/>
+      <c r="E158" s="12"/>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C159" s="12"/>
-      <c r="D159" s="11"/>
-      <c r="E159" s="11"/>
+      <c r="C159" s="13"/>
+      <c r="D159" s="12"/>
+      <c r="E159" s="12"/>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C160" s="12"/>
-      <c r="D160" s="11"/>
-      <c r="E160" s="11"/>
+      <c r="C160" s="13"/>
+      <c r="D160" s="12"/>
+      <c r="E160" s="12"/>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C161" s="12"/>
-      <c r="D161" s="11"/>
-      <c r="E161" s="11"/>
+      <c r="C161" s="13"/>
+      <c r="D161" s="12"/>
+      <c r="E161" s="12"/>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C162" s="12"/>
-      <c r="D162" s="11"/>
-      <c r="E162" s="11"/>
+      <c r="C162" s="13"/>
+      <c r="D162" s="12"/>
+      <c r="E162" s="12"/>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C163" s="12"/>
-      <c r="D163" s="11"/>
-      <c r="E163" s="11"/>
+      <c r="C163" s="13"/>
+      <c r="D163" s="12"/>
+      <c r="E163" s="12"/>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C164" s="12"/>
-      <c r="D164" s="11"/>
-      <c r="E164" s="11"/>
+      <c r="C164" s="13"/>
+      <c r="D164" s="12"/>
+      <c r="E164" s="12"/>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C165" s="12"/>
-      <c r="D165" s="11"/>
-      <c r="E165" s="11"/>
+      <c r="C165" s="13"/>
+      <c r="D165" s="12"/>
+      <c r="E165" s="12"/>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C166" s="12"/>
-      <c r="D166" s="11"/>
-      <c r="E166" s="11"/>
+      <c r="C166" s="13"/>
+      <c r="D166" s="12"/>
+      <c r="E166" s="12"/>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C167" s="12"/>
-      <c r="D167" s="11"/>
-      <c r="E167" s="11"/>
+      <c r="C167" s="13"/>
+      <c r="D167" s="12"/>
+      <c r="E167" s="12"/>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C168" s="12"/>
-      <c r="D168" s="11"/>
-      <c r="E168" s="11"/>
+      <c r="C168" s="13"/>
+      <c r="D168" s="12"/>
+      <c r="E168" s="12"/>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C169" s="12"/>
-      <c r="D169" s="11"/>
-      <c r="E169" s="11"/>
+      <c r="C169" s="13"/>
+      <c r="D169" s="12"/>
+      <c r="E169" s="12"/>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C170" s="12"/>
-      <c r="D170" s="11"/>
-      <c r="E170" s="11"/>
+      <c r="C170" s="13"/>
+      <c r="D170" s="12"/>
+      <c r="E170" s="12"/>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C171" s="12"/>
-      <c r="D171" s="11"/>
-      <c r="E171" s="11"/>
+      <c r="C171" s="13"/>
+      <c r="D171" s="12"/>
+      <c r="E171" s="12"/>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C172" s="12"/>
-      <c r="D172" s="11"/>
-      <c r="E172" s="11"/>
+      <c r="C172" s="13"/>
+      <c r="D172" s="12"/>
+      <c r="E172" s="12"/>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C173" s="12"/>
-      <c r="D173" s="11"/>
-      <c r="E173" s="11"/>
+      <c r="C173" s="13"/>
+      <c r="D173" s="12"/>
+      <c r="E173" s="12"/>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E174" s="11"/>
+      <c r="E174" s="12"/>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E175" s="11"/>
+      <c r="E175" s="12"/>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E176" s="11"/>
+      <c r="E176" s="12"/>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>